<commit_message>
Updated Risk-Adjusted Development Costs
</commit_message>
<xml_diff>
--- a/PALI_rNPV_Model.xlsx
+++ b/PALI_rNPV_Model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dan\OneDrive\Documents\Equity Research\PALI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BD1BD81-1401-49FD-B8D0-CE836D0D4566}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFAB64F3-8DCA-42E6-9F2E-2B9B8C8A8FA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -380,9 +380,6 @@
     <t>UC Phase 2 ($M, committed)</t>
   </si>
   <si>
-    <t>Oral small molecule, CRO-run</t>
-  </si>
-  <si>
     <t>UC Phase 3 ($M, × P(reach Ph3))</t>
   </si>
   <si>
@@ -404,9 +401,6 @@
     <t>G&amp;A to commercialization ($M)</t>
   </si>
   <si>
-    <t>~$5M/yr × 5 yrs</t>
-  </si>
-  <si>
     <t>PV of total dev costs ($M)</t>
   </si>
   <si>
@@ -612,6 +606,12 @@
   </si>
   <si>
     <t>Typical early-stage biotech WACC - PoC &amp; safety proven in UC phase 1a</t>
+  </si>
+  <si>
+    <t>Oral small molecule, CRO-run, large registrational study planned N=195</t>
+  </si>
+  <si>
+    <t>~$6M/yr 2026-2027 (Phase 2) + ~10M/yr 2028-2030 (Phase 3 &amp; NDA)</t>
   </si>
 </sst>
 </file>
@@ -1608,8 +1608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A103" sqref="A103"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B71" sqref="B71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1648,7 +1648,7 @@
         <v>0.13</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -2243,68 +2243,68 @@
         <v>116</v>
       </c>
       <c r="B67" s="22">
-        <v>-15</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>117</v>
+        <v>-25</v>
+      </c>
+      <c r="C67" s="87" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A68" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B68" s="36">
         <f>-55*B21*B22</f>
         <v>-24.75</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A69" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B69" s="22">
         <v>-12</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A70" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B70" s="36">
         <f>-40*B39*B40</f>
         <v>-12.8</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A71" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B71" s="22">
-        <v>-25</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>125</v>
+        <v>-42</v>
+      </c>
+      <c r="C71" s="87" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A72" s="5" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B72" s="36">
         <f>(B67+B68+B69+B70+B71)/(1+B5)^2.5</f>
-        <v>-65.973493432337023</v>
+        <v>-85.86499898982558</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -2314,7 +2314,7 @@
     </row>
     <row r="74" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A74" s="11" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B74" s="37">
         <f>B54+B64</f>
@@ -2324,24 +2324,24 @@
     </row>
     <row r="75" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A75" s="11" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B75" s="37">
         <f>B72</f>
-        <v>-65.973493432337023</v>
+        <v>-85.86499898982558</v>
       </c>
       <c r="C75" s="30"/>
     </row>
     <row r="76" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A76" s="11" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B76" s="37">
         <f>B74+B75</f>
-        <v>262.29591780901507</v>
+        <v>242.40441225152651</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -2351,32 +2351,32 @@
     </row>
     <row r="78" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A78" s="28" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B78" s="38"/>
       <c r="C78" s="30"/>
     </row>
     <row r="79" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A79" s="83" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B79" s="36">
         <f>MAX(0,B76)*0.25</f>
-        <v>65.573979452253766</v>
+        <v>60.601103062881627</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A80" s="5" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B80" s="22">
         <v>50</v>
       </c>
       <c r="C80" s="87" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -2386,25 +2386,25 @@
     </row>
     <row r="82" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A82" s="28" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B82" s="38"/>
       <c r="C82" s="30"/>
     </row>
     <row r="83" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A83" s="5" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B83" s="22">
         <v>205.5</v>
       </c>
       <c r="C83" s="87" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A84" s="5" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B84" s="22">
         <v>-5</v>
@@ -2413,14 +2413,14 @@
     </row>
     <row r="85" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A85" s="33" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B85" s="39">
         <f>B83+B84</f>
         <v>200.5</v>
       </c>
       <c r="C85" s="40" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -2430,14 +2430,14 @@
     </row>
     <row r="87" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A87" s="16" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B87" s="41">
         <f>B76+B79+B80+B85</f>
-        <v>578.36989726126876</v>
+        <v>553.50551531440806</v>
       </c>
       <c r="C87" s="42" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -2447,14 +2447,14 @@
     </row>
     <row r="89" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A89" s="7" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B89" s="43"/>
       <c r="C89" s="27"/>
     </row>
     <row r="90" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A90" s="5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B90" s="44">
         <f>'Diluted Shares'!B24</f>
@@ -2464,11 +2464,11 @@
     </row>
     <row r="91" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A91" s="45" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B91" s="46">
         <f>B87*1000000/B90</f>
-        <v>2.8233093463763055</v>
+        <v>2.7019340080766181</v>
       </c>
       <c r="C91" s="30"/>
     </row>
@@ -2479,7 +2479,7 @@
     </row>
     <row r="93" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A93" s="5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B93" s="47">
         <v>1.74</v>
@@ -2488,11 +2488,11 @@
     </row>
     <row r="94" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A94" s="5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B94" s="25">
         <f>(B91-B93)/B93</f>
-        <v>0.62259157837718704</v>
+        <v>0.55283563682564263</v>
       </c>
       <c r="C94" s="30"/>
     </row>
@@ -2503,13 +2503,13 @@
     </row>
     <row r="96" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A96" s="5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B96" s="10">
         <v>12</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -2519,54 +2519,54 @@
     </row>
     <row r="98" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A98" s="7" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B98" s="48"/>
       <c r="C98" s="48"/>
     </row>
     <row r="99" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A99" s="5" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B99" s="49">
         <f>B85*1000000/B90</f>
         <v>0.97873960354602485</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A100" s="5" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B100" s="49">
         <f>B76*1000000/B90</f>
-        <v>1.2803960229832225</v>
+        <v>1.1832957523434724</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A101" s="5" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B101" s="49">
         <f>(B79+B80)*1000000/B90</f>
-        <v>0.56417371984705877</v>
+        <v>0.53989865218712119</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A102" s="50" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B102" s="51">
         <f>B91</f>
-        <v>2.8233093463763055</v>
+        <v>2.7019340080766181</v>
       </c>
       <c r="C102" s="1"/>
     </row>
@@ -2585,7 +2585,7 @@
   <dimension ref="A1:K49"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2596,7 +2596,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="52" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B1" s="53"/>
       <c r="C1" s="53"/>
@@ -2622,7 +2622,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="54" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B3" s="55"/>
       <c r="C3" s="55"/>
@@ -2636,14 +2636,14 @@
     </row>
     <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="56" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B4" s="77">
         <f>'rNPV Model'!B5</f>
         <v>0.13</v>
       </c>
       <c r="C4" s="80" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D4" s="77">
         <f>'rNPV Model'!B14</f>
@@ -2658,14 +2658,14 @@
     </row>
     <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="57" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B5" s="77">
         <f>'rNPV Model'!B25</f>
         <v>0.28350000000000003</v>
       </c>
       <c r="C5" s="59" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D5" s="77">
         <f>'rNPV Model'!B43</f>
@@ -2680,14 +2680,14 @@
     </row>
     <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="57" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B6" s="84">
         <f>'rNPV Model'!B90</f>
         <v>204855305</v>
       </c>
       <c r="C6" s="59" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D6" s="85">
         <f>'rNPV Model'!B85</f>
@@ -2702,14 +2702,14 @@
     </row>
     <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="80" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B7" s="85">
         <f>'rNPV Model'!B80</f>
         <v>50</v>
       </c>
       <c r="C7" s="79" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D7" s="76">
         <f>0.25</f>
@@ -2724,14 +2724,14 @@
     </row>
     <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="78" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B8" s="61">
         <f>'rNPV Model'!B91</f>
-        <v>2.8233093463763055</v>
+        <v>2.7019340080766181</v>
       </c>
       <c r="C8" s="59" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D8" s="86">
         <f>'rNPV Model'!B93</f>
@@ -2758,7 +2758,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="54" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B10" s="55"/>
       <c r="C10" s="55"/>
@@ -2772,7 +2772,7 @@
     </row>
     <row r="11" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="62" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B11" s="63">
         <v>0.02</v>
@@ -2800,23 +2800,23 @@
       </c>
       <c r="B12" s="64">
         <f>(((((('rNPV Model'!B13*B$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A12)^(-'rNPV Model'!B47))/$A12))/(1+$A12)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A12)^(-'rNPV Model'!B57))/$A12))/(1+$A12)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A12)^2.5))+MAX(0,((((('rNPV Model'!B13*B$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A12)^(-'rNPV Model'!B47))/$A12))/(1+$A12)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A12)^(-'rNPV Model'!B57))/$A12))/(1+$A12)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A12)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>2.6905431312988708</v>
+        <v>2.5636263308330873</v>
       </c>
       <c r="C12" s="64">
         <f>(((((('rNPV Model'!B13*C$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A12)^(-'rNPV Model'!B47))/$A12))/(1+$A12)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A12)^(-'rNPV Model'!B57))/$A12))/(1+$A12)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A12)^2.5))+MAX(0,((((('rNPV Model'!B13*C$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A12)^(-'rNPV Model'!B47))/$A12))/(1+$A12)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A12)^(-'rNPV Model'!B57))/$A12))/(1+$A12)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A12)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>2.944470154638362</v>
+        <v>2.817553354172579</v>
       </c>
       <c r="D12" s="64">
         <f>(((((('rNPV Model'!B13*D$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A12)^(-'rNPV Model'!B47))/$A12))/(1+$A12)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A12)^(-'rNPV Model'!B57))/$A12))/(1+$A12)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A12)^2.5))+MAX(0,((((('rNPV Model'!B13*D$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A12)^(-'rNPV Model'!B47))/$A12))/(1+$A12)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A12)^(-'rNPV Model'!B57))/$A12))/(1+$A12)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A12)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>3.1983971779778524</v>
+        <v>3.0714803775120698</v>
       </c>
       <c r="E12" s="64">
         <f>(((((('rNPV Model'!B13*E$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A12)^(-'rNPV Model'!B47))/$A12))/(1+$A12)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A12)^(-'rNPV Model'!B57))/$A12))/(1+$A12)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A12)^2.5))+MAX(0,((((('rNPV Model'!B13*E$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A12)^(-'rNPV Model'!B47))/$A12))/(1+$A12)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A12)^(-'rNPV Model'!B57))/$A12))/(1+$A12)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A12)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>3.4523242013173436</v>
+        <v>3.3254074008515606</v>
       </c>
       <c r="F12" s="64">
         <f>(((((('rNPV Model'!B13*F$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A12)^(-'rNPV Model'!B47))/$A12))/(1+$A12)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A12)^(-'rNPV Model'!B57))/$A12))/(1+$A12)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A12)^2.5))+MAX(0,((((('rNPV Model'!B13*F$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A12)^(-'rNPV Model'!B47))/$A12))/(1+$A12)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A12)^(-'rNPV Model'!B57))/$A12))/(1+$A12)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A12)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>3.7062512246568349</v>
+        <v>3.5793344241910514</v>
       </c>
       <c r="G12" s="53"/>
       <c r="H12" s="53"/>
@@ -2829,23 +2829,23 @@
       </c>
       <c r="B13" s="65">
         <f>(((((('rNPV Model'!B13*B$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A13)^(-'rNPV Model'!B47))/$A13))/(1+$A13)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A13)^(-'rNPV Model'!B57))/$A13))/(1+$A13)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A13)^2.5))+MAX(0,((((('rNPV Model'!B13*B$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A13)^(-'rNPV Model'!B47))/$A13))/(1+$A13)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A13)^(-'rNPV Model'!B57))/$A13))/(1+$A13)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A13)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>2.5348283328563261</v>
+        <v>2.410725554205464</v>
       </c>
       <c r="C13" s="65">
         <f>(((((('rNPV Model'!B13*C$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A13)^(-'rNPV Model'!B47))/$A13))/(1+$A13)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A13)^(-'rNPV Model'!B57))/$A13))/(1+$A13)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A13)^2.5))+MAX(0,((((('rNPV Model'!B13*C$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A13)^(-'rNPV Model'!B47))/$A13))/(1+$A13)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A13)^(-'rNPV Model'!B57))/$A13))/(1+$A13)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A13)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>2.7677664866591885</v>
+        <v>2.6436637080083267</v>
       </c>
       <c r="D13" s="65">
         <f>(((((('rNPV Model'!B13*D$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A13)^(-'rNPV Model'!B47))/$A13))/(1+$A13)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A13)^(-'rNPV Model'!B57))/$A13))/(1+$A13)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A13)^2.5))+MAX(0,((((('rNPV Model'!B13*D$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A13)^(-'rNPV Model'!B47))/$A13))/(1+$A13)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A13)^(-'rNPV Model'!B57))/$A13))/(1+$A13)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A13)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>3.0007046404620512</v>
+        <v>2.8766018618111886</v>
       </c>
       <c r="E13" s="65">
         <f>(((((('rNPV Model'!B13*E$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A13)^(-'rNPV Model'!B47))/$A13))/(1+$A13)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A13)^(-'rNPV Model'!B57))/$A13))/(1+$A13)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A13)^2.5))+MAX(0,((((('rNPV Model'!B13*E$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A13)^(-'rNPV Model'!B47))/$A13))/(1+$A13)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A13)^(-'rNPV Model'!B57))/$A13))/(1+$A13)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A13)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>3.233642794264914</v>
+        <v>3.1095400156140518</v>
       </c>
       <c r="F13" s="64">
         <f>(((((('rNPV Model'!B13*F$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A13)^(-'rNPV Model'!B47))/$A13))/(1+$A13)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A13)^(-'rNPV Model'!B57))/$A13))/(1+$A13)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A13)^2.5))+MAX(0,((((('rNPV Model'!B13*F$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A13)^(-'rNPV Model'!B47))/$A13))/(1+$A13)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A13)^(-'rNPV Model'!B57))/$A13))/(1+$A13)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A13)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>3.4665809480677754</v>
+        <v>3.3424781694169132</v>
       </c>
       <c r="G13" s="53"/>
       <c r="H13" s="53"/>
@@ -2858,23 +2858,23 @@
       </c>
       <c r="B14" s="65">
         <f>(((((('rNPV Model'!B13*B$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A14)^(-'rNPV Model'!B47))/$A14))/(1+$A14)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A14)^(-'rNPV Model'!B57))/$A14))/(1+$A14)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A14)^2.5))+MAX(0,((((('rNPV Model'!B13*B$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A14)^(-'rNPV Model'!B47))/$A14))/(1+$A14)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A14)^(-'rNPV Model'!B57))/$A14))/(1+$A14)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A14)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>2.3953503045361786</v>
+        <v>2.2739749662364908</v>
       </c>
       <c r="C14" s="82">
         <f>(((((('rNPV Model'!B13*C$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A14)^(-'rNPV Model'!B47))/$A14))/(1+$A14)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A14)^(-'rNPV Model'!B57))/$A14))/(1+$A14)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A14)^2.5))+MAX(0,((((('rNPV Model'!B13*C$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A14)^(-'rNPV Model'!B47))/$A14))/(1+$A14)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A14)^(-'rNPV Model'!B57))/$A14))/(1+$A14)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A14)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>2.6093298254562418</v>
+        <v>2.4879544871565544</v>
       </c>
       <c r="D14" s="81">
         <f>(((((('rNPV Model'!B13*D$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A14)^(-'rNPV Model'!B47))/$A14))/(1+$A14)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A14)^(-'rNPV Model'!B57))/$A14))/(1+$A14)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A14)^2.5))+MAX(0,((((('rNPV Model'!B13*D$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A14)^(-'rNPV Model'!B47))/$A14))/(1+$A14)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A14)^(-'rNPV Model'!B57))/$A14))/(1+$A14)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A14)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>2.8233093463763055</v>
+        <v>2.7019340080766181</v>
       </c>
       <c r="E14" s="65">
         <f>(((((('rNPV Model'!B13*E$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A14)^(-'rNPV Model'!B47))/$A14))/(1+$A14)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A14)^(-'rNPV Model'!B57))/$A14))/(1+$A14)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A14)^2.5))+MAX(0,((((('rNPV Model'!B13*E$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A14)^(-'rNPV Model'!B47))/$A14))/(1+$A14)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A14)^(-'rNPV Model'!B57))/$A14))/(1+$A14)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A14)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>3.03728886729637</v>
+        <v>2.9159135289966822</v>
       </c>
       <c r="F14" s="66">
         <f>(((((('rNPV Model'!B13*F$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A14)^(-'rNPV Model'!B47))/$A14))/(1+$A14)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A14)^(-'rNPV Model'!B57))/$A14))/(1+$A14)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A14)^2.5))+MAX(0,((((('rNPV Model'!B13*F$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A14)^(-'rNPV Model'!B47))/$A14))/(1+$A14)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A14)^(-'rNPV Model'!B57))/$A14))/(1+$A14)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A14)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>3.2512683882164337</v>
+        <v>3.1298930499167454</v>
       </c>
       <c r="G14" s="53"/>
       <c r="H14" s="53"/>
@@ -2887,23 +2887,23 @@
       </c>
       <c r="B15" s="65">
         <f>(((((('rNPV Model'!B13*B$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A15)^(-'rNPV Model'!B47))/$A15))/(1+$A15)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A15)^(-'rNPV Model'!B57))/$A15))/(1+$A15)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A15)^2.5))+MAX(0,((((('rNPV Model'!B13*B$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A15)^(-'rNPV Model'!B47))/$A15))/(1+$A15)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A15)^(-'rNPV Model'!B57))/$A15))/(1+$A15)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A15)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>2.2702704359293522</v>
+        <v>2.1515393516877879</v>
       </c>
       <c r="C15" s="65">
         <f>(((((('rNPV Model'!B13*C$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A15)^(-'rNPV Model'!B47))/$A15))/(1+$A15)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A15)^(-'rNPV Model'!B57))/$A15))/(1+$A15)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A15)^2.5))+MAX(0,((((('rNPV Model'!B13*C$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A15)^(-'rNPV Model'!B47))/$A15))/(1+$A15)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A15)^(-'rNPV Model'!B57))/$A15))/(1+$A15)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A15)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>2.4670989919668704</v>
+        <v>2.3483679077253061</v>
       </c>
       <c r="D15" s="65">
         <f>(((((('rNPV Model'!B13*D$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A15)^(-'rNPV Model'!B47))/$A15))/(1+$A15)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A15)^(-'rNPV Model'!B57))/$A15))/(1+$A15)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A15)^2.5))+MAX(0,((((('rNPV Model'!B13*D$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A15)^(-'rNPV Model'!B47))/$A15))/(1+$A15)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A15)^(-'rNPV Model'!B57))/$A15))/(1+$A15)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A15)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>2.6639275480043887</v>
+        <v>2.5451964637628244</v>
       </c>
       <c r="E15" s="65">
         <f>(((((('rNPV Model'!B13*E$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A15)^(-'rNPV Model'!B47))/$A15))/(1+$A15)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A15)^(-'rNPV Model'!B57))/$A15))/(1+$A15)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A15)^2.5))+MAX(0,((((('rNPV Model'!B13*E$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A15)^(-'rNPV Model'!B47))/$A15))/(1+$A15)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A15)^(-'rNPV Model'!B57))/$A15))/(1+$A15)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A15)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>2.8607561040419074</v>
+        <v>2.7420250198003431</v>
       </c>
       <c r="F15" s="64">
         <f>(((((('rNPV Model'!B13*F$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A15)^(-'rNPV Model'!B47))/$A15))/(1+$A15)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A15)^(-'rNPV Model'!B57))/$A15))/(1+$A15)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A15)^2.5))+MAX(0,((((('rNPV Model'!B13*F$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A15)^(-'rNPV Model'!B47))/$A15))/(1+$A15)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A15)^(-'rNPV Model'!B57))/$A15))/(1+$A15)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A15)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>3.0575846600794256</v>
+        <v>2.9388535758378613</v>
       </c>
       <c r="G15" s="53"/>
       <c r="H15" s="53"/>
@@ -2936,7 +2936,7 @@
     </row>
     <row r="18" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="92" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B18" s="69"/>
       <c r="C18" s="70"/>
@@ -2951,28 +2951,28 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" s="72" t="s">
+        <v>167</v>
+      </c>
+      <c r="B19" s="72" t="s">
+        <v>168</v>
+      </c>
+      <c r="C19" s="72" t="s">
+        <v>159</v>
+      </c>
+      <c r="D19" s="89" t="s">
+        <v>160</v>
+      </c>
+      <c r="E19" s="89" t="s">
+        <v>189</v>
+      </c>
+      <c r="F19" s="72" t="s">
+        <v>157</v>
+      </c>
+      <c r="G19" s="72" t="s">
         <v>169</v>
       </c>
-      <c r="B19" s="72" t="s">
+      <c r="H19" s="72" t="s">
         <v>170</v>
-      </c>
-      <c r="C19" s="72" t="s">
-        <v>161</v>
-      </c>
-      <c r="D19" s="89" t="s">
-        <v>162</v>
-      </c>
-      <c r="E19" s="89" t="s">
-        <v>191</v>
-      </c>
-      <c r="F19" s="72" t="s">
-        <v>159</v>
-      </c>
-      <c r="G19" s="72" t="s">
-        <v>171</v>
-      </c>
-      <c r="H19" s="72" t="s">
-        <v>172</v>
       </c>
       <c r="I19" s="53"/>
       <c r="J19" s="53"/>
@@ -2980,7 +2980,7 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" s="56" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B20" s="76">
         <v>0.02</v>
@@ -2999,10 +2999,10 @@
       </c>
       <c r="G20" s="73">
         <f>((('rNPV Model'!B13*B20*'rNPV Model'!B16*'rNPV Model'!B18*((1-(1+F20)^(-'rNPV Model'!B47))/F20)/(1+F20)^('rNPV Model'!B8-'rNPV Model'!B10)*C20)+('rNPV Model'!B60*((1-(1+F20)^(-'rNPV Model'!B57))/F20)/(1+F20)^('rNPV Model'!B9-'rNPV Model'!B10)*D20)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+F20)^2.5))+MAX(0,(('rNPV Model'!B13*B20*'rNPV Model'!B16*'rNPV Model'!B18*((1-(1+F20)^(-'rNPV Model'!B47))/F20)/(1+F20)^('rNPV Model'!B8-'rNPV Model'!B10)*C20)+('rNPV Model'!B60*((1-(1+F20)^(-'rNPV Model'!B57))/F20)/(1+F20)^('rNPV Model'!B9-'rNPV Model'!B10)*D20)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+F20)^2.5)))*$D$7+E20+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>0.85075968964311455</v>
+        <v>0.75577482224986292</v>
       </c>
       <c r="H20" s="87" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="I20" s="53"/>
       <c r="J20" s="53"/>
@@ -3010,7 +3010,7 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21" s="56" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B21" s="76">
         <f>'rNPV Model'!B14</f>
@@ -3033,7 +3033,7 @@
       </c>
       <c r="G21" s="74">
         <f>((('rNPV Model'!B13*B21*'rNPV Model'!B16*'rNPV Model'!B18*((1-(1+F21)^(-'rNPV Model'!B47))/F21)/(1+F21)^('rNPV Model'!B8-'rNPV Model'!B10)*C21)+('rNPV Model'!B60*((1-(1+F21)^(-'rNPV Model'!B57))/F21)/(1+F21)^('rNPV Model'!B9-'rNPV Model'!B10)*D21)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+F21)^2.5))+MAX(0,(('rNPV Model'!B13*B21*'rNPV Model'!B16*'rNPV Model'!B18*((1-(1+F21)^(-'rNPV Model'!B47))/F21)/(1+F21)^('rNPV Model'!B8-'rNPV Model'!B10)*C21)+('rNPV Model'!B60*((1-(1+F21)^(-'rNPV Model'!B57))/F21)/(1+F21)^('rNPV Model'!B9-'rNPV Model'!B10)*D21)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+F21)^2.5)))*$D$7+E21+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>2.8233093463763055</v>
+        <v>2.7019340080766181</v>
       </c>
       <c r="H21" s="1"/>
       <c r="I21" s="53"/>
@@ -3042,7 +3042,7 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22" s="56" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B22" s="76">
         <v>7.0000000000000007E-2</v>
@@ -3061,10 +3061,10 @@
       </c>
       <c r="G22" s="73">
         <f>((('rNPV Model'!B13*B22*'rNPV Model'!B16*'rNPV Model'!B18*((1-(1+F22)^(-'rNPV Model'!B47))/F22)/(1+F22)^('rNPV Model'!B8-'rNPV Model'!B10)*C22)+('rNPV Model'!B60*((1-(1+F22)^(-'rNPV Model'!B57))/F22)/(1+F22)^('rNPV Model'!B9-'rNPV Model'!B10)*D22)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+F22)^2.5))+MAX(0,(('rNPV Model'!B13*B22*'rNPV Model'!B16*'rNPV Model'!B18*((1-(1+F22)^(-'rNPV Model'!B47))/F22)/(1+F22)^('rNPV Model'!B8-'rNPV Model'!B10)*C22)+('rNPV Model'!B60*((1-(1+F22)^(-'rNPV Model'!B57))/F22)/(1+F22)^('rNPV Model'!B9-'rNPV Model'!B10)*D22)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+F22)^2.5)))*$D$7+E22+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>3.6110761926413444</v>
+        <v>3.489700854341657</v>
       </c>
       <c r="H22" s="87" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="I22" s="53"/>
       <c r="J22" s="53"/>
@@ -3072,7 +3072,7 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23" s="56" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B23" s="76">
         <v>7.0000000000000007E-2</v>
@@ -3091,10 +3091,10 @@
       </c>
       <c r="G23" s="73">
         <f>((('rNPV Model'!B13*B23*'rNPV Model'!B16*'rNPV Model'!B18*((1-(1+F23)^(-'rNPV Model'!B47))/F23)/(1+F23)^('rNPV Model'!B8-'rNPV Model'!B10)*C23)+('rNPV Model'!B60*((1-(1+F23)^(-'rNPV Model'!B57))/F23)/(1+F23)^('rNPV Model'!B9-'rNPV Model'!B10)*D23)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+F23)^2.5))+MAX(0,(('rNPV Model'!B13*B23*'rNPV Model'!B16*'rNPV Model'!B18*((1-(1+F23)^(-'rNPV Model'!B47))/F23)/(1+F23)^('rNPV Model'!B8-'rNPV Model'!B10)*C23)+('rNPV Model'!B60*((1-(1+F23)^(-'rNPV Model'!B57))/F23)/(1+F23)^('rNPV Model'!B9-'rNPV Model'!B10)*D23)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+F23)^2.5)))*$D$7+E23+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>5.1566068922680932</v>
+        <v>5.0325041136172315</v>
       </c>
       <c r="H23" s="87" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="I23" s="53"/>
       <c r="J23" s="53"/>
@@ -3102,7 +3102,7 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24" s="56" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B24" s="76">
         <v>0.1</v>
@@ -3121,10 +3121,10 @@
       </c>
       <c r="G24" s="73">
         <f>((('rNPV Model'!B13*B24*'rNPV Model'!B16*'rNPV Model'!B18*((1-(1+F24)^(-'rNPV Model'!B47))/F24)/(1+F24)^('rNPV Model'!B8-'rNPV Model'!B10)*C24)+('rNPV Model'!B60*((1-(1+F24)^(-'rNPV Model'!B57))/F24)/(1+F24)^('rNPV Model'!B9-'rNPV Model'!B10)*D24)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+F24)^2.5))+MAX(0,(('rNPV Model'!B13*B24*'rNPV Model'!B16*'rNPV Model'!B18*((1-(1+F24)^(-'rNPV Model'!B47))/F24)/(1+F24)^('rNPV Model'!B8-'rNPV Model'!B10)*C24)+('rNPV Model'!B60*((1-(1+F24)^(-'rNPV Model'!B57))/F24)/(1+F24)^('rNPV Model'!B9-'rNPV Model'!B10)*D24)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+F24)^2.5)))*$D$7+E24+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>7.2220686752790542</v>
+        <v>7.0951518748132711</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="I24" s="53"/>
       <c r="J24" s="53"/>
@@ -3144,7 +3144,7 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26" s="75" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B26" s="53"/>
       <c r="C26" s="53"/>
@@ -3158,7 +3158,7 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B27" s="53"/>
       <c r="C27" s="53"/>
@@ -3172,7 +3172,7 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B28" s="53"/>
       <c r="C28" s="53"/>
@@ -3186,7 +3186,7 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B29" s="53"/>
       <c r="C29" s="53"/>
@@ -3200,7 +3200,7 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A30" s="87" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B30" s="53"/>
       <c r="C30" s="53"/>
@@ -3214,7 +3214,7 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B31" s="53"/>
       <c r="C31" s="53"/>

</xml_diff>

<commit_message>
update FSCD target patient population (US)
</commit_message>
<xml_diff>
--- a/PALI_rNPV_Model.xlsx
+++ b/PALI_rNPV_Model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dan\OneDrive\Documents\Equity Research\PALI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91A291D3-274D-4DCB-AA28-CA6C6C07366C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C240F90-209E-4D6D-B315-C82FD28E7A8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -239,9 +239,6 @@
     <t>FSCD Target Patient Population (US)</t>
   </si>
   <si>
-    <t>Est. ~150K FSCD patients; ZERO approved therapies</t>
-  </si>
-  <si>
     <t>Annual Revenue per Patient ($)</t>
   </si>
   <si>
@@ -251,9 +248,6 @@
     <t>US Peak Market Penetration (%)</t>
   </si>
   <si>
-    <t>10% — first &amp; only therapy; strong first-mover</t>
-  </si>
-  <si>
     <t>Peak US Revenue ($M)</t>
   </si>
   <si>
@@ -590,9 +584,6 @@
     <t>Platform ($M)</t>
   </si>
   <si>
-    <t>Zero fibrosis signals, FSCD discontinued, and UC is a commercial flop</t>
-  </si>
-  <si>
     <t>Typical early-stage biotech WACC - PoC &amp; safety proven in UC phase 1a</t>
   </si>
   <si>
@@ -612,6 +603,15 @@
   </si>
   <si>
     <t>Significant reduction in Fibrosis Genes (scRNA-seq) and/or resolution of Inflammatory Edema (precursor to stricture improvement)</t>
+  </si>
+  <si>
+    <t>Zero fibrosis signals, FSCD discontinued, and UC is a commercial flop (immediate cash value is still $0.98)</t>
+  </si>
+  <si>
+    <t>Est. ~150K Symptomatic/Active FSCD patients &amp; ~150k Post-op maintenance; ZERO approved therapies</t>
+  </si>
+  <si>
+    <t>first &amp; only therapy; strong first-mover; blending symptomatic/Active penetration (20%) with Post-op maintenance penetration (10%)</t>
   </si>
 </sst>
 </file>
@@ -1567,7 +1567,7 @@
         <v>6.5</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -1608,8 +1608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C102"/>
   <sheetViews>
-    <sheetView topLeftCell="A75" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A94" sqref="A94"/>
+    <sheetView topLeftCell="A72" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A103" sqref="A103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1648,7 +1648,7 @@
         <v>0.13</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -1732,7 +1732,7 @@
         <v>0.06</v>
       </c>
       <c r="C14" s="21" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -1856,78 +1856,78 @@
         <v>69</v>
       </c>
       <c r="B28" s="4">
-        <v>250000</v>
+        <v>300000</v>
       </c>
       <c r="C28" s="21" t="s">
-        <v>70</v>
+        <v>193</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B29" s="22">
         <v>40000</v>
       </c>
       <c r="C29" s="21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B30" s="20">
         <v>0.15</v>
       </c>
       <c r="C30" s="21" t="s">
-        <v>74</v>
+        <v>194</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B31" s="23">
         <f>B28*B29*B30/1000000</f>
-        <v>1500</v>
+        <v>1800</v>
       </c>
       <c r="C31" s="21" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B32" s="26">
         <v>0.5</v>
       </c>
       <c r="C32" s="21" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B33" s="23">
         <f>B31*(1+B32)</f>
-        <v>2250</v>
+        <v>2700</v>
       </c>
       <c r="C33" s="21" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B34" s="20">
         <v>0.35</v>
       </c>
       <c r="C34" s="21" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -1936,10 +1936,10 @@
       </c>
       <c r="B35" s="23">
         <f>B33*B34</f>
-        <v>787.5</v>
+        <v>944.99999999999989</v>
       </c>
       <c r="C35" s="21" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -1950,12 +1950,12 @@
         <v>0.65</v>
       </c>
       <c r="C36" s="21" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B38" s="8"/>
       <c r="C38" s="8"/>
@@ -1968,7 +1968,7 @@
         <v>0.8</v>
       </c>
       <c r="C39" s="21" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -1979,7 +1979,7 @@
         <v>0.4</v>
       </c>
       <c r="C40" s="21" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -1990,7 +1990,7 @@
         <v>0.65</v>
       </c>
       <c r="C41" s="21" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -2001,7 +2001,7 @@
         <v>0.85</v>
       </c>
       <c r="C42" s="21" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -2018,93 +2018,93 @@
     </row>
     <row r="45" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="7" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B45" s="27"/>
       <c r="C45" s="27"/>
     </row>
     <row r="46" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="28" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B46" s="29"/>
       <c r="C46" s="30"/>
     </row>
     <row r="47" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B47" s="31">
         <f>B7-B8</f>
         <v>10</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B48" s="23">
         <f>B15</f>
         <v>600</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B49" s="23">
         <f>B17</f>
         <v>210</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B50" s="23">
         <f>B17*B18</f>
         <v>126</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B51" s="23">
         <f>B50*((1-(1+B5)^(-B47))/B5)</f>
         <v>683.70667797006286</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B52" s="23">
         <f>B51/(1+B5)^(B8-B10)</f>
         <v>371.08859277742692</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B53" s="32">
         <f>B25</f>
@@ -2114,7 +2114,7 @@
     </row>
     <row r="54" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="33" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B54" s="34">
         <f>B52*B53</f>
@@ -2129,86 +2129,86 @@
     </row>
     <row r="56" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="28" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B56" s="35"/>
       <c r="C56" s="30"/>
     </row>
     <row r="57" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B57" s="31">
         <f>B7-B9</f>
         <v>9</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B58" s="23">
         <f>B33</f>
-        <v>2250</v>
+        <v>2700</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B59" s="23">
         <f>B35</f>
-        <v>787.5</v>
+        <v>944.99999999999989</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B60" s="23">
         <f>B35*B36</f>
-        <v>511.875</v>
+        <v>614.25</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B61" s="23">
         <f>B60*((1-(1+B5)^(-B57))/B5)</f>
-        <v>2626.7659685563203</v>
+        <v>3152.1191622675842</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" s="5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B62" s="23">
         <f>B61/(1+B5)^(B9-B10)</f>
-        <v>1261.6843619284587</v>
+        <v>1514.0212343141504</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A63" s="5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B63" s="32">
         <f>B43</f>
@@ -2218,11 +2218,11 @@
     </row>
     <row r="64" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A64" s="33" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B64" s="34">
         <f>B62*B63</f>
-        <v>223.06579518895154</v>
+        <v>267.67895422674184</v>
       </c>
       <c r="C64" s="30"/>
     </row>
@@ -2233,78 +2233,78 @@
     </row>
     <row r="66" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A66" s="28" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B66" s="35"/>
       <c r="C66" s="30"/>
     </row>
     <row r="67" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A67" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B67" s="22">
         <v>-25</v>
       </c>
       <c r="C67" s="87" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A68" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B68" s="36">
         <f>-55*B21*B22</f>
         <v>-24.75</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A69" s="5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B69" s="22">
         <v>-12</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A70" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B70" s="36">
         <f>-40*B39*B40</f>
         <v>-12.8</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A71" s="5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B71" s="22">
         <v>-42</v>
       </c>
       <c r="C71" s="87" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A72" s="5" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B72" s="36">
         <f>(B67+B68+B69+B70+B71)/(1+B5)^2.5</f>
         <v>-85.86499898982558</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -2314,17 +2314,17 @@
     </row>
     <row r="74" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A74" s="11" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B74" s="37">
         <f>B54+B64</f>
-        <v>328.26941124135209</v>
+        <v>372.88257027914239</v>
       </c>
       <c r="C74" s="30"/>
     </row>
     <row r="75" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A75" s="11" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B75" s="37">
         <f>B72</f>
@@ -2334,14 +2334,14 @@
     </row>
     <row r="76" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A76" s="11" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B76" s="37">
         <f>B74+B75</f>
-        <v>242.40441225152651</v>
+        <v>287.01757128931683</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -2351,32 +2351,32 @@
     </row>
     <row r="78" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A78" s="28" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B78" s="38"/>
       <c r="C78" s="30"/>
     </row>
     <row r="79" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A79" s="83" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B79" s="36">
         <f>MAX(0,B76)*0.25</f>
-        <v>60.601103062881627</v>
+        <v>71.754392822329208</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A80" s="5" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B80" s="22">
         <v>50</v>
       </c>
       <c r="C80" s="87" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -2386,25 +2386,25 @@
     </row>
     <row r="82" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A82" s="28" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B82" s="38"/>
       <c r="C82" s="30"/>
     </row>
     <row r="83" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A83" s="5" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B83" s="22">
         <v>205.5</v>
       </c>
       <c r="C83" s="87" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A84" s="5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B84" s="22">
         <v>-5</v>
@@ -2413,14 +2413,14 @@
     </row>
     <row r="85" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A85" s="33" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B85" s="39">
         <f>B83+B84</f>
         <v>200.5</v>
       </c>
       <c r="C85" s="40" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -2430,14 +2430,14 @@
     </row>
     <row r="87" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A87" s="16" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B87" s="41">
         <f>B76+B79+B80+B85</f>
-        <v>553.50551531440806</v>
+        <v>609.27196411164607</v>
       </c>
       <c r="C87" s="42" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -2447,14 +2447,14 @@
     </row>
     <row r="89" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A89" s="7" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B89" s="43"/>
       <c r="C89" s="27"/>
     </row>
     <row r="90" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A90" s="5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B90" s="44">
         <f>'Diluted Shares'!B24</f>
@@ -2464,11 +2464,11 @@
     </row>
     <row r="91" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A91" s="45" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B91" s="46">
         <f>B87*1000000/B90</f>
-        <v>2.6988937109128535</v>
+        <v>2.9708109976869812</v>
       </c>
       <c r="C91" s="30"/>
     </row>
@@ -2479,7 +2479,7 @@
     </row>
     <row r="93" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A93" s="5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B93" s="47">
         <v>1.74</v>
@@ -2488,11 +2488,11 @@
     </row>
     <row r="94" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A94" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B94" s="25">
         <f>(B91-B93)/B93</f>
-        <v>0.55108833960508818</v>
+        <v>0.70736264234883983</v>
       </c>
       <c r="C94" s="30"/>
     </row>
@@ -2503,13 +2503,13 @@
     </row>
     <row r="96" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A96" s="5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B96" s="10">
         <v>12</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -2519,54 +2519,54 @@
     </row>
     <row r="98" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A98" s="7" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B98" s="48"/>
       <c r="C98" s="48"/>
     </row>
     <row r="99" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A99" s="5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B99" s="49">
         <f>B85*1000000/B90</f>
         <v>0.97763829639646815</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A100" s="5" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B100" s="49">
         <f>B76*1000000/B90</f>
-        <v>1.1819642724816435</v>
+        <v>1.3994981019009454</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A101" s="5" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B101" s="49">
         <f>(B79+B80)*1000000/B90</f>
-        <v>0.53929114203474215</v>
+        <v>0.59367459938956757</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A102" s="50" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B102" s="51">
         <f>B91</f>
-        <v>2.6988937109128535</v>
+        <v>2.9708109976869812</v>
       </c>
       <c r="C102" s="1"/>
     </row>
@@ -2596,7 +2596,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="52" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B1" s="53"/>
       <c r="C1" s="53"/>
@@ -2622,7 +2622,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="54" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B3" s="55"/>
       <c r="C3" s="55"/>
@@ -2636,14 +2636,14 @@
     </row>
     <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="56" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B4" s="77">
         <f>'rNPV Model'!B5</f>
         <v>0.13</v>
       </c>
       <c r="C4" s="80" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D4" s="77">
         <f>'rNPV Model'!B14</f>
@@ -2658,14 +2658,14 @@
     </row>
     <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="57" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B5" s="77">
         <f>'rNPV Model'!B25</f>
         <v>0.28350000000000003</v>
       </c>
       <c r="C5" s="59" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D5" s="77">
         <f>'rNPV Model'!B43</f>
@@ -2680,14 +2680,14 @@
     </row>
     <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="57" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B6" s="84">
         <f>'rNPV Model'!B90</f>
         <v>205086074</v>
       </c>
       <c r="C6" s="59" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D6" s="85">
         <f>'rNPV Model'!B85</f>
@@ -2702,14 +2702,14 @@
     </row>
     <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="80" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B7" s="85">
         <f>'rNPV Model'!B80</f>
         <v>50</v>
       </c>
       <c r="C7" s="79" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D7" s="76">
         <f>0.25</f>
@@ -2724,14 +2724,14 @@
     </row>
     <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="78" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B8" s="61">
         <f>'rNPV Model'!B91</f>
-        <v>2.6988937109128535</v>
+        <v>2.9708109976869812</v>
       </c>
       <c r="C8" s="59" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D8" s="86">
         <f>'rNPV Model'!B93</f>
@@ -2758,7 +2758,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="54" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B10" s="55"/>
       <c r="C10" s="55"/>
@@ -2772,7 +2772,7 @@
     </row>
     <row r="11" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="62" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B11" s="63">
         <v>0.02</v>
@@ -2800,23 +2800,23 @@
       </c>
       <c r="B12" s="64">
         <f>(((((('rNPV Model'!B13*B$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A12)^(-'rNPV Model'!B47))/$A12))/(1+$A12)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A12)^(-'rNPV Model'!B57))/$A12))/(1+$A12)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A12)^2.5))+MAX(0,((((('rNPV Model'!B13*B$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A12)^(-'rNPV Model'!B47))/$A12))/(1+$A12)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A12)^(-'rNPV Model'!B57))/$A12))/(1+$A12)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A12)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>2.5607416616149323</v>
+        <v>2.8873222717278568</v>
       </c>
       <c r="C12" s="64">
         <f>(((((('rNPV Model'!B13*C$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A12)^(-'rNPV Model'!B47))/$A12))/(1+$A12)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A12)^(-'rNPV Model'!B57))/$A12))/(1+$A12)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A12)^2.5))+MAX(0,((((('rNPV Model'!B13*C$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A12)^(-'rNPV Model'!B47))/$A12))/(1+$A12)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A12)^(-'rNPV Model'!B57))/$A12))/(1+$A12)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A12)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>2.8143829586537246</v>
+        <v>3.1409635687666482</v>
       </c>
       <c r="D12" s="64">
         <f>(((((('rNPV Model'!B13*D$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A12)^(-'rNPV Model'!B47))/$A12))/(1+$A12)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A12)^(-'rNPV Model'!B57))/$A12))/(1+$A12)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A12)^2.5))+MAX(0,((((('rNPV Model'!B13*D$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A12)^(-'rNPV Model'!B47))/$A12))/(1+$A12)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A12)^(-'rNPV Model'!B57))/$A12))/(1+$A12)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A12)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>3.0680242556925159</v>
+        <v>3.3946048658054391</v>
       </c>
       <c r="E12" s="64">
         <f>(((((('rNPV Model'!B13*E$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A12)^(-'rNPV Model'!B47))/$A12))/(1+$A12)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A12)^(-'rNPV Model'!B57))/$A12))/(1+$A12)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A12)^2.5))+MAX(0,((((('rNPV Model'!B13*E$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A12)^(-'rNPV Model'!B47))/$A12))/(1+$A12)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A12)^(-'rNPV Model'!B57))/$A12))/(1+$A12)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A12)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>3.3216655527313068</v>
+        <v>3.6482461628442318</v>
       </c>
       <c r="F12" s="64">
         <f>(((((('rNPV Model'!B13*F$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A12)^(-'rNPV Model'!B47))/$A12))/(1+$A12)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A12)^(-'rNPV Model'!B57))/$A12))/(1+$A12)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A12)^2.5))+MAX(0,((((('rNPV Model'!B13*F$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A12)^(-'rNPV Model'!B47))/$A12))/(1+$A12)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A12)^(-'rNPV Model'!B57))/$A12))/(1+$A12)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A12)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>3.5753068497700982</v>
+        <v>3.9018874598830227</v>
       </c>
       <c r="G12" s="53"/>
       <c r="H12" s="53"/>
@@ -2829,23 +2829,23 @@
       </c>
       <c r="B13" s="65">
         <f>(((((('rNPV Model'!B13*B$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A13)^(-'rNPV Model'!B47))/$A13))/(1+$A13)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A13)^(-'rNPV Model'!B57))/$A13))/(1+$A13)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A13)^2.5))+MAX(0,((((('rNPV Model'!B13*B$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A13)^(-'rNPV Model'!B47))/$A13))/(1+$A13)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A13)^(-'rNPV Model'!B57))/$A13))/(1+$A13)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A13)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>2.4080129335259222</v>
+        <v>2.7058141433111724</v>
       </c>
       <c r="C13" s="65">
         <f>(((((('rNPV Model'!B13*C$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A13)^(-'rNPV Model'!B47))/$A13))/(1+$A13)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A13)^(-'rNPV Model'!B57))/$A13))/(1+$A13)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A13)^2.5))+MAX(0,((((('rNPV Model'!B13*C$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A13)^(-'rNPV Model'!B47))/$A13))/(1+$A13)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A13)^(-'rNPV Model'!B57))/$A13))/(1+$A13)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A13)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>2.6406889783334417</v>
+        <v>2.938490188118692</v>
       </c>
       <c r="D13" s="65">
         <f>(((((('rNPV Model'!B13*D$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A13)^(-'rNPV Model'!B47))/$A13))/(1+$A13)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A13)^(-'rNPV Model'!B57))/$A13))/(1+$A13)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A13)^2.5))+MAX(0,((((('rNPV Model'!B13*D$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A13)^(-'rNPV Model'!B47))/$A13))/(1+$A13)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A13)^(-'rNPV Model'!B57))/$A13))/(1+$A13)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A13)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>2.8733650231409613</v>
+        <v>3.1711662329262116</v>
       </c>
       <c r="E13" s="65">
         <f>(((((('rNPV Model'!B13*E$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A13)^(-'rNPV Model'!B47))/$A13))/(1+$A13)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A13)^(-'rNPV Model'!B57))/$A13))/(1+$A13)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A13)^2.5))+MAX(0,((((('rNPV Model'!B13*E$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A13)^(-'rNPV Model'!B47))/$A13))/(1+$A13)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A13)^(-'rNPV Model'!B57))/$A13))/(1+$A13)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A13)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>3.1060410679484818</v>
+        <v>3.4038422777337307</v>
       </c>
       <c r="F13" s="64">
         <f>(((((('rNPV Model'!B13*F$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A13)^(-'rNPV Model'!B47))/$A13))/(1+$A13)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A13)^(-'rNPV Model'!B57))/$A13))/(1+$A13)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A13)^2.5))+MAX(0,((((('rNPV Model'!B13*F$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A13)^(-'rNPV Model'!B47))/$A13))/(1+$A13)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A13)^(-'rNPV Model'!B57))/$A13))/(1+$A13)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A13)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>3.3387171127560005</v>
+        <v>3.6365183225412512</v>
       </c>
       <c r="G13" s="53"/>
       <c r="H13" s="53"/>
@@ -2858,23 +2858,23 @@
       </c>
       <c r="B14" s="65">
         <f>(((((('rNPV Model'!B13*B$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A14)^(-'rNPV Model'!B47))/$A14))/(1+$A14)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A14)^(-'rNPV Model'!B57))/$A14))/(1+$A14)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A14)^2.5))+MAX(0,((((('rNPV Model'!B13*B$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A14)^(-'rNPV Model'!B47))/$A14))/(1+$A14)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A14)^(-'rNPV Model'!B57))/$A14))/(1+$A14)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A14)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>2.2714162214190177</v>
+        <v>2.5433335081931445</v>
       </c>
       <c r="C14" s="82">
         <f>(((((('rNPV Model'!B13*C$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A14)^(-'rNPV Model'!B47))/$A14))/(1+$A14)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A14)^(-'rNPV Model'!B57))/$A14))/(1+$A14)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A14)^2.5))+MAX(0,((((('rNPV Model'!B13*C$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A14)^(-'rNPV Model'!B47))/$A14))/(1+$A14)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A14)^(-'rNPV Model'!B57))/$A14))/(1+$A14)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A14)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>2.4851549661659358</v>
+        <v>2.7570722529400626</v>
       </c>
       <c r="D14" s="81">
         <f>(((((('rNPV Model'!B13*D$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A14)^(-'rNPV Model'!B47))/$A14))/(1+$A14)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A14)^(-'rNPV Model'!B57))/$A14))/(1+$A14)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A14)^2.5))+MAX(0,((((('rNPV Model'!B13*D$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A14)^(-'rNPV Model'!B47))/$A14))/(1+$A14)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A14)^(-'rNPV Model'!B57))/$A14))/(1+$A14)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A14)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>2.6988937109128535</v>
+        <v>2.9708109976869812</v>
       </c>
       <c r="E14" s="65">
         <f>(((((('rNPV Model'!B13*E$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A14)^(-'rNPV Model'!B47))/$A14))/(1+$A14)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A14)^(-'rNPV Model'!B57))/$A14))/(1+$A14)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A14)^2.5))+MAX(0,((((('rNPV Model'!B13*E$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A14)^(-'rNPV Model'!B47))/$A14))/(1+$A14)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A14)^(-'rNPV Model'!B57))/$A14))/(1+$A14)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A14)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>2.912632455659772</v>
+        <v>3.1845497424338984</v>
       </c>
       <c r="F14" s="66">
         <f>(((((('rNPV Model'!B13*F$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A14)^(-'rNPV Model'!B47))/$A14))/(1+$A14)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A14)^(-'rNPV Model'!B57))/$A14))/(1+$A14)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A14)^2.5))+MAX(0,((((('rNPV Model'!B13*F$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A14)^(-'rNPV Model'!B47))/$A14))/(1+$A14)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A14)^(-'rNPV Model'!B57))/$A14))/(1+$A14)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A14)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>3.1263712004066893</v>
+        <v>3.3982884871808166</v>
       </c>
       <c r="G14" s="53"/>
       <c r="H14" s="53"/>
@@ -2887,23 +2887,23 @@
       </c>
       <c r="B15" s="65">
         <f>(((((('rNPV Model'!B13*B$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A15)^(-'rNPV Model'!B47))/$A15))/(1+$A15)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A15)^(-'rNPV Model'!B57))/$A15))/(1+$A15)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A15)^2.5))+MAX(0,((((('rNPV Model'!B13*B$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A15)^(-'rNPV Model'!B47))/$A15))/(1+$A15)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A15)^(-'rNPV Model'!B57))/$A15))/(1+$A15)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A15)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>2.1491183750950542</v>
+        <v>2.3977221219115066</v>
       </c>
       <c r="C15" s="65">
         <f>(((((('rNPV Model'!B13*C$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A15)^(-'rNPV Model'!B47))/$A15))/(1+$A15)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A15)^(-'rNPV Model'!B57))/$A15))/(1+$A15)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A15)^2.5))+MAX(0,((((('rNPV Model'!B13*C$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A15)^(-'rNPV Model'!B47))/$A15))/(1+$A15)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A15)^(-'rNPV Model'!B57))/$A15))/(1+$A15)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A15)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>2.3457254537393868</v>
+        <v>2.5943292005558396</v>
       </c>
       <c r="D15" s="65">
         <f>(((((('rNPV Model'!B13*D$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A15)^(-'rNPV Model'!B47))/$A15))/(1+$A15)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A15)^(-'rNPV Model'!B57))/$A15))/(1+$A15)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A15)^2.5))+MAX(0,((((('rNPV Model'!B13*D$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A15)^(-'rNPV Model'!B47))/$A15))/(1+$A15)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A15)^(-'rNPV Model'!B57))/$A15))/(1+$A15)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A15)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>2.5423325323837194</v>
+        <v>2.7909362792001722</v>
       </c>
       <c r="E15" s="65">
         <f>(((((('rNPV Model'!B13*E$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A15)^(-'rNPV Model'!B47))/$A15))/(1+$A15)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A15)^(-'rNPV Model'!B57))/$A15))/(1+$A15)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A15)^2.5))+MAX(0,((((('rNPV Model'!B13*E$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A15)^(-'rNPV Model'!B47))/$A15))/(1+$A15)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A15)^(-'rNPV Model'!B57))/$A15))/(1+$A15)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A15)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>2.7389396110280519</v>
+        <v>2.9875433578445039</v>
       </c>
       <c r="F15" s="64">
         <f>(((((('rNPV Model'!B13*F$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A15)^(-'rNPV Model'!B47))/$A15))/(1+$A15)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A15)^(-'rNPV Model'!B57))/$A15))/(1+$A15)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A15)^2.5))+MAX(0,((((('rNPV Model'!B13*F$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A15)^(-'rNPV Model'!B47))/$A15))/(1+$A15)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A15)^(-'rNPV Model'!B57))/$A15))/(1+$A15)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A15)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>2.9355466896723845</v>
+        <v>3.1841504364888369</v>
       </c>
       <c r="G15" s="53"/>
       <c r="H15" s="53"/>
@@ -2936,7 +2936,7 @@
     </row>
     <row r="18" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="92" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B18" s="69"/>
       <c r="C18" s="70"/>
@@ -2951,28 +2951,28 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" s="72" t="s">
+        <v>163</v>
+      </c>
+      <c r="B19" s="72" t="s">
+        <v>164</v>
+      </c>
+      <c r="C19" s="72" t="s">
+        <v>155</v>
+      </c>
+      <c r="D19" s="89" t="s">
+        <v>156</v>
+      </c>
+      <c r="E19" s="89" t="s">
+        <v>184</v>
+      </c>
+      <c r="F19" s="72" t="s">
+        <v>153</v>
+      </c>
+      <c r="G19" s="72" t="s">
         <v>165</v>
       </c>
-      <c r="B19" s="72" t="s">
+      <c r="H19" s="72" t="s">
         <v>166</v>
-      </c>
-      <c r="C19" s="72" t="s">
-        <v>157</v>
-      </c>
-      <c r="D19" s="89" t="s">
-        <v>158</v>
-      </c>
-      <c r="E19" s="89" t="s">
-        <v>186</v>
-      </c>
-      <c r="F19" s="72" t="s">
-        <v>155</v>
-      </c>
-      <c r="G19" s="72" t="s">
-        <v>167</v>
-      </c>
-      <c r="H19" s="72" t="s">
-        <v>168</v>
       </c>
       <c r="I19" s="53"/>
       <c r="J19" s="53"/>
@@ -2980,7 +2980,7 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" s="56" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B20" s="76">
         <v>0.02</v>
@@ -3001,8 +3001,8 @@
         <f>((('rNPV Model'!B13*B20*'rNPV Model'!B16*'rNPV Model'!B18*((1-(1+F20)^(-'rNPV Model'!B47))/F20)/(1+F20)^('rNPV Model'!B8-'rNPV Model'!B10)*C20)+('rNPV Model'!B60*((1-(1+F20)^(-'rNPV Model'!B57))/F20)/(1+F20)^('rNPV Model'!B9-'rNPV Model'!B10)*D20)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+F20)^2.5))+MAX(0,(('rNPV Model'!B13*B20*'rNPV Model'!B16*'rNPV Model'!B18*((1-(1+F20)^(-'rNPV Model'!B47))/F20)/(1+F20)^('rNPV Model'!B8-'rNPV Model'!B10)*C20)+('rNPV Model'!B60*((1-(1+F20)^(-'rNPV Model'!B57))/F20)/(1+F20)^('rNPV Model'!B9-'rNPV Model'!B10)*D20)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+F20)^2.5)))*$D$7+E20+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
         <v>0.75492440175785147</v>
       </c>
-      <c r="H20" s="87" t="s">
-        <v>187</v>
+      <c r="H20" s="1" t="s">
+        <v>192</v>
       </c>
       <c r="I20" s="53"/>
       <c r="J20" s="53"/>
@@ -3010,7 +3010,7 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21" s="56" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B21" s="76">
         <f>'rNPV Model'!B14</f>
@@ -3033,7 +3033,7 @@
       </c>
       <c r="G21" s="74">
         <f>((('rNPV Model'!B13*B21*'rNPV Model'!B16*'rNPV Model'!B18*((1-(1+F21)^(-'rNPV Model'!B47))/F21)/(1+F21)^('rNPV Model'!B8-'rNPV Model'!B10)*C21)+('rNPV Model'!B60*((1-(1+F21)^(-'rNPV Model'!B57))/F21)/(1+F21)^('rNPV Model'!B9-'rNPV Model'!B10)*D21)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+F21)^2.5))+MAX(0,(('rNPV Model'!B13*B21*'rNPV Model'!B16*'rNPV Model'!B18*((1-(1+F21)^(-'rNPV Model'!B47))/F21)/(1+F21)^('rNPV Model'!B8-'rNPV Model'!B10)*C21)+('rNPV Model'!B60*((1-(1+F21)^(-'rNPV Model'!B57))/F21)/(1+F21)^('rNPV Model'!B9-'rNPV Model'!B10)*D21)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+F21)^2.5)))*$D$7+E21+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>2.6988937109128535</v>
+        <v>2.9708109976869812</v>
       </c>
       <c r="H21" s="1"/>
       <c r="I21" s="53"/>
@@ -3042,7 +3042,7 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22" s="56" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B22" s="76">
         <v>0.06</v>
@@ -3061,10 +3061,10 @@
       </c>
       <c r="G22" s="73">
         <f>((('rNPV Model'!B13*B22*'rNPV Model'!B16*'rNPV Model'!B18*((1-(1+F22)^(-'rNPV Model'!B47))/F22)/(1+F22)^('rNPV Model'!B8-'rNPV Model'!B10)*C22)+('rNPV Model'!B60*((1-(1+F22)^(-'rNPV Model'!B57))/F22)/(1+F22)^('rNPV Model'!B9-'rNPV Model'!B10)*D22)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+F22)^2.5))+MAX(0,(('rNPV Model'!B13*B22*'rNPV Model'!B16*'rNPV Model'!B18*((1-(1+F22)^(-'rNPV Model'!B47))/F22)/(1+F22)^('rNPV Model'!B8-'rNPV Model'!B10)*C22)+('rNPV Model'!B60*((1-(1+F22)^(-'rNPV Model'!B57))/F22)/(1+F22)^('rNPV Model'!B9-'rNPV Model'!B10)*D22)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+F22)^2.5)))*$D$7+E22+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>3.2432455328801386</v>
+        <v>3.5831421413477971</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="I22" s="53"/>
       <c r="J22" s="53"/>
@@ -3072,7 +3072,7 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23" s="56" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B23" s="76">
         <v>7.0000000000000007E-2</v>
@@ -3091,10 +3091,10 @@
       </c>
       <c r="G23" s="73">
         <f>((('rNPV Model'!B13*B23*'rNPV Model'!B16*'rNPV Model'!B18*((1-(1+F23)^(-'rNPV Model'!B47))/F23)/(1+F23)^('rNPV Model'!B8-'rNPV Model'!B10)*C23)+('rNPV Model'!B60*((1-(1+F23)^(-'rNPV Model'!B57))/F23)/(1+F23)^('rNPV Model'!B9-'rNPV Model'!B10)*D23)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+F23)^2.5))+MAX(0,(('rNPV Model'!B13*B23*'rNPV Model'!B16*'rNPV Model'!B18*((1-(1+F23)^(-'rNPV Model'!B47))/F23)/(1+F23)^('rNPV Model'!B8-'rNPV Model'!B10)*C23)+('rNPV Model'!B60*((1-(1+F23)^(-'rNPV Model'!B57))/F23)/(1+F23)^('rNPV Model'!B9-'rNPV Model'!B10)*D23)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+F23)^2.5)))*$D$7+E23+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>4.7920915920043878</v>
+        <v>5.2974103868888633</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="I23" s="53"/>
       <c r="J23" s="53"/>
@@ -3102,7 +3102,7 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24" s="56" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B24" s="76">
         <v>0.1</v>
@@ -3114,17 +3114,17 @@
         <v>0.3</v>
       </c>
       <c r="E24" s="90">
-        <v>300</v>
+        <v>250</v>
       </c>
       <c r="F24" s="76">
         <v>0.1</v>
       </c>
       <c r="G24" s="73">
         <f>((('rNPV Model'!B13*B24*'rNPV Model'!B16*'rNPV Model'!B18*((1-(1+F24)^(-'rNPV Model'!B47))/F24)/(1+F24)^('rNPV Model'!B8-'rNPV Model'!B10)*C24)+('rNPV Model'!B60*((1-(1+F24)^(-'rNPV Model'!B57))/F24)/(1+F24)^('rNPV Model'!B9-'rNPV Model'!B10)*D24)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+F24)^2.5))+MAX(0,(('rNPV Model'!B13*B24*'rNPV Model'!B16*'rNPV Model'!B18*((1-(1+F24)^(-'rNPV Model'!B47))/F24)/(1+F24)^('rNPV Model'!B8-'rNPV Model'!B10)*C24)+('rNPV Model'!B60*((1-(1+F24)^(-'rNPV Model'!B57))/F24)/(1+F24)^('rNPV Model'!B9-'rNPV Model'!B10)*D24)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+F24)^2.5)))*$D$7+E24+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>6.7790103856288475</v>
+        <v>7.1437400052351867</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="I24" s="53"/>
       <c r="J24" s="53"/>
@@ -3144,7 +3144,7 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26" s="75" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B26" s="53"/>
       <c r="C26" s="53"/>
@@ -3158,7 +3158,7 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B27" s="53"/>
       <c r="C27" s="53"/>
@@ -3172,7 +3172,7 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B28" s="53"/>
       <c r="C28" s="53"/>
@@ -3186,7 +3186,7 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B29" s="53"/>
       <c r="C29" s="53"/>
@@ -3200,7 +3200,7 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A30" s="87" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B30" s="53"/>
       <c r="C30" s="53"/>
@@ -3214,7 +3214,7 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B31" s="53"/>
       <c r="C31" s="53"/>

</xml_diff>

<commit_message>
Correct fully diluted share count
</commit_message>
<xml_diff>
--- a/PALI_rNPV_Model.xlsx
+++ b/PALI_rNPV_Model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dan\OneDrive\Documents\Equity Research\PALI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F880CFF8-996B-449F-A51C-DCFB25C03BC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B8281C9-0131-448D-B825-1C368E176A8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Diluted Shares" sheetId="1" r:id="rId1"/>
@@ -56,9 +56,6 @@
     <t>WARRANTS</t>
   </si>
   <si>
-    <t>Oct 2025 Offering Overallotment (fully exercised)</t>
-  </si>
-  <si>
     <t>Oct 2025 $138M offering; full overallotment</t>
   </si>
   <si>
@@ -68,15 +65,6 @@
     <t>July 2025 warrant exercise; SH approval Dec 2025</t>
   </si>
   <si>
-    <t>Placement Agent Warrants (est.)</t>
-  </si>
-  <si>
-    <t>Est. from Oct 2025 offering placement agent</t>
-  </si>
-  <si>
-    <t>Legacy / Other Warrants (est.)</t>
-  </si>
-  <si>
     <t>Remaining older warrants from prior financings</t>
   </si>
   <si>
@@ -569,9 +557,6 @@
     <t>UC 6% share: Oral gut-targeted, no systemic immunosuppression vs JAK/biologics. Convenience advantage.</t>
   </si>
   <si>
-    <t xml:space="preserve">Post Oct 2025 raise ($138M gross) + projected $60M future raise + $15.5M warrants </t>
-  </si>
-  <si>
     <t>Platform ($M)</t>
   </si>
   <si>
@@ -596,9 +581,6 @@
     <t>Significant reduction in Fibrosis Genes (scRNA-seq) and/or resolution of Inflammatory Edema (precursor to stricture improvement)</t>
   </si>
   <si>
-    <t>Est. ~150K Symptomatic/Active FSCD patients &amp; ~150k Post-op maintenance; ZERO approved therapies</t>
-  </si>
-  <si>
     <t>first &amp; only therapy; strong first-mover; blending symptomatic/Active penetration (20%) with Post-op maintenance penetration (10%)</t>
   </si>
   <si>
@@ -612,6 +594,24 @@
   </si>
   <si>
     <t>NOLs and R&amp;D credits cover taxes for primary forecasting period</t>
+  </si>
+  <si>
+    <t>Placement Agent Warrants</t>
+  </si>
+  <si>
+    <t>Legacy / Other Warrants</t>
+  </si>
+  <si>
+    <t>Oct 2025 Pre-Funded Warrants (fully exercised)</t>
+  </si>
+  <si>
+    <t>Oct 2025 offering placement agent</t>
+  </si>
+  <si>
+    <t>Est. ~160K Symptomatic/Active FSCD patients &amp; ~160k Post-op maintenance; ZERO approved therapies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Post Oct 2025 raise ($138M gross) + projected $60M future raise + $15.7M warrants </t>
   </si>
 </sst>
 </file>
@@ -1358,8 +1358,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1422,21 +1422,21 @@
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
-        <v>9</v>
+        <v>191</v>
       </c>
       <c r="B8" s="9">
-        <v>25714285</v>
+        <v>57270786</v>
       </c>
       <c r="C8" s="10">
         <v>0.7</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9" s="9">
         <v>8637810</v>
@@ -1445,51 +1445,51 @@
         <v>0.90469999999999995</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
-        <v>13</v>
+        <v>189</v>
       </c>
       <c r="B10" s="9">
-        <v>5000000</v>
+        <v>6850356</v>
       </c>
       <c r="C10" s="10">
-        <v>0.7</v>
+        <v>1.155</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>14</v>
+        <v>192</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
-        <v>15</v>
+        <v>190</v>
       </c>
       <c r="B11" s="9">
-        <v>3000000</v>
+        <v>0</v>
       </c>
       <c r="C11" s="10">
-        <v>1.4</v>
+        <v>0</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="11" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B12" s="12">
         <f>SUM(B8:B11)</f>
-        <v>42352095</v>
+        <v>72758952</v>
       </c>
       <c r="C12" s="13"/>
       <c r="D12" s="13"/>
     </row>
     <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
@@ -1497,7 +1497,7 @@
     </row>
     <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B15" s="9">
         <v>2500000</v>
@@ -1506,12 +1506,12 @@
         <v>1.5</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B16" s="9">
         <v>1500000</v>
@@ -1520,12 +1520,12 @@
         <v>1.2</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B17" s="9">
         <v>500000</v>
@@ -1534,12 +1534,12 @@
         <v>0</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="11" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B18" s="12">
         <f>SUM(B15:B17)</f>
@@ -1550,7 +1550,7 @@
     </row>
     <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="7" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
@@ -1558,7 +1558,7 @@
     </row>
     <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="14" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B21" s="4">
         <v>9230769</v>
@@ -1567,12 +1567,12 @@
         <v>6.5</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="11" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B22" s="12">
         <f>B21</f>
@@ -1583,15 +1583,15 @@
     </row>
     <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="16" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B24" s="17">
         <f>B5+B12+B18+B22</f>
-        <v>205086074</v>
+        <v>235492931</v>
       </c>
       <c r="C24" s="18"/>
       <c r="D24" s="19" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1608,8 +1608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C102"/>
   <sheetViews>
-    <sheetView topLeftCell="A75" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A103" sqref="A103"/>
+    <sheetView topLeftCell="A74" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C84" sqref="C84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1621,490 +1621,490 @@
   <sheetData>
     <row r="1" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="93" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B1" s="93"/>
       <c r="C1" s="93"/>
     </row>
     <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="94" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B2" s="94"/>
       <c r="C2" s="94"/>
     </row>
     <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
     </row>
     <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B5" s="20">
         <v>0.13</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B6" s="20">
         <v>0</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B7" s="91">
         <v>2041</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B8" s="91">
         <v>2031</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B9" s="91">
         <v>2032</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B10" s="91">
         <v>2026</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="7" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
     </row>
     <row r="13" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B13" s="22">
         <v>10000</v>
       </c>
       <c r="C13" s="21" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B14" s="20">
         <v>0.06</v>
       </c>
       <c r="C14" s="21" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B15" s="23">
         <f>B13*B14</f>
         <v>600</v>
       </c>
       <c r="C15" s="21" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B16" s="20">
         <v>0.35</v>
       </c>
       <c r="C16" s="21" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B17" s="23">
         <f>B15*B16</f>
         <v>210</v>
       </c>
       <c r="C17" s="21" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B18" s="24">
         <v>0.6</v>
       </c>
       <c r="C18" s="21" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="7" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
     </row>
     <row r="21" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B21" s="20">
         <v>0.9</v>
       </c>
       <c r="C21" s="21" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B22" s="20">
         <v>0.5</v>
       </c>
       <c r="C22" s="21" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B23" s="20">
         <v>0.7</v>
       </c>
       <c r="C23" s="21" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B24" s="20">
         <v>0.9</v>
       </c>
       <c r="C24" s="21" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B25" s="25">
         <f>B21*B22*B23*B24</f>
         <v>0.28350000000000003</v>
       </c>
       <c r="C25" s="21" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="7" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B27" s="8"/>
       <c r="C27" s="8"/>
     </row>
     <row r="28" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="5" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B28" s="4">
-        <v>300000</v>
+        <v>320000</v>
       </c>
       <c r="C28" s="21" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="5" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B29" s="22">
         <v>40000</v>
       </c>
       <c r="C29" s="21" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="5" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B30" s="20">
         <v>0.15</v>
       </c>
       <c r="C30" s="21" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="5" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B31" s="23">
         <f>B28*B29*B30/1000000</f>
-        <v>1800</v>
+        <v>1920</v>
       </c>
       <c r="C31" s="21" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="5" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B32" s="26">
         <v>0.5</v>
       </c>
       <c r="C32" s="21" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="5" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B33" s="23">
         <f>B31*(1+B32)</f>
-        <v>2700</v>
+        <v>2880</v>
       </c>
       <c r="C33" s="21" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="5" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B34" s="20">
         <v>0.35</v>
       </c>
       <c r="C34" s="21" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="5" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B35" s="23">
         <f>B33*B34</f>
-        <v>944.99999999999989</v>
+        <v>1007.9999999999999</v>
       </c>
       <c r="C35" s="21" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="5" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B36" s="24">
         <v>0.65</v>
       </c>
       <c r="C36" s="21" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="7" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B38" s="8"/>
       <c r="C38" s="8"/>
     </row>
     <row r="39" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="5" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B39" s="20">
         <v>0.8</v>
       </c>
       <c r="C39" s="21" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="5" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B40" s="20">
         <v>0.4</v>
       </c>
       <c r="C40" s="21" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="5" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B41" s="20">
         <v>0.65</v>
       </c>
       <c r="C41" s="21" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="5" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B42" s="20">
         <v>0.85</v>
       </c>
       <c r="C42" s="21" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="5" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B43" s="25">
         <f>B39*B40*B41*B42</f>
         <v>0.17680000000000004</v>
       </c>
       <c r="C43" s="21" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="7" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B45" s="27"/>
       <c r="C45" s="27"/>
     </row>
     <row r="46" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="28" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B46" s="29"/>
       <c r="C46" s="30"/>
     </row>
     <row r="47" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="5" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B47" s="31">
         <f>B7-B8</f>
         <v>10</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="5" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B48" s="23">
         <f>B15</f>
         <v>600</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="5" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B49" s="23">
         <f>B17</f>
         <v>210</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="5" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B50" s="23">
         <f>B17*B18</f>
         <v>126</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="5" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B51" s="23">
         <f>B50*((1-(1+B5)^(-B47))/B5)</f>
         <v>683.70667797006286</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="5" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B52" s="23">
         <f>B51/(1+B5)^(B8-B10)</f>
         <v>371.08859277742692</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="5" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B53" s="32">
         <f>B25</f>
@@ -2114,7 +2114,7 @@
     </row>
     <row r="54" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="33" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B54" s="34">
         <f>B52*B53</f>
@@ -2129,86 +2129,86 @@
     </row>
     <row r="56" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="28" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B56" s="35"/>
       <c r="C56" s="30"/>
     </row>
     <row r="57" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" s="5" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B57" s="31">
         <f>B7-B9</f>
         <v>9</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="5" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B58" s="23">
         <f>B33</f>
-        <v>2700</v>
+        <v>2880</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" s="5" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B59" s="23">
         <f>B35</f>
-        <v>944.99999999999989</v>
+        <v>1007.9999999999999</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="5" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B60" s="23">
         <f>B35*B36</f>
-        <v>614.25</v>
+        <v>655.19999999999993</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" s="5" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B61" s="23">
         <f>B60*((1-(1+B5)^(-B57))/B5)</f>
-        <v>3152.1191622675842</v>
+        <v>3362.2604397520895</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" s="5" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B62" s="23">
         <f>B61/(1+B5)^(B9-B10)</f>
-        <v>1514.0212343141504</v>
+        <v>1614.955983268427</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A63" s="5" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B63" s="32">
         <f>B43</f>
@@ -2218,11 +2218,11 @@
     </row>
     <row r="64" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A64" s="33" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B64" s="34">
         <f>B62*B63</f>
-        <v>267.67895422674184</v>
+        <v>285.52421784185793</v>
       </c>
       <c r="C64" s="30"/>
     </row>
@@ -2233,78 +2233,78 @@
     </row>
     <row r="66" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A66" s="28" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B66" s="35"/>
       <c r="C66" s="30"/>
     </row>
     <row r="67" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A67" s="5" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B67" s="22">
         <v>-25</v>
       </c>
       <c r="C67" s="87" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A68" s="5" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B68" s="36">
         <f>-55*B21*B22</f>
         <v>-24.75</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A69" s="5" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B69" s="22">
         <v>-12</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A70" s="5" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B70" s="36">
         <f>-40*B39*B40</f>
         <v>-12.8</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A71" s="5" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B71" s="22">
         <v>-42</v>
       </c>
       <c r="C71" s="87" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A72" s="5" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B72" s="36">
         <f>(B67+B68+B69+B70+B71)/(1+B5)^2.5</f>
         <v>-85.86499898982558</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -2314,17 +2314,17 @@
     </row>
     <row r="74" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A74" s="11" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B74" s="37">
         <f>B54+B64</f>
-        <v>372.88257027914239</v>
+        <v>390.72783389425848</v>
       </c>
       <c r="C74" s="30"/>
     </row>
     <row r="75" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A75" s="11" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B75" s="37">
         <f>B72</f>
@@ -2334,14 +2334,14 @@
     </row>
     <row r="76" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A76" s="11" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B76" s="37">
         <f>B74+B75</f>
-        <v>287.01757128931683</v>
+        <v>304.86283490443293</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -2351,32 +2351,32 @@
     </row>
     <row r="78" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A78" s="28" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B78" s="38"/>
       <c r="C78" s="30"/>
     </row>
     <row r="79" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A79" s="83" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B79" s="36">
         <f>MAX(0,B76)*0.25</f>
-        <v>71.754392822329208</v>
+        <v>76.215708726108232</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A80" s="5" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B80" s="22">
         <v>50</v>
       </c>
       <c r="C80" s="87" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -2386,25 +2386,25 @@
     </row>
     <row r="82" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A82" s="28" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B82" s="38"/>
       <c r="C82" s="30"/>
     </row>
     <row r="83" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A83" s="5" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B83" s="22">
-        <v>205.5</v>
-      </c>
-      <c r="C83" s="87" t="s">
-        <v>180</v>
+        <v>205.7</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A84" s="5" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B84" s="22">
         <v>-5</v>
@@ -2413,14 +2413,14 @@
     </row>
     <row r="85" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A85" s="33" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B85" s="39">
         <f>B83+B84</f>
-        <v>200.5</v>
+        <v>200.7</v>
       </c>
       <c r="C85" s="40" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -2430,14 +2430,14 @@
     </row>
     <row r="87" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A87" s="16" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B87" s="41">
         <f>B76+B79+B80+B85</f>
-        <v>609.27196411164607</v>
+        <v>631.77854363054121</v>
       </c>
       <c r="C87" s="42" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -2447,28 +2447,28 @@
     </row>
     <row r="89" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A89" s="7" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B89" s="43"/>
       <c r="C89" s="27"/>
     </row>
     <row r="90" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A90" s="5" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B90" s="44">
         <f>'Diluted Shares'!B24</f>
-        <v>205086074</v>
+        <v>235492931</v>
       </c>
       <c r="C90" s="30"/>
     </row>
     <row r="91" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A91" s="45" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B91" s="46">
         <f>B87*1000000/B90</f>
-        <v>2.9708109976869812</v>
+        <v>2.6827919672482281</v>
       </c>
       <c r="C91" s="30"/>
     </row>
@@ -2479,7 +2479,7 @@
     </row>
     <row r="93" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A93" s="5" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B93" s="47">
         <v>1.74</v>
@@ -2488,11 +2488,11 @@
     </row>
     <row r="94" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A94" s="5" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B94" s="25">
         <f>(B91-B93)/B93</f>
-        <v>0.70736264234883983</v>
+        <v>0.54183446393576329</v>
       </c>
       <c r="C94" s="30"/>
     </row>
@@ -2503,13 +2503,13 @@
     </row>
     <row r="96" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A96" s="5" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B96" s="10">
         <v>12</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -2519,54 +2519,54 @@
     </row>
     <row r="98" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A98" s="7" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B98" s="48"/>
       <c r="C98" s="48"/>
     </row>
     <row r="99" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A99" s="5" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B99" s="49">
         <f>B85*1000000/B90</f>
-        <v>0.97763829639646815</v>
+        <v>0.8522548814851687</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A100" s="5" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B100" s="49">
         <f>B76*1000000/B90</f>
-        <v>1.3994981019009454</v>
+        <v>1.2945731899885902</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A101" s="5" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B101" s="49">
         <f>(B79+B80)*1000000/B90</f>
-        <v>0.59367459938956757</v>
+        <v>0.53596389577446912</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A102" s="50" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B102" s="51">
         <f>B91</f>
-        <v>2.9708109976869812</v>
+        <v>2.6827919672482281</v>
       </c>
       <c r="C102" s="1"/>
     </row>
@@ -2584,7 +2584,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
@@ -2596,7 +2596,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="52" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B1" s="53"/>
       <c r="C1" s="53"/>
@@ -2622,7 +2622,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="54" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B3" s="55"/>
       <c r="C3" s="55"/>
@@ -2636,14 +2636,14 @@
     </row>
     <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="56" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B4" s="77">
         <f>'rNPV Model'!B5</f>
         <v>0.13</v>
       </c>
       <c r="C4" s="80" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D4" s="77">
         <f>'rNPV Model'!B14</f>
@@ -2658,14 +2658,14 @@
     </row>
     <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="57" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B5" s="77">
         <f>'rNPV Model'!B25</f>
         <v>0.28350000000000003</v>
       </c>
       <c r="C5" s="59" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="D5" s="77">
         <f>'rNPV Model'!B43</f>
@@ -2680,18 +2680,18 @@
     </row>
     <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="57" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B6" s="84">
         <f>'rNPV Model'!B90</f>
-        <v>205086074</v>
+        <v>235492931</v>
       </c>
       <c r="C6" s="59" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="D6" s="85">
         <f>'rNPV Model'!B85</f>
-        <v>200.5</v>
+        <v>200.7</v>
       </c>
       <c r="E6" s="60"/>
       <c r="F6" s="60"/>
@@ -2702,14 +2702,14 @@
     </row>
     <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="80" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B7" s="85">
         <f>'rNPV Model'!B80</f>
         <v>50</v>
       </c>
       <c r="C7" s="79" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D7" s="76">
         <f>0.25</f>
@@ -2724,14 +2724,14 @@
     </row>
     <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="78" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="B8" s="61">
         <f>'rNPV Model'!B91</f>
-        <v>2.9708109976869812</v>
+        <v>2.6827919672482281</v>
       </c>
       <c r="C8" s="59" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D8" s="86">
         <f>'rNPV Model'!B93</f>
@@ -2758,7 +2758,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="54" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B10" s="55"/>
       <c r="C10" s="55"/>
@@ -2772,7 +2772,7 @@
     </row>
     <row r="11" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="62" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B11" s="63">
         <v>0.02</v>
@@ -2800,23 +2800,23 @@
       </c>
       <c r="B12" s="64">
         <f>(((((('rNPV Model'!B13*B$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A12)^(-'rNPV Model'!B47))/$A12))/(1+$A12)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A12)^(-'rNPV Model'!B57))/$A12))/(1+$A12)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A12)^2.5))+MAX(0,((((('rNPV Model'!B13*B$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A12)^(-'rNPV Model'!B47))/$A12))/(1+$A12)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A12)^(-'rNPV Model'!B57))/$A12))/(1+$A12)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A12)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>2.8873222717278568</v>
+        <v>2.6291253861478365</v>
       </c>
       <c r="C12" s="64">
         <f>(((((('rNPV Model'!B13*C$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A12)^(-'rNPV Model'!B47))/$A12))/(1+$A12)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A12)^(-'rNPV Model'!B57))/$A12))/(1+$A12)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A12)^2.5))+MAX(0,((((('rNPV Model'!B13*C$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A12)^(-'rNPV Model'!B47))/$A12))/(1+$A12)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A12)^(-'rNPV Model'!B57))/$A12))/(1+$A12)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A12)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>3.1409635687666482</v>
+        <v>2.8500165084123674</v>
       </c>
       <c r="D12" s="64">
         <f>(((((('rNPV Model'!B13*D$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A12)^(-'rNPV Model'!B47))/$A12))/(1+$A12)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A12)^(-'rNPV Model'!B57))/$A12))/(1+$A12)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A12)^2.5))+MAX(0,((((('rNPV Model'!B13*D$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A12)^(-'rNPV Model'!B47))/$A12))/(1+$A12)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A12)^(-'rNPV Model'!B57))/$A12))/(1+$A12)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A12)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>3.3946048658054391</v>
+        <v>3.0709076306768974</v>
       </c>
       <c r="E12" s="64">
         <f>(((((('rNPV Model'!B13*E$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A12)^(-'rNPV Model'!B47))/$A12))/(1+$A12)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A12)^(-'rNPV Model'!B57))/$A12))/(1+$A12)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A12)^2.5))+MAX(0,((((('rNPV Model'!B13*E$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A12)^(-'rNPV Model'!B47))/$A12))/(1+$A12)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A12)^(-'rNPV Model'!B57))/$A12))/(1+$A12)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A12)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>3.6482461628442318</v>
+        <v>3.2917987529414283</v>
       </c>
       <c r="F12" s="64">
         <f>(((((('rNPV Model'!B13*F$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A12)^(-'rNPV Model'!B47))/$A12))/(1+$A12)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A12)^(-'rNPV Model'!B57))/$A12))/(1+$A12)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A12)^2.5))+MAX(0,((((('rNPV Model'!B13*F$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A12)^(-'rNPV Model'!B47))/$A12))/(1+$A12)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A12)^(-'rNPV Model'!B57))/$A12))/(1+$A12)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A12)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>3.9018874598830227</v>
+        <v>3.5126898752059583</v>
       </c>
       <c r="G12" s="53"/>
       <c r="H12" s="53"/>
@@ -2829,23 +2829,23 @@
       </c>
       <c r="B13" s="65">
         <f>(((((('rNPV Model'!B13*B$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A13)^(-'rNPV Model'!B47))/$A13))/(1+$A13)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A13)^(-'rNPV Model'!B57))/$A13))/(1+$A13)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A13)^2.5))+MAX(0,((((('rNPV Model'!B13*B$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A13)^(-'rNPV Model'!B47))/$A13))/(1+$A13)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A13)^(-'rNPV Model'!B57))/$A13))/(1+$A13)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A13)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>2.7058141433111724</v>
+        <v>2.4610282336002887</v>
       </c>
       <c r="C13" s="65">
         <f>(((((('rNPV Model'!B13*C$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A13)^(-'rNPV Model'!B47))/$A13))/(1+$A13)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A13)^(-'rNPV Model'!B57))/$A13))/(1+$A13)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A13)^2.5))+MAX(0,((((('rNPV Model'!B13*C$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A13)^(-'rNPV Model'!B47))/$A13))/(1+$A13)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A13)^(-'rNPV Model'!B57))/$A13))/(1+$A13)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A13)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>2.938490188118692</v>
+        <v>2.6636611378695991</v>
       </c>
       <c r="D13" s="65">
         <f>(((((('rNPV Model'!B13*D$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A13)^(-'rNPV Model'!B47))/$A13))/(1+$A13)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A13)^(-'rNPV Model'!B57))/$A13))/(1+$A13)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A13)^2.5))+MAX(0,((((('rNPV Model'!B13*D$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A13)^(-'rNPV Model'!B47))/$A13))/(1+$A13)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A13)^(-'rNPV Model'!B57))/$A13))/(1+$A13)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A13)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>3.1711662329262116</v>
+        <v>2.8662940421389091</v>
       </c>
       <c r="E13" s="65">
         <f>(((((('rNPV Model'!B13*E$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A13)^(-'rNPV Model'!B47))/$A13))/(1+$A13)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A13)^(-'rNPV Model'!B57))/$A13))/(1+$A13)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A13)^2.5))+MAX(0,((((('rNPV Model'!B13*E$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A13)^(-'rNPV Model'!B47))/$A13))/(1+$A13)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A13)^(-'rNPV Model'!B57))/$A13))/(1+$A13)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A13)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>3.4038422777337307</v>
+        <v>3.0689269464082196</v>
       </c>
       <c r="F13" s="64">
         <f>(((((('rNPV Model'!B13*F$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A13)^(-'rNPV Model'!B47))/$A13))/(1+$A13)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A13)^(-'rNPV Model'!B57))/$A13))/(1+$A13)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A13)^2.5))+MAX(0,((((('rNPV Model'!B13*F$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A13)^(-'rNPV Model'!B47))/$A13))/(1+$A13)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A13)^(-'rNPV Model'!B57))/$A13))/(1+$A13)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A13)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>3.6365183225412512</v>
+        <v>3.2715598506775296</v>
       </c>
       <c r="G13" s="53"/>
       <c r="H13" s="53"/>
@@ -2858,23 +2858,23 @@
       </c>
       <c r="B14" s="65">
         <f>(((((('rNPV Model'!B13*B$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A14)^(-'rNPV Model'!B47))/$A14))/(1+$A14)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A14)^(-'rNPV Model'!B57))/$A14))/(1+$A14)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A14)^2.5))+MAX(0,((((('rNPV Model'!B13*B$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A14)^(-'rNPV Model'!B47))/$A14))/(1+$A14)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A14)^(-'rNPV Model'!B57))/$A14))/(1+$A14)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A14)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>2.5433335081931445</v>
+        <v>2.3105103888951724</v>
       </c>
       <c r="C14" s="82">
         <f>(((((('rNPV Model'!B13*C$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A14)^(-'rNPV Model'!B47))/$A14))/(1+$A14)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A14)^(-'rNPV Model'!B57))/$A14))/(1+$A14)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A14)^2.5))+MAX(0,((((('rNPV Model'!B13*C$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A14)^(-'rNPV Model'!B47))/$A14))/(1+$A14)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A14)^(-'rNPV Model'!B57))/$A14))/(1+$A14)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A14)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>2.7570722529400626</v>
+        <v>2.4966511780716996</v>
       </c>
       <c r="D14" s="81">
         <f>(((((('rNPV Model'!B13*D$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A14)^(-'rNPV Model'!B47))/$A14))/(1+$A14)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A14)^(-'rNPV Model'!B57))/$A14))/(1+$A14)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A14)^2.5))+MAX(0,((((('rNPV Model'!B13*D$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A14)^(-'rNPV Model'!B47))/$A14))/(1+$A14)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A14)^(-'rNPV Model'!B57))/$A14))/(1+$A14)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A14)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>2.9708109976869812</v>
+        <v>2.6827919672482281</v>
       </c>
       <c r="E14" s="65">
         <f>(((((('rNPV Model'!B13*E$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A14)^(-'rNPV Model'!B47))/$A14))/(1+$A14)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A14)^(-'rNPV Model'!B57))/$A14))/(1+$A14)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A14)^2.5))+MAX(0,((((('rNPV Model'!B13*E$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A14)^(-'rNPV Model'!B47))/$A14))/(1+$A14)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A14)^(-'rNPV Model'!B57))/$A14))/(1+$A14)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A14)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>3.1845497424338984</v>
+        <v>2.8689327564247553</v>
       </c>
       <c r="F14" s="66">
         <f>(((((('rNPV Model'!B13*F$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A14)^(-'rNPV Model'!B47))/$A14))/(1+$A14)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A14)^(-'rNPV Model'!B57))/$A14))/(1+$A14)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A14)^2.5))+MAX(0,((((('rNPV Model'!B13*F$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A14)^(-'rNPV Model'!B47))/$A14))/(1+$A14)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A14)^(-'rNPV Model'!B57))/$A14))/(1+$A14)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A14)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>3.3982884871808166</v>
+        <v>3.055073545601283</v>
       </c>
       <c r="G14" s="53"/>
       <c r="H14" s="53"/>
@@ -2887,23 +2887,23 @@
       </c>
       <c r="B15" s="65">
         <f>(((((('rNPV Model'!B13*B$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A15)^(-'rNPV Model'!B47))/$A15))/(1+$A15)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A15)^(-'rNPV Model'!B57))/$A15))/(1+$A15)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A15)^2.5))+MAX(0,((((('rNPV Model'!B13*B$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A15)^(-'rNPV Model'!B47))/$A15))/(1+$A15)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A15)^(-'rNPV Model'!B57))/$A15))/(1+$A15)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A15)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>2.3977221219115066</v>
+        <v>2.1755790329531837</v>
       </c>
       <c r="C15" s="65">
         <f>(((((('rNPV Model'!B13*C$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A15)^(-'rNPV Model'!B47))/$A15))/(1+$A15)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A15)^(-'rNPV Model'!B57))/$A15))/(1+$A15)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A15)^2.5))+MAX(0,((((('rNPV Model'!B13*C$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A15)^(-'rNPV Model'!B47))/$A15))/(1+$A15)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A15)^(-'rNPV Model'!B57))/$A15))/(1+$A15)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A15)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>2.5943292005558396</v>
+        <v>2.3468001974635335</v>
       </c>
       <c r="D15" s="65">
         <f>(((((('rNPV Model'!B13*D$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A15)^(-'rNPV Model'!B47))/$A15))/(1+$A15)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A15)^(-'rNPV Model'!B57))/$A15))/(1+$A15)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A15)^2.5))+MAX(0,((((('rNPV Model'!B13*D$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A15)^(-'rNPV Model'!B47))/$A15))/(1+$A15)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A15)^(-'rNPV Model'!B57))/$A15))/(1+$A15)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A15)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>2.7909362792001722</v>
+        <v>2.5180213619738825</v>
       </c>
       <c r="E15" s="65">
         <f>(((((('rNPV Model'!B13*E$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A15)^(-'rNPV Model'!B47))/$A15))/(1+$A15)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A15)^(-'rNPV Model'!B57))/$A15))/(1+$A15)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A15)^2.5))+MAX(0,((((('rNPV Model'!B13*E$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A15)^(-'rNPV Model'!B47))/$A15))/(1+$A15)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A15)^(-'rNPV Model'!B57))/$A15))/(1+$A15)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A15)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>2.9875433578445039</v>
+        <v>2.6892425264842323</v>
       </c>
       <c r="F15" s="64">
         <f>(((((('rNPV Model'!B13*F$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A15)^(-'rNPV Model'!B47))/$A15))/(1+$A15)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A15)^(-'rNPV Model'!B57))/$A15))/(1+$A15)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A15)^2.5))+MAX(0,((((('rNPV Model'!B13*F$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A15)^(-'rNPV Model'!B47))/$A15))/(1+$A15)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A15)^(-'rNPV Model'!B57))/$A15))/(1+$A15)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A15)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>3.1841504364888369</v>
+        <v>2.8604636909945822</v>
       </c>
       <c r="G15" s="53"/>
       <c r="H15" s="53"/>
@@ -2936,7 +2936,7 @@
     </row>
     <row r="18" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="92" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B18" s="69"/>
       <c r="C18" s="70"/>
@@ -2951,28 +2951,28 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" s="72" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B19" s="72" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C19" s="72" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D19" s="89" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="E19" s="89" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="F19" s="72" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="G19" s="72" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="H19" s="72" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="I19" s="53"/>
       <c r="J19" s="53"/>
@@ -2980,7 +2980,7 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" s="56" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B20" s="76">
         <v>0.02</v>
@@ -2999,10 +2999,10 @@
       </c>
       <c r="G20" s="73">
         <f>((('rNPV Model'!B13*B20*'rNPV Model'!B16*'rNPV Model'!B18*((1-(1+F20)^(-'rNPV Model'!B47))/F20)/(1+F20)^('rNPV Model'!B8-'rNPV Model'!B10)*C20)+('rNPV Model'!B60*((1-(1+F20)^(-'rNPV Model'!B57))/F20)/(1+F20)^('rNPV Model'!B9-'rNPV Model'!B10)*D20)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+F20)^2.5))+MAX(0,(('rNPV Model'!B13*B20*'rNPV Model'!B16*'rNPV Model'!B18*((1-(1+F20)^(-'rNPV Model'!B47))/F20)/(1+F20)^('rNPV Model'!B8-'rNPV Model'!B10)*C20)+('rNPV Model'!B60*((1-(1+F20)^(-'rNPV Model'!B57))/F20)/(1+F20)^('rNPV Model'!B9-'rNPV Model'!B10)*D20)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+F20)^2.5)))*$D$7+E20+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>0.75492440175785147</v>
+        <v>0.65829781414252497</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="I20" s="53"/>
       <c r="J20" s="53"/>
@@ -3010,7 +3010,7 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21" s="56" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B21" s="76">
         <f>'rNPV Model'!B14</f>
@@ -3033,7 +3033,7 @@
       </c>
       <c r="G21" s="74">
         <f>((('rNPV Model'!B13*B21*'rNPV Model'!B16*'rNPV Model'!B18*((1-(1+F21)^(-'rNPV Model'!B47))/F21)/(1+F21)^('rNPV Model'!B8-'rNPV Model'!B10)*C21)+('rNPV Model'!B60*((1-(1+F21)^(-'rNPV Model'!B57))/F21)/(1+F21)^('rNPV Model'!B9-'rNPV Model'!B10)*D21)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+F21)^2.5))+MAX(0,(('rNPV Model'!B13*B21*'rNPV Model'!B16*'rNPV Model'!B18*((1-(1+F21)^(-'rNPV Model'!B47))/F21)/(1+F21)^('rNPV Model'!B8-'rNPV Model'!B10)*C21)+('rNPV Model'!B60*((1-(1+F21)^(-'rNPV Model'!B57))/F21)/(1+F21)^('rNPV Model'!B9-'rNPV Model'!B10)*D21)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+F21)^2.5)))*$D$7+E21+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>2.9708109976869812</v>
+        <v>2.6827919672482281</v>
       </c>
       <c r="H21" s="1"/>
       <c r="I21" s="53"/>
@@ -3042,7 +3042,7 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22" s="56" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B22" s="76">
         <v>0.06</v>
@@ -3061,10 +3061,10 @@
       </c>
       <c r="G22" s="73">
         <f>((('rNPV Model'!B13*B22*'rNPV Model'!B16*'rNPV Model'!B18*((1-(1+F22)^(-'rNPV Model'!B47))/F22)/(1+F22)^('rNPV Model'!B8-'rNPV Model'!B10)*C22)+('rNPV Model'!B60*((1-(1+F22)^(-'rNPV Model'!B57))/F22)/(1+F22)^('rNPV Model'!B9-'rNPV Model'!B10)*D22)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+F22)^2.5))+MAX(0,(('rNPV Model'!B13*B22*'rNPV Model'!B16*'rNPV Model'!B18*((1-(1+F22)^(-'rNPV Model'!B47))/F22)/(1+F22)^('rNPV Model'!B8-'rNPV Model'!B10)*C22)+('rNPV Model'!B60*((1-(1+F22)^(-'rNPV Model'!B57))/F22)/(1+F22)^('rNPV Model'!B9-'rNPV Model'!B10)*D22)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+F22)^2.5)))*$D$7+E22+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>3.5831421413477971</v>
+        <v>3.2397396198342441</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="I22" s="53"/>
       <c r="J22" s="53"/>
@@ -3072,7 +3072,7 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23" s="56" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B23" s="76">
         <v>7.0000000000000007E-2</v>
@@ -3091,10 +3091,10 @@
       </c>
       <c r="G23" s="73">
         <f>((('rNPV Model'!B13*B23*'rNPV Model'!B16*'rNPV Model'!B18*((1-(1+F23)^(-'rNPV Model'!B47))/F23)/(1+F23)^('rNPV Model'!B8-'rNPV Model'!B10)*C23)+('rNPV Model'!B60*((1-(1+F23)^(-'rNPV Model'!B57))/F23)/(1+F23)^('rNPV Model'!B9-'rNPV Model'!B10)*D23)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+F23)^2.5))+MAX(0,(('rNPV Model'!B13*B23*'rNPV Model'!B16*'rNPV Model'!B18*((1-(1+F23)^(-'rNPV Model'!B47))/F23)/(1+F23)^('rNPV Model'!B8-'rNPV Model'!B10)*C23)+('rNPV Model'!B60*((1-(1+F23)^(-'rNPV Model'!B57))/F23)/(1+F23)^('rNPV Model'!B9-'rNPV Model'!B10)*D23)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+F23)^2.5)))*$D$7+E23+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>5.2974103868888633</v>
+        <v>4.7902866252845833</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="I23" s="53"/>
       <c r="J23" s="53"/>
@@ -3102,7 +3102,7 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24" s="56" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B24" s="76">
         <v>0.1</v>
@@ -3121,10 +3121,10 @@
       </c>
       <c r="G24" s="73">
         <f>((('rNPV Model'!B13*B24*'rNPV Model'!B16*'rNPV Model'!B18*((1-(1+F24)^(-'rNPV Model'!B47))/F24)/(1+F24)^('rNPV Model'!B8-'rNPV Model'!B10)*C24)+('rNPV Model'!B60*((1-(1+F24)^(-'rNPV Model'!B57))/F24)/(1+F24)^('rNPV Model'!B9-'rNPV Model'!B10)*D24)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+F24)^2.5))+MAX(0,(('rNPV Model'!B13*B24*'rNPV Model'!B16*'rNPV Model'!B18*((1-(1+F24)^(-'rNPV Model'!B47))/F24)/(1+F24)^('rNPV Model'!B8-'rNPV Model'!B10)*C24)+('rNPV Model'!B60*((1-(1+F24)^(-'rNPV Model'!B57))/F24)/(1+F24)^('rNPV Model'!B9-'rNPV Model'!B10)*D24)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+F24)^2.5)))*$D$7+E24+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>7.1437400052351867</v>
+        <v>6.4341718081255479</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="I24" s="53"/>
       <c r="J24" s="53"/>
@@ -3144,7 +3144,7 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26" s="75" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B26" s="53"/>
       <c r="C26" s="53"/>
@@ -3158,7 +3158,7 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="B27" s="53"/>
       <c r="C27" s="53"/>
@@ -3172,7 +3172,7 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="B28" s="53"/>
       <c r="C28" s="53"/>
@@ -3186,7 +3186,7 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="B29" s="53"/>
       <c r="C29" s="53"/>
@@ -3200,7 +3200,7 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A30" s="87" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="B30" s="53"/>
       <c r="C30" s="53"/>
@@ -3214,7 +3214,7 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B31" s="53"/>
       <c r="C31" s="53"/>

</xml_diff>

<commit_message>
Fully diluted clarification and patient update
</commit_message>
<xml_diff>
--- a/PALI_rNPV_Model.xlsx
+++ b/PALI_rNPV_Model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dan\OneDrive\Documents\Equity Research\PALI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B8281C9-0131-448D-B825-1C368E176A8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C465893-DE6D-48FB-93E4-013002615616}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -56,9 +56,6 @@
     <t>WARRANTS</t>
   </si>
   <si>
-    <t>Oct 2025 $138M offering; full overallotment</t>
-  </si>
-  <si>
     <t>Replacement Warrants (July 2025 inducement)</t>
   </si>
   <si>
@@ -581,18 +578,12 @@
     <t>Significant reduction in Fibrosis Genes (scRNA-seq) and/or resolution of Inflammatory Edema (precursor to stricture improvement)</t>
   </si>
   <si>
-    <t>first &amp; only therapy; strong first-mover; blending symptomatic/Active penetration (20%) with Post-op maintenance penetration (10%)</t>
-  </si>
-  <si>
     <t>$55M × P(Ph1b→Ph2) × P(Ph2→Ph3)</t>
   </si>
   <si>
     <t>$40M × P(Ph1b→Ph2) × P(Ph2→Ph3)</t>
   </si>
   <si>
-    <t>Zero fibrosis signals, FSCD discontinued, and UC becomes a commercial flop (immediate cash value is still $0.98)</t>
-  </si>
-  <si>
     <t>NOLs and R&amp;D credits cover taxes for primary forecasting period</t>
   </si>
   <si>
@@ -612,6 +603,15 @@
   </si>
   <si>
     <t xml:space="preserve">Post Oct 2025 raise ($138M gross) + projected $60M future raise + $15.7M warrants </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sold along with ~140M shares for $0.70 in the Oct 2025 $138M offering; </t>
+  </si>
+  <si>
+    <t>first &amp; only therapy; strong first-mover; blending symptomatic/Active penetration (22%) with Post-op maintenance penetration (10%)</t>
+  </si>
+  <si>
+    <t>Zero fibrosis signals, FSCD discontinued, and UC becomes a commercial flop (immediate cash value is still $0.85)</t>
   </si>
 </sst>
 </file>
@@ -1422,7 +1422,7 @@
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B8" s="9">
         <v>57270786</v>
@@ -1431,12 +1431,12 @@
         <v>0.7</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>9</v>
+        <v>192</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" s="9">
         <v>8637810</v>
@@ -1445,12 +1445,12 @@
         <v>0.90469999999999995</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B10" s="9">
         <v>6850356</v>
@@ -1459,12 +1459,12 @@
         <v>1.155</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B11" s="9">
         <v>0</v>
@@ -1473,12 +1473,12 @@
         <v>0</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B12" s="12">
         <f>SUM(B8:B11)</f>
@@ -1489,7 +1489,7 @@
     </row>
     <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
@@ -1497,7 +1497,7 @@
     </row>
     <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15" s="9">
         <v>2500000</v>
@@ -1506,12 +1506,12 @@
         <v>1.5</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B16" s="9">
         <v>1500000</v>
@@ -1520,12 +1520,12 @@
         <v>1.2</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B17" s="9">
         <v>500000</v>
@@ -1534,12 +1534,12 @@
         <v>0</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B18" s="12">
         <f>SUM(B15:B17)</f>
@@ -1550,7 +1550,7 @@
     </row>
     <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
@@ -1558,7 +1558,7 @@
     </row>
     <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B21" s="4">
         <v>9230769</v>
@@ -1567,12 +1567,12 @@
         <v>6.5</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B22" s="12">
         <f>B21</f>
@@ -1583,7 +1583,7 @@
     </row>
     <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B24" s="17">
         <f>B5+B12+B18+B22</f>
@@ -1591,7 +1591,7 @@
       </c>
       <c r="C24" s="18"/>
       <c r="D24" s="19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -1608,8 +1608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C102"/>
   <sheetViews>
-    <sheetView topLeftCell="A74" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C84" sqref="C84"/>
+    <sheetView topLeftCell="A69" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1621,490 +1621,490 @@
   <sheetData>
     <row r="1" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="93" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B1" s="93"/>
       <c r="C1" s="93"/>
     </row>
     <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="94" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B2" s="94"/>
       <c r="C2" s="94"/>
     </row>
     <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
     </row>
     <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B5" s="20">
         <v>0.13</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B6" s="20">
         <v>0</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B7" s="91">
         <v>2041</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B8" s="91">
         <v>2031</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B9" s="91">
         <v>2032</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B10" s="91">
         <v>2026</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
     </row>
     <row r="13" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B13" s="22">
         <v>10000</v>
       </c>
       <c r="C13" s="21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B14" s="20">
         <v>0.06</v>
       </c>
       <c r="C14" s="21" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B15" s="23">
         <f>B13*B14</f>
         <v>600</v>
       </c>
       <c r="C15" s="21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B16" s="20">
         <v>0.35</v>
       </c>
       <c r="C16" s="21" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B17" s="23">
         <f>B15*B16</f>
         <v>210</v>
       </c>
       <c r="C17" s="21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B18" s="24">
         <v>0.6</v>
       </c>
       <c r="C18" s="21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
     </row>
     <row r="21" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B21" s="20">
         <v>0.9</v>
       </c>
       <c r="C21" s="21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B22" s="20">
         <v>0.5</v>
       </c>
       <c r="C22" s="21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B23" s="20">
         <v>0.7</v>
       </c>
       <c r="C23" s="21" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B24" s="20">
         <v>0.9</v>
       </c>
       <c r="C24" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B25" s="25">
         <f>B21*B22*B23*B24</f>
         <v>0.28350000000000003</v>
       </c>
       <c r="C25" s="21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B27" s="8"/>
       <c r="C27" s="8"/>
     </row>
     <row r="28" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B28" s="4">
         <v>320000</v>
       </c>
       <c r="C28" s="21" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B29" s="22">
         <v>40000</v>
       </c>
       <c r="C29" s="21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B30" s="20">
-        <v>0.15</v>
+        <v>0.16</v>
       </c>
       <c r="C30" s="21" t="s">
-        <v>184</v>
+        <v>193</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B31" s="23">
         <f>B28*B29*B30/1000000</f>
-        <v>1920</v>
+        <v>2048</v>
       </c>
       <c r="C31" s="21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B32" s="26">
         <v>0.5</v>
       </c>
       <c r="C32" s="21" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B33" s="23">
         <f>B31*(1+B32)</f>
-        <v>2880</v>
+        <v>3072</v>
       </c>
       <c r="C33" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B34" s="20">
         <v>0.35</v>
       </c>
       <c r="C34" s="21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B35" s="23">
         <f>B33*B34</f>
-        <v>1007.9999999999999</v>
+        <v>1075.1999999999998</v>
       </c>
       <c r="C35" s="21" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B36" s="24">
         <v>0.65</v>
       </c>
       <c r="C36" s="21" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B38" s="8"/>
       <c r="C38" s="8"/>
     </row>
     <row r="39" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B39" s="20">
         <v>0.8</v>
       </c>
       <c r="C39" s="21" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B40" s="20">
         <v>0.4</v>
       </c>
       <c r="C40" s="21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B41" s="20">
         <v>0.65</v>
       </c>
       <c r="C41" s="21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B42" s="20">
         <v>0.85</v>
       </c>
       <c r="C42" s="21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B43" s="25">
         <f>B39*B40*B41*B42</f>
         <v>0.17680000000000004</v>
       </c>
       <c r="C43" s="21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B45" s="27"/>
       <c r="C45" s="27"/>
     </row>
     <row r="46" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="28" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B46" s="29"/>
       <c r="C46" s="30"/>
     </row>
     <row r="47" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B47" s="31">
         <f>B7-B8</f>
         <v>10</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B48" s="23">
         <f>B15</f>
         <v>600</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B49" s="23">
         <f>B17</f>
         <v>210</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B50" s="23">
         <f>B17*B18</f>
         <v>126</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B51" s="23">
         <f>B50*((1-(1+B5)^(-B47))/B5)</f>
         <v>683.70667797006286</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B52" s="23">
         <f>B51/(1+B5)^(B8-B10)</f>
         <v>371.08859277742692</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B53" s="32">
         <f>B25</f>
@@ -2114,7 +2114,7 @@
     </row>
     <row r="54" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="33" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B54" s="34">
         <f>B52*B53</f>
@@ -2129,86 +2129,86 @@
     </row>
     <row r="56" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="28" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B56" s="35"/>
       <c r="C56" s="30"/>
     </row>
     <row r="57" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B57" s="31">
         <f>B7-B9</f>
         <v>9</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B58" s="23">
         <f>B33</f>
-        <v>2880</v>
+        <v>3072</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B59" s="23">
         <f>B35</f>
-        <v>1007.9999999999999</v>
+        <v>1075.1999999999998</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B60" s="23">
         <f>B35*B36</f>
-        <v>655.19999999999993</v>
+        <v>698.87999999999988</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B61" s="23">
         <f>B60*((1-(1+B5)^(-B57))/B5)</f>
-        <v>3362.2604397520895</v>
+        <v>3586.4111357355619</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B62" s="23">
         <f>B61/(1+B5)^(B9-B10)</f>
-        <v>1614.955983268427</v>
+        <v>1722.6197154863219</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A63" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B63" s="32">
         <f>B43</f>
@@ -2218,11 +2218,11 @@
     </row>
     <row r="64" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A64" s="33" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B64" s="34">
         <f>B62*B63</f>
-        <v>285.52421784185793</v>
+        <v>304.55916569798177</v>
       </c>
       <c r="C64" s="30"/>
     </row>
@@ -2233,78 +2233,78 @@
     </row>
     <row r="66" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A66" s="28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B66" s="35"/>
       <c r="C66" s="30"/>
     </row>
     <row r="67" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A67" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B67" s="22">
         <v>-25</v>
       </c>
       <c r="C67" s="87" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A68" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B68" s="36">
         <f>-55*B21*B22</f>
         <v>-24.75</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A69" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B69" s="22">
         <v>-12</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A70" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B70" s="36">
         <f>-40*B39*B40</f>
         <v>-12.8</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A71" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B71" s="22">
         <v>-42</v>
       </c>
       <c r="C71" s="87" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A72" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B72" s="36">
         <f>(B67+B68+B69+B70+B71)/(1+B5)^2.5</f>
         <v>-85.86499898982558</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -2314,17 +2314,17 @@
     </row>
     <row r="74" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A74" s="11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B74" s="37">
         <f>B54+B64</f>
-        <v>390.72783389425848</v>
+        <v>409.76278175038232</v>
       </c>
       <c r="C74" s="30"/>
     </row>
     <row r="75" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A75" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B75" s="37">
         <f>B72</f>
@@ -2334,14 +2334,14 @@
     </row>
     <row r="76" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A76" s="11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B76" s="37">
         <f>B74+B75</f>
-        <v>304.86283490443293</v>
+        <v>323.89778276055677</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -2351,32 +2351,32 @@
     </row>
     <row r="78" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A78" s="28" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B78" s="38"/>
       <c r="C78" s="30"/>
     </row>
     <row r="79" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A79" s="83" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B79" s="36">
         <f>MAX(0,B76)*0.25</f>
-        <v>76.215708726108232</v>
+        <v>80.974445690139191</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A80" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B80" s="22">
         <v>50</v>
       </c>
       <c r="C80" s="87" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -2386,25 +2386,25 @@
     </row>
     <row r="82" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A82" s="28" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B82" s="38"/>
       <c r="C82" s="30"/>
     </row>
     <row r="83" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A83" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B83" s="22">
         <v>205.7</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A84" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B84" s="22">
         <v>-5</v>
@@ -2413,14 +2413,14 @@
     </row>
     <row r="85" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A85" s="33" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B85" s="39">
         <f>B83+B84</f>
         <v>200.7</v>
       </c>
       <c r="C85" s="40" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -2430,14 +2430,14 @@
     </row>
     <row r="87" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A87" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B87" s="41">
         <f>B76+B79+B80+B85</f>
-        <v>631.77854363054121</v>
+        <v>655.572228450696</v>
       </c>
       <c r="C87" s="42" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -2447,14 +2447,14 @@
     </row>
     <row r="89" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A89" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B89" s="43"/>
       <c r="C89" s="27"/>
     </row>
     <row r="90" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A90" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B90" s="44">
         <f>'Diluted Shares'!B24</f>
@@ -2464,11 +2464,11 @@
     </row>
     <row r="91" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A91" s="45" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B91" s="46">
         <f>B87*1000000/B90</f>
-        <v>2.6827919672482281</v>
+        <v>2.7838297551729738</v>
       </c>
       <c r="C91" s="30"/>
     </row>
@@ -2479,7 +2479,7 @@
     </row>
     <row r="93" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A93" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B93" s="47">
         <v>1.74</v>
@@ -2488,11 +2488,11 @@
     </row>
     <row r="94" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A94" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B94" s="25">
         <f>(B91-B93)/B93</f>
-        <v>0.54183446393576329</v>
+        <v>0.59990215814538728</v>
       </c>
       <c r="C94" s="30"/>
     </row>
@@ -2503,13 +2503,13 @@
     </row>
     <row r="96" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A96" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B96" s="10">
         <v>12</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -2519,54 +2519,54 @@
     </row>
     <row r="98" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A98" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B98" s="48"/>
       <c r="C98" s="48"/>
     </row>
     <row r="99" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A99" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B99" s="49">
         <f>B85*1000000/B90</f>
         <v>0.8522548814851687</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A100" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B100" s="49">
         <f>B76*1000000/B90</f>
-        <v>1.2945731899885902</v>
+        <v>1.3754034203283867</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A101" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B101" s="49">
         <f>(B79+B80)*1000000/B90</f>
-        <v>0.53596389577446912</v>
+        <v>0.5561714533594182</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A102" s="50" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B102" s="51">
         <f>B91</f>
-        <v>2.6827919672482281</v>
+        <v>2.7838297551729738</v>
       </c>
       <c r="C102" s="1"/>
     </row>
@@ -2585,7 +2585,7 @@
   <dimension ref="A1:K49"/>
   <sheetViews>
     <sheetView topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2596,7 +2596,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="52" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B1" s="53"/>
       <c r="C1" s="53"/>
@@ -2622,7 +2622,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="54" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B3" s="55"/>
       <c r="C3" s="55"/>
@@ -2636,14 +2636,14 @@
     </row>
     <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="56" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B4" s="77">
         <f>'rNPV Model'!B5</f>
         <v>0.13</v>
       </c>
       <c r="C4" s="80" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D4" s="77">
         <f>'rNPV Model'!B14</f>
@@ -2658,14 +2658,14 @@
     </row>
     <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="57" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B5" s="77">
         <f>'rNPV Model'!B25</f>
         <v>0.28350000000000003</v>
       </c>
       <c r="C5" s="59" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D5" s="77">
         <f>'rNPV Model'!B43</f>
@@ -2680,14 +2680,14 @@
     </row>
     <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="57" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B6" s="84">
         <f>'rNPV Model'!B90</f>
         <v>235492931</v>
       </c>
       <c r="C6" s="59" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D6" s="85">
         <f>'rNPV Model'!B85</f>
@@ -2702,14 +2702,14 @@
     </row>
     <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="80" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B7" s="85">
         <f>'rNPV Model'!B80</f>
         <v>50</v>
       </c>
       <c r="C7" s="79" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D7" s="76">
         <f>0.25</f>
@@ -2724,14 +2724,14 @@
     </row>
     <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="78" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B8" s="61">
         <f>'rNPV Model'!B91</f>
-        <v>2.6827919672482281</v>
+        <v>2.7838297551729738</v>
       </c>
       <c r="C8" s="59" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D8" s="86">
         <f>'rNPV Model'!B93</f>
@@ -2758,7 +2758,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="54" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B10" s="55"/>
       <c r="C10" s="55"/>
@@ -2772,7 +2772,7 @@
     </row>
     <row r="11" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="62" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B11" s="63">
         <v>0.02</v>
@@ -2800,23 +2800,23 @@
       </c>
       <c r="B12" s="64">
         <f>(((((('rNPV Model'!B13*B$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A12)^(-'rNPV Model'!B47))/$A12))/(1+$A12)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A12)^(-'rNPV Model'!B57))/$A12))/(1+$A12)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A12)^2.5))+MAX(0,((((('rNPV Model'!B13*B$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A12)^(-'rNPV Model'!B47))/$A12))/(1+$A12)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A12)^(-'rNPV Model'!B57))/$A12))/(1+$A12)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A12)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>2.6291253861478365</v>
+        <v>2.750474722986187</v>
       </c>
       <c r="C12" s="64">
         <f>(((((('rNPV Model'!B13*C$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A12)^(-'rNPV Model'!B47))/$A12))/(1+$A12)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A12)^(-'rNPV Model'!B57))/$A12))/(1+$A12)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A12)^2.5))+MAX(0,((((('rNPV Model'!B13*C$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A12)^(-'rNPV Model'!B47))/$A12))/(1+$A12)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A12)^(-'rNPV Model'!B57))/$A12))/(1+$A12)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A12)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>2.8500165084123674</v>
+        <v>2.971365845250717</v>
       </c>
       <c r="D12" s="64">
         <f>(((((('rNPV Model'!B13*D$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A12)^(-'rNPV Model'!B47))/$A12))/(1+$A12)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A12)^(-'rNPV Model'!B57))/$A12))/(1+$A12)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A12)^2.5))+MAX(0,((((('rNPV Model'!B13*D$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A12)^(-'rNPV Model'!B47))/$A12))/(1+$A12)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A12)^(-'rNPV Model'!B57))/$A12))/(1+$A12)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A12)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>3.0709076306768974</v>
+        <v>3.1922569675152475</v>
       </c>
       <c r="E12" s="64">
         <f>(((((('rNPV Model'!B13*E$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A12)^(-'rNPV Model'!B47))/$A12))/(1+$A12)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A12)^(-'rNPV Model'!B57))/$A12))/(1+$A12)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A12)^2.5))+MAX(0,((((('rNPV Model'!B13*E$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A12)^(-'rNPV Model'!B47))/$A12))/(1+$A12)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A12)^(-'rNPV Model'!B57))/$A12))/(1+$A12)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A12)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>3.2917987529414283</v>
+        <v>3.4131480897797775</v>
       </c>
       <c r="F12" s="64">
         <f>(((((('rNPV Model'!B13*F$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A12)^(-'rNPV Model'!B47))/$A12))/(1+$A12)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A12)^(-'rNPV Model'!B57))/$A12))/(1+$A12)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A12)^2.5))+MAX(0,((((('rNPV Model'!B13*F$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A12)^(-'rNPV Model'!B47))/$A12))/(1+$A12)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A12)^(-'rNPV Model'!B57))/$A12))/(1+$A12)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A12)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>3.5126898752059583</v>
+        <v>3.6340392120443075</v>
       </c>
       <c r="G12" s="53"/>
       <c r="H12" s="53"/>
@@ -2829,23 +2829,23 @@
       </c>
       <c r="B13" s="65">
         <f>(((((('rNPV Model'!B13*B$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A13)^(-'rNPV Model'!B47))/$A13))/(1+$A13)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A13)^(-'rNPV Model'!B57))/$A13))/(1+$A13)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A13)^2.5))+MAX(0,((((('rNPV Model'!B13*B$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A13)^(-'rNPV Model'!B47))/$A13))/(1+$A13)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A13)^(-'rNPV Model'!B57))/$A13))/(1+$A13)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A13)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>2.4610282336002887</v>
+        <v>2.571683851839849</v>
       </c>
       <c r="C13" s="65">
         <f>(((((('rNPV Model'!B13*C$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A13)^(-'rNPV Model'!B47))/$A13))/(1+$A13)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A13)^(-'rNPV Model'!B57))/$A13))/(1+$A13)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A13)^2.5))+MAX(0,((((('rNPV Model'!B13*C$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A13)^(-'rNPV Model'!B47))/$A13))/(1+$A13)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A13)^(-'rNPV Model'!B57))/$A13))/(1+$A13)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A13)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>2.6636611378695991</v>
+        <v>2.7743167561091591</v>
       </c>
       <c r="D13" s="65">
         <f>(((((('rNPV Model'!B13*D$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A13)^(-'rNPV Model'!B47))/$A13))/(1+$A13)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A13)^(-'rNPV Model'!B57))/$A13))/(1+$A13)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A13)^2.5))+MAX(0,((((('rNPV Model'!B13*D$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A13)^(-'rNPV Model'!B47))/$A13))/(1+$A13)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A13)^(-'rNPV Model'!B57))/$A13))/(1+$A13)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A13)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>2.8662940421389091</v>
+        <v>2.9769496603784695</v>
       </c>
       <c r="E13" s="65">
         <f>(((((('rNPV Model'!B13*E$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A13)^(-'rNPV Model'!B47))/$A13))/(1+$A13)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A13)^(-'rNPV Model'!B57))/$A13))/(1+$A13)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A13)^2.5))+MAX(0,((((('rNPV Model'!B13*E$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A13)^(-'rNPV Model'!B47))/$A13))/(1+$A13)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A13)^(-'rNPV Model'!B57))/$A13))/(1+$A13)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A13)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>3.0689269464082196</v>
+        <v>3.1795825646477796</v>
       </c>
       <c r="F13" s="64">
         <f>(((((('rNPV Model'!B13*F$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A13)^(-'rNPV Model'!B47))/$A13))/(1+$A13)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A13)^(-'rNPV Model'!B57))/$A13))/(1+$A13)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A13)^2.5))+MAX(0,((((('rNPV Model'!B13*F$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A13)^(-'rNPV Model'!B47))/$A13))/(1+$A13)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A13)^(-'rNPV Model'!B57))/$A13))/(1+$A13)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A13)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>3.2715598506775296</v>
+        <v>3.38221546891709</v>
       </c>
       <c r="G13" s="53"/>
       <c r="H13" s="53"/>
@@ -2858,23 +2858,23 @@
       </c>
       <c r="B14" s="65">
         <f>(((((('rNPV Model'!B13*B$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A14)^(-'rNPV Model'!B47))/$A14))/(1+$A14)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A14)^(-'rNPV Model'!B57))/$A14))/(1+$A14)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A14)^2.5))+MAX(0,((((('rNPV Model'!B13*B$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A14)^(-'rNPV Model'!B47))/$A14))/(1+$A14)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A14)^(-'rNPV Model'!B57))/$A14))/(1+$A14)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A14)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>2.3105103888951724</v>
+        <v>2.4115481768199181</v>
       </c>
       <c r="C14" s="82">
         <f>(((((('rNPV Model'!B13*C$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A14)^(-'rNPV Model'!B47))/$A14))/(1+$A14)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A14)^(-'rNPV Model'!B57))/$A14))/(1+$A14)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A14)^2.5))+MAX(0,((((('rNPV Model'!B13*C$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A14)^(-'rNPV Model'!B47))/$A14))/(1+$A14)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A14)^(-'rNPV Model'!B57))/$A14))/(1+$A14)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A14)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>2.4966511780716996</v>
+        <v>2.5976889659964453</v>
       </c>
       <c r="D14" s="81">
         <f>(((((('rNPV Model'!B13*D$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A14)^(-'rNPV Model'!B47))/$A14))/(1+$A14)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A14)^(-'rNPV Model'!B57))/$A14))/(1+$A14)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A14)^2.5))+MAX(0,((((('rNPV Model'!B13*D$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A14)^(-'rNPV Model'!B47))/$A14))/(1+$A14)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A14)^(-'rNPV Model'!B57))/$A14))/(1+$A14)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A14)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>2.6827919672482281</v>
+        <v>2.7838297551729738</v>
       </c>
       <c r="E14" s="65">
         <f>(((((('rNPV Model'!B13*E$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A14)^(-'rNPV Model'!B47))/$A14))/(1+$A14)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A14)^(-'rNPV Model'!B57))/$A14))/(1+$A14)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A14)^2.5))+MAX(0,((((('rNPV Model'!B13*E$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A14)^(-'rNPV Model'!B47))/$A14))/(1+$A14)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A14)^(-'rNPV Model'!B57))/$A14))/(1+$A14)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A14)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>2.8689327564247553</v>
+        <v>2.969970544349501</v>
       </c>
       <c r="F14" s="66">
         <f>(((((('rNPV Model'!B13*F$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A14)^(-'rNPV Model'!B47))/$A14))/(1+$A14)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A14)^(-'rNPV Model'!B57))/$A14))/(1+$A14)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A14)^2.5))+MAX(0,((((('rNPV Model'!B13*F$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A14)^(-'rNPV Model'!B47))/$A14))/(1+$A14)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A14)^(-'rNPV Model'!B57))/$A14))/(1+$A14)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A14)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>3.055073545601283</v>
+        <v>3.1561113335260287</v>
       </c>
       <c r="G14" s="53"/>
       <c r="H14" s="53"/>
@@ -2887,23 +2887,23 @@
       </c>
       <c r="B15" s="65">
         <f>(((((('rNPV Model'!B13*B$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A15)^(-'rNPV Model'!B47))/$A15))/(1+$A15)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A15)^(-'rNPV Model'!B57))/$A15))/(1+$A15)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A15)^2.5))+MAX(0,((((('rNPV Model'!B13*B$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A15)^(-'rNPV Model'!B47))/$A15))/(1+$A15)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A15)^(-'rNPV Model'!B57))/$A15))/(1+$A15)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A15)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>2.1755790329531837</v>
+        <v>2.2679540818003092</v>
       </c>
       <c r="C15" s="65">
         <f>(((((('rNPV Model'!B13*C$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A15)^(-'rNPV Model'!B47))/$A15))/(1+$A15)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A15)^(-'rNPV Model'!B57))/$A15))/(1+$A15)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A15)^2.5))+MAX(0,((((('rNPV Model'!B13*C$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A15)^(-'rNPV Model'!B47))/$A15))/(1+$A15)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A15)^(-'rNPV Model'!B57))/$A15))/(1+$A15)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A15)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>2.3468001974635335</v>
+        <v>2.43917524631066</v>
       </c>
       <c r="D15" s="65">
         <f>(((((('rNPV Model'!B13*D$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A15)^(-'rNPV Model'!B47))/$A15))/(1+$A15)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A15)^(-'rNPV Model'!B57))/$A15))/(1+$A15)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A15)^2.5))+MAX(0,((((('rNPV Model'!B13*D$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A15)^(-'rNPV Model'!B47))/$A15))/(1+$A15)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A15)^(-'rNPV Model'!B57))/$A15))/(1+$A15)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A15)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>2.5180213619738825</v>
+        <v>2.6103964108210089</v>
       </c>
       <c r="E15" s="65">
         <f>(((((('rNPV Model'!B13*E$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A15)^(-'rNPV Model'!B47))/$A15))/(1+$A15)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A15)^(-'rNPV Model'!B57))/$A15))/(1+$A15)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A15)^2.5))+MAX(0,((((('rNPV Model'!B13*E$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A15)^(-'rNPV Model'!B47))/$A15))/(1+$A15)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A15)^(-'rNPV Model'!B57))/$A15))/(1+$A15)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A15)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>2.6892425264842323</v>
+        <v>2.7816175753313583</v>
       </c>
       <c r="F15" s="64">
         <f>(((((('rNPV Model'!B13*F$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A15)^(-'rNPV Model'!B47))/$A15))/(1+$A15)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A15)^(-'rNPV Model'!B57))/$A15))/(1+$A15)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A15)^2.5))+MAX(0,((((('rNPV Model'!B13*F$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A15)^(-'rNPV Model'!B47))/$A15))/(1+$A15)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A15)^(-'rNPV Model'!B57))/$A15))/(1+$A15)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A15)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>2.8604636909945822</v>
+        <v>2.9528387398417082</v>
       </c>
       <c r="G15" s="53"/>
       <c r="H15" s="53"/>
@@ -2936,7 +2936,7 @@
     </row>
     <row r="18" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="92" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B18" s="69"/>
       <c r="C18" s="70"/>
@@ -2951,28 +2951,28 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" s="72" t="s">
+        <v>155</v>
+      </c>
+      <c r="B19" s="72" t="s">
         <v>156</v>
       </c>
-      <c r="B19" s="72" t="s">
+      <c r="C19" s="72" t="s">
+        <v>147</v>
+      </c>
+      <c r="D19" s="89" t="s">
+        <v>148</v>
+      </c>
+      <c r="E19" s="89" t="s">
+        <v>175</v>
+      </c>
+      <c r="F19" s="72" t="s">
+        <v>145</v>
+      </c>
+      <c r="G19" s="72" t="s">
         <v>157</v>
       </c>
-      <c r="C19" s="72" t="s">
-        <v>148</v>
-      </c>
-      <c r="D19" s="89" t="s">
-        <v>149</v>
-      </c>
-      <c r="E19" s="89" t="s">
-        <v>176</v>
-      </c>
-      <c r="F19" s="72" t="s">
-        <v>146</v>
-      </c>
-      <c r="G19" s="72" t="s">
+      <c r="H19" s="72" t="s">
         <v>158</v>
-      </c>
-      <c r="H19" s="72" t="s">
-        <v>159</v>
       </c>
       <c r="I19" s="53"/>
       <c r="J19" s="53"/>
@@ -2980,7 +2980,7 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" s="56" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B20" s="76">
         <v>0.02</v>
@@ -3002,7 +3002,7 @@
         <v>0.65829781414252497</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
       <c r="I20" s="53"/>
       <c r="J20" s="53"/>
@@ -3010,7 +3010,7 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21" s="56" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B21" s="76">
         <f>'rNPV Model'!B14</f>
@@ -3033,7 +3033,7 @@
       </c>
       <c r="G21" s="74">
         <f>((('rNPV Model'!B13*B21*'rNPV Model'!B16*'rNPV Model'!B18*((1-(1+F21)^(-'rNPV Model'!B47))/F21)/(1+F21)^('rNPV Model'!B8-'rNPV Model'!B10)*C21)+('rNPV Model'!B60*((1-(1+F21)^(-'rNPV Model'!B57))/F21)/(1+F21)^('rNPV Model'!B9-'rNPV Model'!B10)*D21)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+F21)^2.5))+MAX(0,(('rNPV Model'!B13*B21*'rNPV Model'!B16*'rNPV Model'!B18*((1-(1+F21)^(-'rNPV Model'!B47))/F21)/(1+F21)^('rNPV Model'!B8-'rNPV Model'!B10)*C21)+('rNPV Model'!B60*((1-(1+F21)^(-'rNPV Model'!B57))/F21)/(1+F21)^('rNPV Model'!B9-'rNPV Model'!B10)*D21)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+F21)^2.5)))*$D$7+E21+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>2.6827919672482281</v>
+        <v>2.7838297551729738</v>
       </c>
       <c r="H21" s="1"/>
       <c r="I21" s="53"/>
@@ -3042,7 +3042,7 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22" s="56" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B22" s="76">
         <v>0.06</v>
@@ -3061,10 +3061,10 @@
       </c>
       <c r="G22" s="73">
         <f>((('rNPV Model'!B13*B22*'rNPV Model'!B16*'rNPV Model'!B18*((1-(1+F22)^(-'rNPV Model'!B47))/F22)/(1+F22)^('rNPV Model'!B8-'rNPV Model'!B10)*C22)+('rNPV Model'!B60*((1-(1+F22)^(-'rNPV Model'!B57))/F22)/(1+F22)^('rNPV Model'!B9-'rNPV Model'!B10)*D22)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+F22)^2.5))+MAX(0,(('rNPV Model'!B13*B22*'rNPV Model'!B16*'rNPV Model'!B18*((1-(1+F22)^(-'rNPV Model'!B47))/F22)/(1+F22)^('rNPV Model'!B8-'rNPV Model'!B10)*C22)+('rNPV Model'!B60*((1-(1+F22)^(-'rNPV Model'!B57))/F22)/(1+F22)^('rNPV Model'!B9-'rNPV Model'!B10)*D22)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+F22)^2.5)))*$D$7+E22+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>3.2397396198342441</v>
+        <v>3.3660368547401749</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="I22" s="53"/>
       <c r="J22" s="53"/>
@@ -3072,7 +3072,7 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23" s="56" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B23" s="76">
         <v>7.0000000000000007E-2</v>
@@ -3091,10 +3091,10 @@
       </c>
       <c r="G23" s="73">
         <f>((('rNPV Model'!B13*B23*'rNPV Model'!B16*'rNPV Model'!B18*((1-(1+F23)^(-'rNPV Model'!B47))/F23)/(1+F23)^('rNPV Model'!B8-'rNPV Model'!B10)*C23)+('rNPV Model'!B60*((1-(1+F23)^(-'rNPV Model'!B57))/F23)/(1+F23)^('rNPV Model'!B9-'rNPV Model'!B10)*D23)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+F23)^2.5))+MAX(0,(('rNPV Model'!B13*B23*'rNPV Model'!B16*'rNPV Model'!B18*((1-(1+F23)^(-'rNPV Model'!B47))/F23)/(1+F23)^('rNPV Model'!B8-'rNPV Model'!B10)*C23)+('rNPV Model'!B60*((1-(1+F23)^(-'rNPV Model'!B57))/F23)/(1+F23)^('rNPV Model'!B9-'rNPV Model'!B10)*D23)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+F23)^2.5)))*$D$7+E23+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>4.7902866252845833</v>
+        <v>4.9780506833833842</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="I23" s="53"/>
       <c r="J23" s="53"/>
@@ -3102,7 +3102,7 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24" s="56" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B24" s="76">
         <v>0.1</v>
@@ -3121,10 +3121,10 @@
       </c>
       <c r="G24" s="73">
         <f>((('rNPV Model'!B13*B24*'rNPV Model'!B16*'rNPV Model'!B18*((1-(1+F24)^(-'rNPV Model'!B47))/F24)/(1+F24)^('rNPV Model'!B8-'rNPV Model'!B10)*C24)+('rNPV Model'!B60*((1-(1+F24)^(-'rNPV Model'!B57))/F24)/(1+F24)^('rNPV Model'!B9-'rNPV Model'!B10)*D24)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+F24)^2.5))+MAX(0,(('rNPV Model'!B13*B24*'rNPV Model'!B16*'rNPV Model'!B18*((1-(1+F24)^(-'rNPV Model'!B47))/F24)/(1+F24)^('rNPV Model'!B8-'rNPV Model'!B10)*C24)+('rNPV Model'!B60*((1-(1+F24)^(-'rNPV Model'!B57))/F24)/(1+F24)^('rNPV Model'!B9-'rNPV Model'!B10)*D24)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+F24)^2.5)))*$D$7+E24+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>6.4341718081255479</v>
+        <v>6.6602865022270858</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I24" s="53"/>
       <c r="J24" s="53"/>
@@ -3144,7 +3144,7 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26" s="75" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B26" s="53"/>
       <c r="C26" s="53"/>
@@ -3158,7 +3158,7 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B27" s="53"/>
       <c r="C27" s="53"/>
@@ -3172,7 +3172,7 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B28" s="53"/>
       <c r="C28" s="53"/>
@@ -3186,7 +3186,7 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B29" s="53"/>
       <c r="C29" s="53"/>
@@ -3200,7 +3200,7 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A30" s="87" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B30" s="53"/>
       <c r="C30" s="53"/>
@@ -3214,7 +3214,7 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B31" s="53"/>
       <c r="C31" s="53"/>

</xml_diff>

<commit_message>
Update future dilution estimate
</commit_message>
<xml_diff>
--- a/PALI_rNPV_Model.xlsx
+++ b/PALI_rNPV_Model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dan\OneDrive\Documents\Equity Research\PALI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C465893-DE6D-48FB-93E4-013002615616}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81F05C13-4150-4A98-84C1-BCA08344F536}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -566,9 +566,6 @@
     <t>~$6M/yr 2026-2027 (Phase 2) + ~10M/yr 2028-2030 (Phase 3 &amp; NDA)</t>
   </si>
   <si>
-    <t>Assumption: ~$60M raise at ~$6.50/share Phase 3 funding event (2028)</t>
-  </si>
-  <si>
     <t>oral PDE4 in crowded biologics market</t>
   </si>
   <si>
@@ -612,6 +609,9 @@
   </si>
   <si>
     <t>Zero fibrosis signals, FSCD discontinued, and UC becomes a commercial flop (immediate cash value is still $0.85)</t>
+  </si>
+  <si>
+    <t>Assumption: ~$60M raise at ~$6.00/share Phase 3 funding event (2028)</t>
   </si>
 </sst>
 </file>
@@ -1422,16 +1422,16 @@
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B8" s="9">
         <v>57270786</v>
       </c>
       <c r="C8" s="10">
-        <v>0.7</v>
+        <v>1E-4</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -1450,7 +1450,7 @@
     </row>
     <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B10" s="9">
         <v>6850356</v>
@@ -1459,12 +1459,12 @@
         <v>1.155</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B11" s="9">
         <v>0</v>
@@ -1561,13 +1561,13 @@
         <v>22</v>
       </c>
       <c r="B21" s="4">
-        <v>9230769</v>
+        <v>10000000</v>
       </c>
       <c r="C21" s="10">
-        <v>6.5</v>
+        <v>6</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>179</v>
+        <v>194</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -1576,7 +1576,7 @@
       </c>
       <c r="B22" s="12">
         <f>B21</f>
-        <v>9230769</v>
+        <v>10000000</v>
       </c>
       <c r="C22" s="13"/>
       <c r="D22" s="13"/>
@@ -1587,7 +1587,7 @@
       </c>
       <c r="B24" s="17">
         <f>B5+B12+B18+B22</f>
-        <v>235492931</v>
+        <v>236262162</v>
       </c>
       <c r="C24" s="18"/>
       <c r="D24" s="19" t="s">
@@ -1608,8 +1608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C102"/>
   <sheetViews>
-    <sheetView topLeftCell="A69" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView topLeftCell="A72" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1659,7 +1659,7 @@
         <v>0</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -1732,7 +1732,7 @@
         <v>0.06</v>
       </c>
       <c r="C14" s="21" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -1859,7 +1859,7 @@
         <v>320000</v>
       </c>
       <c r="C28" s="21" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -1881,7 +1881,7 @@
         <v>0.16</v>
       </c>
       <c r="C30" s="21" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -2258,7 +2258,7 @@
         <v>-24.75</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -2281,7 +2281,7 @@
         <v>-12.8</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -2399,7 +2399,7 @@
         <v>205.7</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -2458,7 +2458,7 @@
       </c>
       <c r="B90" s="44">
         <f>'Diluted Shares'!B24</f>
-        <v>235492931</v>
+        <v>236262162</v>
       </c>
       <c r="C90" s="30"/>
     </row>
@@ -2468,7 +2468,7 @@
       </c>
       <c r="B91" s="46">
         <f>B87*1000000/B90</f>
-        <v>2.7838297551729738</v>
+        <v>2.7747660602999815</v>
       </c>
       <c r="C91" s="30"/>
     </row>
@@ -2492,7 +2492,7 @@
       </c>
       <c r="B94" s="25">
         <f>(B91-B93)/B93</f>
-        <v>0.59990215814538728</v>
+        <v>0.59469313810343771</v>
       </c>
       <c r="C94" s="30"/>
     </row>
@@ -2530,7 +2530,7 @@
       </c>
       <c r="B99" s="49">
         <f>B85*1000000/B90</f>
-        <v>0.8522548814851687</v>
+        <v>0.8494800788287038</v>
       </c>
       <c r="C99" s="1" t="s">
         <v>137</v>
@@ -2542,7 +2542,7 @@
       </c>
       <c r="B100" s="49">
         <f>B76*1000000/B90</f>
-        <v>1.3754034203283867</v>
+        <v>1.3709253314991536</v>
       </c>
       <c r="C100" s="1" t="s">
         <v>139</v>
@@ -2554,7 +2554,7 @@
       </c>
       <c r="B101" s="49">
         <f>(B79+B80)*1000000/B90</f>
-        <v>0.5561714533594182</v>
+        <v>0.55436064997212375</v>
       </c>
       <c r="C101" s="1" t="s">
         <v>141</v>
@@ -2566,7 +2566,7 @@
       </c>
       <c r="B102" s="51">
         <f>B91</f>
-        <v>2.7838297551729738</v>
+        <v>2.7747660602999815</v>
       </c>
       <c r="C102" s="1"/>
     </row>
@@ -2584,7 +2584,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
@@ -2684,7 +2684,7 @@
       </c>
       <c r="B6" s="84">
         <f>'rNPV Model'!B90</f>
-        <v>235492931</v>
+        <v>236262162</v>
       </c>
       <c r="C6" s="59" t="s">
         <v>149</v>
@@ -2728,7 +2728,7 @@
       </c>
       <c r="B8" s="61">
         <f>'rNPV Model'!B91</f>
-        <v>2.7838297551729738</v>
+        <v>2.7747660602999815</v>
       </c>
       <c r="C8" s="59" t="s">
         <v>151</v>
@@ -2800,23 +2800,23 @@
       </c>
       <c r="B12" s="64">
         <f>(((((('rNPV Model'!B13*B$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A12)^(-'rNPV Model'!B47))/$A12))/(1+$A12)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A12)^(-'rNPV Model'!B57))/$A12))/(1+$A12)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A12)^2.5))+MAX(0,((((('rNPV Model'!B13*B$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A12)^(-'rNPV Model'!B47))/$A12))/(1+$A12)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A12)^(-'rNPV Model'!B57))/$A12))/(1+$A12)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A12)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>2.750474722986187</v>
+        <v>2.7415196266485968</v>
       </c>
       <c r="C12" s="64">
         <f>(((((('rNPV Model'!B13*C$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A12)^(-'rNPV Model'!B47))/$A12))/(1+$A12)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A12)^(-'rNPV Model'!B57))/$A12))/(1+$A12)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A12)^2.5))+MAX(0,((((('rNPV Model'!B13*C$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A12)^(-'rNPV Model'!B47))/$A12))/(1+$A12)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A12)^(-'rNPV Model'!B57))/$A12))/(1+$A12)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A12)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>2.971365845250717</v>
+        <v>2.9616915635072525</v>
       </c>
       <c r="D12" s="64">
         <f>(((((('rNPV Model'!B13*D$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A12)^(-'rNPV Model'!B47))/$A12))/(1+$A12)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A12)^(-'rNPV Model'!B57))/$A12))/(1+$A12)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A12)^2.5))+MAX(0,((((('rNPV Model'!B13*D$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A12)^(-'rNPV Model'!B47))/$A12))/(1+$A12)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A12)^(-'rNPV Model'!B57))/$A12))/(1+$A12)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A12)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>3.1922569675152475</v>
+        <v>3.181863500365909</v>
       </c>
       <c r="E12" s="64">
         <f>(((((('rNPV Model'!B13*E$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A12)^(-'rNPV Model'!B47))/$A12))/(1+$A12)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A12)^(-'rNPV Model'!B57))/$A12))/(1+$A12)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A12)^2.5))+MAX(0,((((('rNPV Model'!B13*E$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A12)^(-'rNPV Model'!B47))/$A12))/(1+$A12)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A12)^(-'rNPV Model'!B57))/$A12))/(1+$A12)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A12)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>3.4131480897797775</v>
+        <v>3.4020354372245647</v>
       </c>
       <c r="F12" s="64">
         <f>(((((('rNPV Model'!B13*F$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A12)^(-'rNPV Model'!B47))/$A12))/(1+$A12)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A12)^(-'rNPV Model'!B57))/$A12))/(1+$A12)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A12)^2.5))+MAX(0,((((('rNPV Model'!B13*F$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A12)^(-'rNPV Model'!B47))/$A12))/(1+$A12)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A12)^(-'rNPV Model'!B57))/$A12))/(1+$A12)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A12)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>3.6340392120443075</v>
+        <v>3.6222073740832208</v>
       </c>
       <c r="G12" s="53"/>
       <c r="H12" s="53"/>
@@ -2829,23 +2829,23 @@
       </c>
       <c r="B13" s="65">
         <f>(((((('rNPV Model'!B13*B$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A13)^(-'rNPV Model'!B47))/$A13))/(1+$A13)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A13)^(-'rNPV Model'!B57))/$A13))/(1+$A13)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A13)^2.5))+MAX(0,((((('rNPV Model'!B13*B$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A13)^(-'rNPV Model'!B47))/$A13))/(1+$A13)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A13)^(-'rNPV Model'!B57))/$A13))/(1+$A13)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A13)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>2.571683851839849</v>
+        <v>2.5633108693686455</v>
       </c>
       <c r="C13" s="65">
         <f>(((((('rNPV Model'!B13*C$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A13)^(-'rNPV Model'!B47))/$A13))/(1+$A13)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A13)^(-'rNPV Model'!B57))/$A13))/(1+$A13)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A13)^2.5))+MAX(0,((((('rNPV Model'!B13*C$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A13)^(-'rNPV Model'!B47))/$A13))/(1+$A13)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A13)^(-'rNPV Model'!B57))/$A13))/(1+$A13)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A13)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>2.7743167561091591</v>
+        <v>2.7652840340069265</v>
       </c>
       <c r="D13" s="65">
         <f>(((((('rNPV Model'!B13*D$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A13)^(-'rNPV Model'!B47))/$A13))/(1+$A13)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A13)^(-'rNPV Model'!B57))/$A13))/(1+$A13)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A13)^2.5))+MAX(0,((((('rNPV Model'!B13*D$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A13)^(-'rNPV Model'!B47))/$A13))/(1+$A13)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A13)^(-'rNPV Model'!B57))/$A13))/(1+$A13)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A13)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>2.9769496603784695</v>
+        <v>2.9672571986452083</v>
       </c>
       <c r="E13" s="65">
         <f>(((((('rNPV Model'!B13*E$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A13)^(-'rNPV Model'!B47))/$A13))/(1+$A13)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A13)^(-'rNPV Model'!B57))/$A13))/(1+$A13)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A13)^2.5))+MAX(0,((((('rNPV Model'!B13*E$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A13)^(-'rNPV Model'!B47))/$A13))/(1+$A13)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A13)^(-'rNPV Model'!B57))/$A13))/(1+$A13)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A13)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>3.1795825646477796</v>
+        <v>3.1692303632834893</v>
       </c>
       <c r="F13" s="64">
         <f>(((((('rNPV Model'!B13*F$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A13)^(-'rNPV Model'!B47))/$A13))/(1+$A13)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A13)^(-'rNPV Model'!B57))/$A13))/(1+$A13)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A13)^2.5))+MAX(0,((((('rNPV Model'!B13*F$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A13)^(-'rNPV Model'!B47))/$A13))/(1+$A13)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A13)^(-'rNPV Model'!B57))/$A13))/(1+$A13)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A13)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>3.38221546891709</v>
+        <v>3.3712035279217707</v>
       </c>
       <c r="G13" s="53"/>
       <c r="H13" s="53"/>
@@ -2858,23 +2858,23 @@
       </c>
       <c r="B14" s="65">
         <f>(((((('rNPV Model'!B13*B$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A14)^(-'rNPV Model'!B47))/$A14))/(1+$A14)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A14)^(-'rNPV Model'!B57))/$A14))/(1+$A14)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A14)^2.5))+MAX(0,((((('rNPV Model'!B13*B$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A14)^(-'rNPV Model'!B47))/$A14))/(1+$A14)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A14)^(-'rNPV Model'!B57))/$A14))/(1+$A14)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A14)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>2.4115481768199181</v>
+        <v>2.403696569944318</v>
       </c>
       <c r="C14" s="82">
         <f>(((((('rNPV Model'!B13*C$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A14)^(-'rNPV Model'!B47))/$A14))/(1+$A14)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A14)^(-'rNPV Model'!B57))/$A14))/(1+$A14)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A14)^2.5))+MAX(0,((((('rNPV Model'!B13*C$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A14)^(-'rNPV Model'!B47))/$A14))/(1+$A14)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A14)^(-'rNPV Model'!B57))/$A14))/(1+$A14)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A14)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>2.5976889659964453</v>
+        <v>2.5892313151221491</v>
       </c>
       <c r="D14" s="81">
         <f>(((((('rNPV Model'!B13*D$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A14)^(-'rNPV Model'!B47))/$A14))/(1+$A14)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A14)^(-'rNPV Model'!B57))/$A14))/(1+$A14)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A14)^2.5))+MAX(0,((((('rNPV Model'!B13*D$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A14)^(-'rNPV Model'!B47))/$A14))/(1+$A14)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A14)^(-'rNPV Model'!B57))/$A14))/(1+$A14)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A14)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>2.7838297551729738</v>
+        <v>2.7747660602999815</v>
       </c>
       <c r="E14" s="65">
         <f>(((((('rNPV Model'!B13*E$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A14)^(-'rNPV Model'!B47))/$A14))/(1+$A14)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A14)^(-'rNPV Model'!B57))/$A14))/(1+$A14)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A14)^2.5))+MAX(0,((((('rNPV Model'!B13*E$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A14)^(-'rNPV Model'!B47))/$A14))/(1+$A14)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A14)^(-'rNPV Model'!B57))/$A14))/(1+$A14)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A14)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>2.969970544349501</v>
+        <v>2.960300805477813</v>
       </c>
       <c r="F14" s="66">
         <f>(((((('rNPV Model'!B13*F$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A14)^(-'rNPV Model'!B47))/$A14))/(1+$A14)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A14)^(-'rNPV Model'!B57))/$A14))/(1+$A14)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A14)^2.5))+MAX(0,((((('rNPV Model'!B13*F$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A14)^(-'rNPV Model'!B47))/$A14))/(1+$A14)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A14)^(-'rNPV Model'!B57))/$A14))/(1+$A14)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A14)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>3.1561113335260287</v>
+        <v>3.1458355506556446</v>
       </c>
       <c r="G14" s="53"/>
       <c r="H14" s="53"/>
@@ -2887,23 +2887,23 @@
       </c>
       <c r="B15" s="65">
         <f>(((((('rNPV Model'!B13*B$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A15)^(-'rNPV Model'!B47))/$A15))/(1+$A15)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A15)^(-'rNPV Model'!B57))/$A15))/(1+$A15)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A15)^2.5))+MAX(0,((((('rNPV Model'!B13*B$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A15)^(-'rNPV Model'!B47))/$A15))/(1+$A15)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A15)^(-'rNPV Model'!B57))/$A15))/(1+$A15)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A15)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>2.2679540818003092</v>
+        <v>2.2605699938383217</v>
       </c>
       <c r="C15" s="65">
         <f>(((((('rNPV Model'!B13*C$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A15)^(-'rNPV Model'!B47))/$A15))/(1+$A15)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A15)^(-'rNPV Model'!B57))/$A15))/(1+$A15)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A15)^2.5))+MAX(0,((((('rNPV Model'!B13*C$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A15)^(-'rNPV Model'!B47))/$A15))/(1+$A15)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A15)^(-'rNPV Model'!B57))/$A15))/(1+$A15)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A15)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>2.43917524631066</v>
+        <v>2.4312336902103868</v>
       </c>
       <c r="D15" s="65">
         <f>(((((('rNPV Model'!B13*D$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A15)^(-'rNPV Model'!B47))/$A15))/(1+$A15)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A15)^(-'rNPV Model'!B57))/$A15))/(1+$A15)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A15)^2.5))+MAX(0,((((('rNPV Model'!B13*D$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A15)^(-'rNPV Model'!B47))/$A15))/(1+$A15)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A15)^(-'rNPV Model'!B57))/$A15))/(1+$A15)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A15)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>2.6103964108210089</v>
+        <v>2.6018973865824502</v>
       </c>
       <c r="E15" s="65">
         <f>(((((('rNPV Model'!B13*E$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A15)^(-'rNPV Model'!B47))/$A15))/(1+$A15)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A15)^(-'rNPV Model'!B57))/$A15))/(1+$A15)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A15)^2.5))+MAX(0,((((('rNPV Model'!B13*E$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A15)^(-'rNPV Model'!B47))/$A15))/(1+$A15)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A15)^(-'rNPV Model'!B57))/$A15))/(1+$A15)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A15)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>2.7816175753313583</v>
+        <v>2.7725610829545144</v>
       </c>
       <c r="F15" s="64">
         <f>(((((('rNPV Model'!B13*F$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A15)^(-'rNPV Model'!B47))/$A15))/(1+$A15)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A15)^(-'rNPV Model'!B57))/$A15))/(1+$A15)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A15)^2.5))+MAX(0,((((('rNPV Model'!B13*F$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A15)^(-'rNPV Model'!B47))/$A15))/(1+$A15)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A15)^(-'rNPV Model'!B57))/$A15))/(1+$A15)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A15)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>2.9528387398417082</v>
+        <v>2.9432247793265782</v>
       </c>
       <c r="G15" s="53"/>
       <c r="H15" s="53"/>
@@ -2999,10 +2999,10 @@
       </c>
       <c r="G20" s="73">
         <f>((('rNPV Model'!B13*B20*'rNPV Model'!B16*'rNPV Model'!B18*((1-(1+F20)^(-'rNPV Model'!B47))/F20)/(1+F20)^('rNPV Model'!B8-'rNPV Model'!B10)*C20)+('rNPV Model'!B60*((1-(1+F20)^(-'rNPV Model'!B57))/F20)/(1+F20)^('rNPV Model'!B9-'rNPV Model'!B10)*D20)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+F20)^2.5))+MAX(0,(('rNPV Model'!B13*B20*'rNPV Model'!B16*'rNPV Model'!B18*((1-(1+F20)^(-'rNPV Model'!B47))/F20)/(1+F20)^('rNPV Model'!B8-'rNPV Model'!B10)*C20)+('rNPV Model'!B60*((1-(1+F20)^(-'rNPV Model'!B57))/F20)/(1+F20)^('rNPV Model'!B9-'rNPV Model'!B10)*D20)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+F20)^2.5)))*$D$7+E20+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>0.65829781414252497</v>
+        <v>0.65615450400947595</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I20" s="53"/>
       <c r="J20" s="53"/>
@@ -3033,7 +3033,7 @@
       </c>
       <c r="G21" s="74">
         <f>((('rNPV Model'!B13*B21*'rNPV Model'!B16*'rNPV Model'!B18*((1-(1+F21)^(-'rNPV Model'!B47))/F21)/(1+F21)^('rNPV Model'!B8-'rNPV Model'!B10)*C21)+('rNPV Model'!B60*((1-(1+F21)^(-'rNPV Model'!B57))/F21)/(1+F21)^('rNPV Model'!B9-'rNPV Model'!B10)*D21)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+F21)^2.5))+MAX(0,(('rNPV Model'!B13*B21*'rNPV Model'!B16*'rNPV Model'!B18*((1-(1+F21)^(-'rNPV Model'!B47))/F21)/(1+F21)^('rNPV Model'!B8-'rNPV Model'!B10)*C21)+('rNPV Model'!B60*((1-(1+F21)^(-'rNPV Model'!B57))/F21)/(1+F21)^('rNPV Model'!B9-'rNPV Model'!B10)*D21)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+F21)^2.5)))*$D$7+E21+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>2.7838297551729738</v>
+        <v>2.7747660602999815</v>
       </c>
       <c r="H21" s="1"/>
       <c r="I21" s="53"/>
@@ -3061,10 +3061,10 @@
       </c>
       <c r="G22" s="73">
         <f>((('rNPV Model'!B13*B22*'rNPV Model'!B16*'rNPV Model'!B18*((1-(1+F22)^(-'rNPV Model'!B47))/F22)/(1+F22)^('rNPV Model'!B8-'rNPV Model'!B10)*C22)+('rNPV Model'!B60*((1-(1+F22)^(-'rNPV Model'!B57))/F22)/(1+F22)^('rNPV Model'!B9-'rNPV Model'!B10)*D22)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+F22)^2.5))+MAX(0,(('rNPV Model'!B13*B22*'rNPV Model'!B16*'rNPV Model'!B18*((1-(1+F22)^(-'rNPV Model'!B47))/F22)/(1+F22)^('rNPV Model'!B8-'rNPV Model'!B10)*C22)+('rNPV Model'!B60*((1-(1+F22)^(-'rNPV Model'!B57))/F22)/(1+F22)^('rNPV Model'!B9-'rNPV Model'!B10)*D22)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+F22)^2.5)))*$D$7+E22+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>3.3660368547401749</v>
+        <v>3.3550775886694248</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I22" s="53"/>
       <c r="J22" s="53"/>
@@ -3091,10 +3091,10 @@
       </c>
       <c r="G23" s="73">
         <f>((('rNPV Model'!B13*B23*'rNPV Model'!B16*'rNPV Model'!B18*((1-(1+F23)^(-'rNPV Model'!B47))/F23)/(1+F23)^('rNPV Model'!B8-'rNPV Model'!B10)*C23)+('rNPV Model'!B60*((1-(1+F23)^(-'rNPV Model'!B57))/F23)/(1+F23)^('rNPV Model'!B9-'rNPV Model'!B10)*D23)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+F23)^2.5))+MAX(0,(('rNPV Model'!B13*B23*'rNPV Model'!B16*'rNPV Model'!B18*((1-(1+F23)^(-'rNPV Model'!B47))/F23)/(1+F23)^('rNPV Model'!B8-'rNPV Model'!B10)*C23)+('rNPV Model'!B60*((1-(1+F23)^(-'rNPV Model'!B57))/F23)/(1+F23)^('rNPV Model'!B9-'rNPV Model'!B10)*D23)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+F23)^2.5)))*$D$7+E23+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>4.9780506833833842</v>
+        <v>4.9618429636502954</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="I23" s="53"/>
       <c r="J23" s="53"/>
@@ -3121,7 +3121,7 @@
       </c>
       <c r="G24" s="73">
         <f>((('rNPV Model'!B13*B24*'rNPV Model'!B16*'rNPV Model'!B18*((1-(1+F24)^(-'rNPV Model'!B47))/F24)/(1+F24)^('rNPV Model'!B8-'rNPV Model'!B10)*C24)+('rNPV Model'!B60*((1-(1+F24)^(-'rNPV Model'!B57))/F24)/(1+F24)^('rNPV Model'!B9-'rNPV Model'!B10)*D24)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+F24)^2.5))+MAX(0,(('rNPV Model'!B13*B24*'rNPV Model'!B16*'rNPV Model'!B18*((1-(1+F24)^(-'rNPV Model'!B47))/F24)/(1+F24)^('rNPV Model'!B8-'rNPV Model'!B10)*C24)+('rNPV Model'!B60*((1-(1+F24)^(-'rNPV Model'!B57))/F24)/(1+F24)^('rNPV Model'!B9-'rNPV Model'!B10)*D24)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+F24)^2.5)))*$D$7+E24+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
-        <v>6.6602865022270858</v>
+        <v>6.6386016975041242</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>164</v>

</xml_diff>

<commit_message>
Justification for high FSCD market penetration
</commit_message>
<xml_diff>
--- a/PALI_rNPV_Model.xlsx
+++ b/PALI_rNPV_Model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dan\OneDrive\Documents\Equity Research\PALI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBF4201F-7C90-418A-9665-34E16C90113C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36AC6B6E-C3FA-4547-9409-272580D47DF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Diluted Shares" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="196">
   <si>
     <t>PALISADE BIO (PALI) — Fully Diluted Share Count</t>
   </si>
@@ -612,6 +612,9 @@
   </si>
   <si>
     <t>FSCD $3B peak: 320K US patients, $40K/yr orphan-adjacent pricing, 16% penetration, 0.5x ROW.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Competitor: Cardiac toxicity risks and REMS monitoring severly restricts Agomab adoption; PALI-2108 captures FSCD first-line oral and becomes SoC </t>
   </si>
 </sst>
 </file>
@@ -1608,7 +1611,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A77" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A103" sqref="A103"/>
     </sheetView>
   </sheetViews>
@@ -2582,10 +2585,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:K49"/>
+  <dimension ref="A1:K50"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3171,8 +3174,8 @@
       <c r="J27" s="53"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A28" s="1" t="s">
-        <v>166</v>
+      <c r="A28" s="87" t="s">
+        <v>172</v>
       </c>
       <c r="B28" s="53"/>
       <c r="C28" s="53"/>
@@ -3186,7 +3189,7 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
-        <v>194</v>
+        <v>166</v>
       </c>
       <c r="B29" s="53"/>
       <c r="C29" s="53"/>
@@ -3199,8 +3202,8 @@
       <c r="J29" s="53"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A30" s="87" t="s">
-        <v>172</v>
+      <c r="A30" s="1" t="s">
+        <v>194</v>
       </c>
       <c r="B30" s="53"/>
       <c r="C30" s="53"/>
@@ -3227,7 +3230,9 @@
       <c r="J31" s="53"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A32" s="1"/>
+      <c r="A32" s="1" t="s">
+        <v>195</v>
+      </c>
       <c r="B32" s="53"/>
       <c r="C32" s="53"/>
       <c r="D32" s="53"/>
@@ -3239,7 +3244,7 @@
       <c r="J32" s="53"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A33" s="88"/>
+      <c r="A33" s="1"/>
       <c r="B33" s="53"/>
       <c r="C33" s="53"/>
       <c r="D33" s="53"/>
@@ -3251,7 +3256,7 @@
       <c r="J33" s="53"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A34" s="53"/>
+      <c r="A34" s="88"/>
       <c r="B34" s="53"/>
       <c r="C34" s="53"/>
       <c r="D34" s="53"/>
@@ -3442,6 +3447,18 @@
       <c r="I49" s="53"/>
       <c r="J49" s="53"/>
     </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A50" s="53"/>
+      <c r="B50" s="53"/>
+      <c r="C50" s="53"/>
+      <c r="D50" s="53"/>
+      <c r="E50" s="53"/>
+      <c r="F50" s="53"/>
+      <c r="G50" s="53"/>
+      <c r="H50" s="53"/>
+      <c r="I50" s="53"/>
+      <c r="J50" s="53"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Variable M&A premium (%)
</commit_message>
<xml_diff>
--- a/PALI_rNPV_Model.xlsx
+++ b/PALI_rNPV_Model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dan\OneDrive\Documents\Equity Research\PALI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36AC6B6E-C3FA-4547-9409-272580D47DF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AE4AD2D-5C16-4351-93A3-E60FED631349}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="197">
   <si>
     <t>PALISADE BIO (PALI) — Fully Diluted Share Count</t>
   </si>
@@ -383,9 +383,6 @@
     <t>STRATEGIC &amp; OPTION VALUE</t>
   </si>
   <si>
-    <t>25% — oral dual-mechanism, IP to 2041, validated PDE4B target</t>
-  </si>
-  <si>
     <t>Platform / preclinical optionality ($M)</t>
   </si>
   <si>
@@ -536,9 +533,6 @@
     <t>M&amp;A Premium</t>
   </si>
   <si>
-    <t>Partnership / M&amp;A premium (25%)</t>
-  </si>
-  <si>
     <t>Base Fair Value</t>
   </si>
   <si>
@@ -602,9 +596,6 @@
     <t>first &amp; only therapy; strong first-mover; blending symptomatic/Active penetration (22%) with Post-op maintenance penetration (10%)</t>
   </si>
   <si>
-    <t>Zero fibrosis signals, FSCD discontinued, and UC becomes a commercial flop (immediate cash value is still $0.85)</t>
-  </si>
-  <si>
     <t>Assumption: ~$60M raise at ~$6.00/share Phase 3 funding event (2028)</t>
   </si>
   <si>
@@ -615,6 +606,18 @@
   </si>
   <si>
     <t xml:space="preserve">Competitor: Cardiac toxicity risks and REMS monitoring severly restricts Agomab adoption; PALI-2108 captures FSCD first-line oral and becomes SoC </t>
+  </si>
+  <si>
+    <t>Zero fibrosis signals, FSCD discontinued, and UC becomes a commercial flop. Immediate cash floor is $0.89 ($0.62 w/o Phase 3 raise projection)</t>
+  </si>
+  <si>
+    <t>Partnership / M&amp;A premium ($M)</t>
+  </si>
+  <si>
+    <t>Partnership / M&amp;A premium (%)</t>
+  </si>
+  <si>
+    <t>oral dual-mechanism, IP to 2041, validated PDE4B target</t>
   </si>
 </sst>
 </file>
@@ -630,7 +633,7 @@
     <numFmt numFmtId="169" formatCode="\$#,##0.00_);[Red]&quot;($&quot;#,##0.00\)"/>
     <numFmt numFmtId="170" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
-  <fonts count="35" x14ac:knownFonts="1">
+  <fonts count="34" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -846,12 +849,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <i/>
       <sz val="9"/>
       <color rgb="FF666666"/>
@@ -960,7 +957,7 @@
     <xf numFmtId="9" fontId="25" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="21" fillId="2" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1070,7 +1067,6 @@
     <xf numFmtId="164" fontId="31" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="27" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1080,7 +1076,7 @@
     <xf numFmtId="164" fontId="27" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="28" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1089,7 +1085,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="5" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="34" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="33" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -1374,20 +1370,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="93" t="s">
+      <c r="A1" s="92" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="93"/>
-      <c r="C1" s="93"/>
-      <c r="D1" s="93"/>
+      <c r="B1" s="92"/>
+      <c r="C1" s="92"/>
+      <c r="D1" s="92"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="94" t="s">
+      <c r="A2" s="93" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="94"/>
-      <c r="C2" s="94"/>
-      <c r="D2" s="94"/>
+      <c r="B2" s="93"/>
+      <c r="C2" s="93"/>
+      <c r="D2" s="93"/>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
@@ -1425,7 +1421,7 @@
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B8" s="9">
         <v>57270786</v>
@@ -1434,7 +1430,7 @@
         <v>1E-4</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -1453,7 +1449,7 @@
     </row>
     <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B10" s="9">
         <v>6850356</v>
@@ -1462,12 +1458,12 @@
         <v>1.155</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B11" s="9">
         <v>0</v>
@@ -1570,7 +1566,7 @@
         <v>6</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -1609,10 +1605,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C102"/>
+  <dimension ref="A1:C103"/>
   <sheetViews>
-    <sheetView topLeftCell="A77" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A103" sqref="A103"/>
+    <sheetView topLeftCell="A71" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A104" sqref="A104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1623,18 +1619,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="93" t="s">
+      <c r="A1" s="92" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="93"/>
-      <c r="C1" s="93"/>
+      <c r="B1" s="92"/>
+      <c r="C1" s="92"/>
     </row>
     <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="94" t="s">
+      <c r="A2" s="93" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="94"/>
-      <c r="C2" s="94"/>
+      <c r="B2" s="93"/>
+      <c r="C2" s="93"/>
     </row>
     <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
@@ -1651,7 +1647,7 @@
         <v>0.13</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -1662,14 +1658,14 @@
         <v>0</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="91">
+      <c r="B7" s="90">
         <v>2041</v>
       </c>
       <c r="C7" s="21" t="s">
@@ -1680,7 +1676,7 @@
       <c r="A8" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="91">
+      <c r="B8" s="90">
         <v>2031</v>
       </c>
       <c r="C8" s="21" t="s">
@@ -1691,7 +1687,7 @@
       <c r="A9" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="91">
+      <c r="B9" s="90">
         <v>2032</v>
       </c>
       <c r="C9" s="21" t="s">
@@ -1702,7 +1698,7 @@
       <c r="A10" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="91">
+      <c r="B10" s="90">
         <v>2026</v>
       </c>
       <c r="C10" s="21" t="s">
@@ -1735,7 +1731,7 @@
         <v>0.06</v>
       </c>
       <c r="C14" s="21" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -1862,7 +1858,7 @@
         <v>320000</v>
       </c>
       <c r="C28" s="21" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -1884,7 +1880,7 @@
         <v>0.16</v>
       </c>
       <c r="C30" s="21" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -2158,7 +2154,7 @@
         <v>3072</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -2248,8 +2244,8 @@
       <c r="B67" s="22">
         <v>-25</v>
       </c>
-      <c r="C67" s="87" t="s">
-        <v>175</v>
+      <c r="C67" s="86" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -2261,7 +2257,7 @@
         <v>-24.75</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -2284,7 +2280,7 @@
         <v>-12.8</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -2294,8 +2290,8 @@
       <c r="B71" s="22">
         <v>-42</v>
       </c>
-      <c r="C71" s="87" t="s">
-        <v>176</v>
+      <c r="C71" s="86" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -2360,218 +2356,227 @@
       <c r="C78" s="30"/>
     </row>
     <row r="79" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A79" s="83" t="s">
+      <c r="A79" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="B79" s="20">
+        <v>0.25</v>
+      </c>
+      <c r="C79" s="1"/>
+    </row>
+    <row r="80" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A80" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="B80" s="36">
+        <f>MAX(0,B76)*B79</f>
+        <v>80.974445690139191</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A81" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B81" s="22">
+        <v>50</v>
+      </c>
+      <c r="C81" s="86" t="s">
         <v>169</v>
       </c>
-      <c r="B79" s="36">
-        <f>MAX(0,B76)*0.25</f>
-        <v>80.974445690139191</v>
-      </c>
-      <c r="C79" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A80" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="B80" s="22">
-        <v>50</v>
-      </c>
-      <c r="C80" s="87" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A81" s="5"/>
-      <c r="B81" s="38"/>
-      <c r="C81" s="30"/>
     </row>
     <row r="82" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A82" s="28" t="s">
-        <v>120</v>
-      </c>
+      <c r="A82" s="5"/>
       <c r="B82" s="38"/>
       <c r="C82" s="30"/>
     </row>
     <row r="83" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A83" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="B83" s="22">
-        <v>205.7</v>
-      </c>
-      <c r="C83" s="1" t="s">
-        <v>188</v>
-      </c>
+      <c r="A83" s="28" t="s">
+        <v>119</v>
+      </c>
+      <c r="B83" s="38"/>
+      <c r="C83" s="30"/>
     </row>
     <row r="84" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A84" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B84" s="22">
+        <v>205.7</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A85" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B85" s="22">
+        <v>-5</v>
+      </c>
+      <c r="C85" s="30"/>
+    </row>
+    <row r="86" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A86" s="33" t="s">
         <v>122</v>
       </c>
-      <c r="B84" s="22">
-        <v>-5</v>
-      </c>
-      <c r="C84" s="30"/>
-    </row>
-    <row r="85" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A85" s="33" t="s">
+      <c r="B86" s="39">
+        <f>B84+B85</f>
+        <v>200.7</v>
+      </c>
+      <c r="C86" s="40" t="s">
         <v>123</v>
       </c>
-      <c r="B85" s="39">
-        <f>B83+B84</f>
-        <v>200.7</v>
-      </c>
-      <c r="C85" s="40" t="s">
+    </row>
+    <row r="87" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A87" s="5"/>
+      <c r="B87" s="30"/>
+      <c r="C87" s="30"/>
+    </row>
+    <row r="88" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A88" s="16" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A86" s="5"/>
-      <c r="B86" s="30"/>
-      <c r="C86" s="30"/>
-    </row>
-    <row r="87" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A87" s="16" t="s">
+      <c r="B88" s="41">
+        <f>B76+B80+B81+B86</f>
+        <v>655.572228450696</v>
+      </c>
+      <c r="C88" s="42" t="s">
         <v>125</v>
       </c>
-      <c r="B87" s="41">
-        <f>B76+B79+B80+B85</f>
-        <v>655.572228450696</v>
-      </c>
-      <c r="C87" s="42" t="s">
+    </row>
+    <row r="89" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A89" s="30"/>
+      <c r="B89" s="38"/>
+      <c r="C89" s="30"/>
+    </row>
+    <row r="90" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A90" s="7" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A88" s="30"/>
-      <c r="B88" s="38"/>
-      <c r="C88" s="30"/>
-    </row>
-    <row r="89" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A89" s="7" t="s">
+      <c r="B90" s="43"/>
+      <c r="C90" s="27"/>
+    </row>
+    <row r="91" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A91" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="B89" s="43"/>
-      <c r="C89" s="27"/>
-    </row>
-    <row r="90" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A90" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="B90" s="44">
+      <c r="B91" s="44">
         <f>'Diluted Shares'!B24</f>
         <v>236262162</v>
       </c>
-      <c r="C90" s="30"/>
-    </row>
-    <row r="91" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A91" s="45" t="s">
-        <v>129</v>
-      </c>
-      <c r="B91" s="46">
-        <f>B87*1000000/B90</f>
+      <c r="C91" s="30"/>
+    </row>
+    <row r="92" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A92" s="45" t="s">
+        <v>128</v>
+      </c>
+      <c r="B92" s="46">
+        <f>B88*1000000/B91</f>
         <v>2.7747660602999815</v>
       </c>
-      <c r="C91" s="30"/>
-    </row>
-    <row r="92" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A92" s="30"/>
-      <c r="B92" s="30"/>
       <c r="C92" s="30"/>
     </row>
     <row r="93" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A93" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="B93" s="47">
-        <v>1.74</v>
-      </c>
+      <c r="A93" s="30"/>
+      <c r="B93" s="30"/>
       <c r="C93" s="30"/>
     </row>
     <row r="94" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A94" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="B94" s="47">
+        <v>1.74</v>
+      </c>
+      <c r="C94" s="30"/>
+    </row>
+    <row r="95" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A95" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="B95" s="25">
+        <f>(B92-B94)/B94</f>
+        <v>0.59469313810343771</v>
+      </c>
+      <c r="C95" s="30"/>
+    </row>
+    <row r="96" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A96" s="30"/>
+      <c r="B96" s="30"/>
+      <c r="C96" s="30"/>
+    </row>
+    <row r="97" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A97" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="B94" s="25">
-        <f>(B91-B93)/B93</f>
-        <v>0.59469313810343771</v>
-      </c>
-      <c r="C94" s="30"/>
-    </row>
-    <row r="95" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A95" s="30"/>
-      <c r="B95" s="30"/>
-      <c r="C95" s="30"/>
-    </row>
-    <row r="96" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A96" s="5" t="s">
+      <c r="B97" s="10">
+        <v>12</v>
+      </c>
+      <c r="C97" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="B96" s="10">
-        <v>12</v>
-      </c>
-      <c r="C96" s="1" t="s">
+    </row>
+    <row r="98" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A98" s="30"/>
+      <c r="B98" s="30"/>
+      <c r="C98" s="30"/>
+    </row>
+    <row r="99" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A99" s="7" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="97" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A97" s="30"/>
-      <c r="B97" s="30"/>
-      <c r="C97" s="30"/>
-    </row>
-    <row r="98" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A98" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="B98" s="48"/>
-      <c r="C98" s="48"/>
-    </row>
-    <row r="99" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A99" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="B99" s="49">
-        <f>B85*1000000/B90</f>
-        <v>0.8494800788287038</v>
-      </c>
-      <c r="C99" s="1" t="s">
-        <v>136</v>
-      </c>
+      <c r="B99" s="48"/>
+      <c r="C99" s="48"/>
     </row>
     <row r="100" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A100" s="5" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B100" s="49">
-        <f>B76*1000000/B90</f>
-        <v>1.3709253314991536</v>
+        <f>B86*1000000/B91</f>
+        <v>0.8494800788287038</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A101" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="B101" s="49">
+        <f>B76*1000000/B91</f>
+        <v>1.3709253314991536</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A102" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="B102" s="49">
+        <f>(B80+B81)*1000000/B91</f>
+        <v>0.55436064997212375</v>
+      </c>
+      <c r="C102" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B101" s="49">
-        <f>(B79+B80)*1000000/B90</f>
-        <v>0.55436064997212375</v>
-      </c>
-      <c r="C101" s="1" t="s">
+    </row>
+    <row r="103" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A103" s="50" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="102" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A102" s="50" t="s">
-        <v>141</v>
-      </c>
-      <c r="B102" s="51">
-        <f>B91</f>
+      <c r="B103" s="51">
+        <f>B92</f>
         <v>2.7747660602999815</v>
       </c>
-      <c r="C102" s="1"/>
+      <c r="C103" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2599,7 +2604,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="52" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B1" s="53"/>
       <c r="C1" s="53"/>
@@ -2625,7 +2630,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="54" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B3" s="55"/>
       <c r="C3" s="55"/>
@@ -2639,14 +2644,14 @@
     </row>
     <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="56" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B4" s="77">
         <f>'rNPV Model'!B5</f>
         <v>0.13</v>
       </c>
       <c r="C4" s="80" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D4" s="77">
         <f>'rNPV Model'!B14</f>
@@ -2661,14 +2666,14 @@
     </row>
     <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="57" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B5" s="77">
         <f>'rNPV Model'!B25</f>
         <v>0.28350000000000003</v>
       </c>
       <c r="C5" s="59" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D5" s="77">
         <f>'rNPV Model'!B43</f>
@@ -2683,17 +2688,17 @@
     </row>
     <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="57" t="s">
-        <v>128</v>
-      </c>
-      <c r="B6" s="84">
-        <f>'rNPV Model'!B90</f>
+        <v>127</v>
+      </c>
+      <c r="B6" s="83">
+        <f>'rNPV Model'!B91</f>
         <v>236262162</v>
       </c>
       <c r="C6" s="59" t="s">
-        <v>148</v>
-      </c>
-      <c r="D6" s="85">
-        <f>'rNPV Model'!B85</f>
+        <v>147</v>
+      </c>
+      <c r="D6" s="84">
+        <f>'rNPV Model'!B86</f>
         <v>200.7</v>
       </c>
       <c r="E6" s="60"/>
@@ -2705,17 +2710,17 @@
     </row>
     <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="80" t="s">
-        <v>149</v>
-      </c>
-      <c r="B7" s="85">
-        <f>'rNPV Model'!B80</f>
+        <v>148</v>
+      </c>
+      <c r="B7" s="84">
+        <f>'rNPV Model'!B81</f>
         <v>50</v>
       </c>
       <c r="C7" s="79" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D7" s="76">
-        <f>0.25</f>
+        <f>'rNPV Model'!B79</f>
         <v>0.25</v>
       </c>
       <c r="E7" s="60"/>
@@ -2727,17 +2732,17 @@
     </row>
     <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="78" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B8" s="61">
-        <f>'rNPV Model'!B91</f>
+        <f>'rNPV Model'!B92</f>
         <v>2.7747660602999815</v>
       </c>
       <c r="C8" s="59" t="s">
-        <v>150</v>
-      </c>
-      <c r="D8" s="86">
-        <f>'rNPV Model'!B93</f>
+        <v>149</v>
+      </c>
+      <c r="D8" s="85">
+        <f>'rNPV Model'!B94</f>
         <v>1.74</v>
       </c>
       <c r="E8" s="60"/>
@@ -2761,7 +2766,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="54" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B10" s="55"/>
       <c r="C10" s="55"/>
@@ -2775,7 +2780,7 @@
     </row>
     <row r="11" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="62" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B11" s="63">
         <v>0.02</v>
@@ -2802,23 +2807,23 @@
         <v>0.11</v>
       </c>
       <c r="B12" s="64">
-        <f>(((((('rNPV Model'!B13*B$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A12)^(-'rNPV Model'!B47))/$A12))/(1+$A12)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A12)^(-'rNPV Model'!B57))/$A12))/(1+$A12)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A12)^2.5))+MAX(0,((((('rNPV Model'!B13*B$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A12)^(-'rNPV Model'!B47))/$A12))/(1+$A12)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A12)^(-'rNPV Model'!B57))/$A12))/(1+$A12)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A12)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
+        <f>(((((('rNPV Model'!B13*B$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A12)^(-'rNPV Model'!B47))/$A12))/(1+$A12)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A12)^(-'rNPV Model'!B57))/$A12))/(1+$A12)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A12)^2.5))+MAX(0,((((('rNPV Model'!B13*B$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A12)^(-'rNPV Model'!B47))/$A12))/(1+$A12)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A12)^(-'rNPV Model'!B57))/$A12))/(1+$A12)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A12)^2.5)))*$D$7+'rNPV Model'!B81+'rNPV Model'!B86)*1000000/'rNPV Model'!B91</f>
         <v>2.7415196266485968</v>
       </c>
       <c r="C12" s="64">
-        <f>(((((('rNPV Model'!B13*C$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A12)^(-'rNPV Model'!B47))/$A12))/(1+$A12)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A12)^(-'rNPV Model'!B57))/$A12))/(1+$A12)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A12)^2.5))+MAX(0,((((('rNPV Model'!B13*C$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A12)^(-'rNPV Model'!B47))/$A12))/(1+$A12)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A12)^(-'rNPV Model'!B57))/$A12))/(1+$A12)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A12)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
+        <f>(((((('rNPV Model'!B13*C$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A12)^(-'rNPV Model'!B47))/$A12))/(1+$A12)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A12)^(-'rNPV Model'!B57))/$A12))/(1+$A12)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A12)^2.5))+MAX(0,((((('rNPV Model'!B13*C$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A12)^(-'rNPV Model'!B47))/$A12))/(1+$A12)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A12)^(-'rNPV Model'!B57))/$A12))/(1+$A12)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A12)^2.5)))*$D$7+'rNPV Model'!B81+'rNPV Model'!B86)*1000000/'rNPV Model'!B91</f>
         <v>2.9616915635072525</v>
       </c>
       <c r="D12" s="64">
-        <f>(((((('rNPV Model'!B13*D$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A12)^(-'rNPV Model'!B47))/$A12))/(1+$A12)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A12)^(-'rNPV Model'!B57))/$A12))/(1+$A12)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A12)^2.5))+MAX(0,((((('rNPV Model'!B13*D$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A12)^(-'rNPV Model'!B47))/$A12))/(1+$A12)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A12)^(-'rNPV Model'!B57))/$A12))/(1+$A12)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A12)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
+        <f>(((((('rNPV Model'!B13*D$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A12)^(-'rNPV Model'!B47))/$A12))/(1+$A12)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A12)^(-'rNPV Model'!B57))/$A12))/(1+$A12)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A12)^2.5))+MAX(0,((((('rNPV Model'!B13*D$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A12)^(-'rNPV Model'!B47))/$A12))/(1+$A12)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A12)^(-'rNPV Model'!B57))/$A12))/(1+$A12)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A12)^2.5)))*$D$7+'rNPV Model'!B81+'rNPV Model'!B86)*1000000/'rNPV Model'!B91</f>
         <v>3.181863500365909</v>
       </c>
       <c r="E12" s="64">
-        <f>(((((('rNPV Model'!B13*E$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A12)^(-'rNPV Model'!B47))/$A12))/(1+$A12)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A12)^(-'rNPV Model'!B57))/$A12))/(1+$A12)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A12)^2.5))+MAX(0,((((('rNPV Model'!B13*E$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A12)^(-'rNPV Model'!B47))/$A12))/(1+$A12)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A12)^(-'rNPV Model'!B57))/$A12))/(1+$A12)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A12)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
+        <f>(((((('rNPV Model'!B13*E$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A12)^(-'rNPV Model'!B47))/$A12))/(1+$A12)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A12)^(-'rNPV Model'!B57))/$A12))/(1+$A12)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A12)^2.5))+MAX(0,((((('rNPV Model'!B13*E$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A12)^(-'rNPV Model'!B47))/$A12))/(1+$A12)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A12)^(-'rNPV Model'!B57))/$A12))/(1+$A12)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A12)^2.5)))*$D$7+'rNPV Model'!B81+'rNPV Model'!B86)*1000000/'rNPV Model'!B91</f>
         <v>3.4020354372245647</v>
       </c>
       <c r="F12" s="64">
-        <f>(((((('rNPV Model'!B13*F$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A12)^(-'rNPV Model'!B47))/$A12))/(1+$A12)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A12)^(-'rNPV Model'!B57))/$A12))/(1+$A12)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A12)^2.5))+MAX(0,((((('rNPV Model'!B13*F$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A12)^(-'rNPV Model'!B47))/$A12))/(1+$A12)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A12)^(-'rNPV Model'!B57))/$A12))/(1+$A12)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A12)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
+        <f>(((((('rNPV Model'!B13*F$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A12)^(-'rNPV Model'!B47))/$A12))/(1+$A12)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A12)^(-'rNPV Model'!B57))/$A12))/(1+$A12)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A12)^2.5))+MAX(0,((((('rNPV Model'!B13*F$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A12)^(-'rNPV Model'!B47))/$A12))/(1+$A12)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A12)^(-'rNPV Model'!B57))/$A12))/(1+$A12)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A12)^2.5)))*$D$7+'rNPV Model'!B81+'rNPV Model'!B86)*1000000/'rNPV Model'!B91</f>
         <v>3.6222073740832208</v>
       </c>
       <c r="G12" s="53"/>
@@ -2831,23 +2836,23 @@
         <v>0.12</v>
       </c>
       <c r="B13" s="65">
-        <f>(((((('rNPV Model'!B13*B$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A13)^(-'rNPV Model'!B47))/$A13))/(1+$A13)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A13)^(-'rNPV Model'!B57))/$A13))/(1+$A13)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A13)^2.5))+MAX(0,((((('rNPV Model'!B13*B$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A13)^(-'rNPV Model'!B47))/$A13))/(1+$A13)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A13)^(-'rNPV Model'!B57))/$A13))/(1+$A13)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A13)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
+        <f>(((((('rNPV Model'!B13*B$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A13)^(-'rNPV Model'!B47))/$A13))/(1+$A13)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A13)^(-'rNPV Model'!B57))/$A13))/(1+$A13)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A13)^2.5))+MAX(0,((((('rNPV Model'!B13*B$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A13)^(-'rNPV Model'!B47))/$A13))/(1+$A13)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A13)^(-'rNPV Model'!B57))/$A13))/(1+$A13)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A13)^2.5)))*$D$7+'rNPV Model'!B81+'rNPV Model'!B86)*1000000/'rNPV Model'!B91</f>
         <v>2.5633108693686455</v>
       </c>
       <c r="C13" s="65">
-        <f>(((((('rNPV Model'!B13*C$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A13)^(-'rNPV Model'!B47))/$A13))/(1+$A13)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A13)^(-'rNPV Model'!B57))/$A13))/(1+$A13)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A13)^2.5))+MAX(0,((((('rNPV Model'!B13*C$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A13)^(-'rNPV Model'!B47))/$A13))/(1+$A13)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A13)^(-'rNPV Model'!B57))/$A13))/(1+$A13)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A13)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
+        <f>(((((('rNPV Model'!B13*C$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A13)^(-'rNPV Model'!B47))/$A13))/(1+$A13)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A13)^(-'rNPV Model'!B57))/$A13))/(1+$A13)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A13)^2.5))+MAX(0,((((('rNPV Model'!B13*C$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A13)^(-'rNPV Model'!B47))/$A13))/(1+$A13)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A13)^(-'rNPV Model'!B57))/$A13))/(1+$A13)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A13)^2.5)))*$D$7+'rNPV Model'!B81+'rNPV Model'!B86)*1000000/'rNPV Model'!B91</f>
         <v>2.7652840340069265</v>
       </c>
       <c r="D13" s="65">
-        <f>(((((('rNPV Model'!B13*D$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A13)^(-'rNPV Model'!B47))/$A13))/(1+$A13)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A13)^(-'rNPV Model'!B57))/$A13))/(1+$A13)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A13)^2.5))+MAX(0,((((('rNPV Model'!B13*D$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A13)^(-'rNPV Model'!B47))/$A13))/(1+$A13)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A13)^(-'rNPV Model'!B57))/$A13))/(1+$A13)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A13)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
+        <f>(((((('rNPV Model'!B13*D$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A13)^(-'rNPV Model'!B47))/$A13))/(1+$A13)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A13)^(-'rNPV Model'!B57))/$A13))/(1+$A13)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A13)^2.5))+MAX(0,((((('rNPV Model'!B13*D$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A13)^(-'rNPV Model'!B47))/$A13))/(1+$A13)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A13)^(-'rNPV Model'!B57))/$A13))/(1+$A13)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A13)^2.5)))*$D$7+'rNPV Model'!B81+'rNPV Model'!B86)*1000000/'rNPV Model'!B91</f>
         <v>2.9672571986452083</v>
       </c>
       <c r="E13" s="65">
-        <f>(((((('rNPV Model'!B13*E$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A13)^(-'rNPV Model'!B47))/$A13))/(1+$A13)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A13)^(-'rNPV Model'!B57))/$A13))/(1+$A13)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A13)^2.5))+MAX(0,((((('rNPV Model'!B13*E$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A13)^(-'rNPV Model'!B47))/$A13))/(1+$A13)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A13)^(-'rNPV Model'!B57))/$A13))/(1+$A13)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A13)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
+        <f>(((((('rNPV Model'!B13*E$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A13)^(-'rNPV Model'!B47))/$A13))/(1+$A13)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A13)^(-'rNPV Model'!B57))/$A13))/(1+$A13)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A13)^2.5))+MAX(0,((((('rNPV Model'!B13*E$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A13)^(-'rNPV Model'!B47))/$A13))/(1+$A13)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A13)^(-'rNPV Model'!B57))/$A13))/(1+$A13)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A13)^2.5)))*$D$7+'rNPV Model'!B81+'rNPV Model'!B86)*1000000/'rNPV Model'!B91</f>
         <v>3.1692303632834893</v>
       </c>
       <c r="F13" s="64">
-        <f>(((((('rNPV Model'!B13*F$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A13)^(-'rNPV Model'!B47))/$A13))/(1+$A13)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A13)^(-'rNPV Model'!B57))/$A13))/(1+$A13)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A13)^2.5))+MAX(0,((((('rNPV Model'!B13*F$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A13)^(-'rNPV Model'!B47))/$A13))/(1+$A13)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A13)^(-'rNPV Model'!B57))/$A13))/(1+$A13)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A13)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
+        <f>(((((('rNPV Model'!B13*F$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A13)^(-'rNPV Model'!B47))/$A13))/(1+$A13)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A13)^(-'rNPV Model'!B57))/$A13))/(1+$A13)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A13)^2.5))+MAX(0,((((('rNPV Model'!B13*F$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A13)^(-'rNPV Model'!B47))/$A13))/(1+$A13)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A13)^(-'rNPV Model'!B57))/$A13))/(1+$A13)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A13)^2.5)))*$D$7+'rNPV Model'!B81+'rNPV Model'!B86)*1000000/'rNPV Model'!B91</f>
         <v>3.3712035279217707</v>
       </c>
       <c r="G13" s="53"/>
@@ -2860,23 +2865,23 @@
         <v>0.13</v>
       </c>
       <c r="B14" s="65">
-        <f>(((((('rNPV Model'!B13*B$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A14)^(-'rNPV Model'!B47))/$A14))/(1+$A14)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A14)^(-'rNPV Model'!B57))/$A14))/(1+$A14)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A14)^2.5))+MAX(0,((((('rNPV Model'!B13*B$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A14)^(-'rNPV Model'!B47))/$A14))/(1+$A14)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A14)^(-'rNPV Model'!B57))/$A14))/(1+$A14)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A14)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
+        <f>(((((('rNPV Model'!B13*B$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A14)^(-'rNPV Model'!B47))/$A14))/(1+$A14)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A14)^(-'rNPV Model'!B57))/$A14))/(1+$A14)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A14)^2.5))+MAX(0,((((('rNPV Model'!B13*B$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A14)^(-'rNPV Model'!B47))/$A14))/(1+$A14)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A14)^(-'rNPV Model'!B57))/$A14))/(1+$A14)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A14)^2.5)))*$D$7+'rNPV Model'!B81+'rNPV Model'!B86)*1000000/'rNPV Model'!B91</f>
         <v>2.403696569944318</v>
       </c>
       <c r="C14" s="82">
-        <f>(((((('rNPV Model'!B13*C$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A14)^(-'rNPV Model'!B47))/$A14))/(1+$A14)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A14)^(-'rNPV Model'!B57))/$A14))/(1+$A14)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A14)^2.5))+MAX(0,((((('rNPV Model'!B13*C$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A14)^(-'rNPV Model'!B47))/$A14))/(1+$A14)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A14)^(-'rNPV Model'!B57))/$A14))/(1+$A14)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A14)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
+        <f>(((((('rNPV Model'!B13*C$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A14)^(-'rNPV Model'!B47))/$A14))/(1+$A14)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A14)^(-'rNPV Model'!B57))/$A14))/(1+$A14)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A14)^2.5))+MAX(0,((((('rNPV Model'!B13*C$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A14)^(-'rNPV Model'!B47))/$A14))/(1+$A14)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A14)^(-'rNPV Model'!B57))/$A14))/(1+$A14)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A14)^2.5)))*$D$7+'rNPV Model'!B81+'rNPV Model'!B86)*1000000/'rNPV Model'!B91</f>
         <v>2.5892313151221491</v>
       </c>
       <c r="D14" s="81">
-        <f>(((((('rNPV Model'!B13*D$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A14)^(-'rNPV Model'!B47))/$A14))/(1+$A14)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A14)^(-'rNPV Model'!B57))/$A14))/(1+$A14)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A14)^2.5))+MAX(0,((((('rNPV Model'!B13*D$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A14)^(-'rNPV Model'!B47))/$A14))/(1+$A14)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A14)^(-'rNPV Model'!B57))/$A14))/(1+$A14)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A14)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
+        <f>(((((('rNPV Model'!B13*D$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A14)^(-'rNPV Model'!B47))/$A14))/(1+$A14)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A14)^(-'rNPV Model'!B57))/$A14))/(1+$A14)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A14)^2.5))+MAX(0,((((('rNPV Model'!B13*D$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A14)^(-'rNPV Model'!B47))/$A14))/(1+$A14)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A14)^(-'rNPV Model'!B57))/$A14))/(1+$A14)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A14)^2.5)))*$D$7+'rNPV Model'!B81+'rNPV Model'!B86)*1000000/'rNPV Model'!B91</f>
         <v>2.7747660602999815</v>
       </c>
       <c r="E14" s="65">
-        <f>(((((('rNPV Model'!B13*E$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A14)^(-'rNPV Model'!B47))/$A14))/(1+$A14)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A14)^(-'rNPV Model'!B57))/$A14))/(1+$A14)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A14)^2.5))+MAX(0,((((('rNPV Model'!B13*E$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A14)^(-'rNPV Model'!B47))/$A14))/(1+$A14)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A14)^(-'rNPV Model'!B57))/$A14))/(1+$A14)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A14)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
+        <f>(((((('rNPV Model'!B13*E$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A14)^(-'rNPV Model'!B47))/$A14))/(1+$A14)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A14)^(-'rNPV Model'!B57))/$A14))/(1+$A14)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A14)^2.5))+MAX(0,((((('rNPV Model'!B13*E$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A14)^(-'rNPV Model'!B47))/$A14))/(1+$A14)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A14)^(-'rNPV Model'!B57))/$A14))/(1+$A14)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A14)^2.5)))*$D$7+'rNPV Model'!B81+'rNPV Model'!B86)*1000000/'rNPV Model'!B91</f>
         <v>2.960300805477813</v>
       </c>
       <c r="F14" s="66">
-        <f>(((((('rNPV Model'!B13*F$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A14)^(-'rNPV Model'!B47))/$A14))/(1+$A14)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A14)^(-'rNPV Model'!B57))/$A14))/(1+$A14)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A14)^2.5))+MAX(0,((((('rNPV Model'!B13*F$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A14)^(-'rNPV Model'!B47))/$A14))/(1+$A14)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A14)^(-'rNPV Model'!B57))/$A14))/(1+$A14)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A14)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
+        <f>(((((('rNPV Model'!B13*F$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A14)^(-'rNPV Model'!B47))/$A14))/(1+$A14)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A14)^(-'rNPV Model'!B57))/$A14))/(1+$A14)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A14)^2.5))+MAX(0,((((('rNPV Model'!B13*F$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A14)^(-'rNPV Model'!B47))/$A14))/(1+$A14)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A14)^(-'rNPV Model'!B57))/$A14))/(1+$A14)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A14)^2.5)))*$D$7+'rNPV Model'!B81+'rNPV Model'!B86)*1000000/'rNPV Model'!B91</f>
         <v>3.1458355506556446</v>
       </c>
       <c r="G14" s="53"/>
@@ -2889,23 +2894,23 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="B15" s="65">
-        <f>(((((('rNPV Model'!B13*B$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A15)^(-'rNPV Model'!B47))/$A15))/(1+$A15)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A15)^(-'rNPV Model'!B57))/$A15))/(1+$A15)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A15)^2.5))+MAX(0,((((('rNPV Model'!B13*B$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A15)^(-'rNPV Model'!B47))/$A15))/(1+$A15)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A15)^(-'rNPV Model'!B57))/$A15))/(1+$A15)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A15)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
+        <f>(((((('rNPV Model'!B13*B$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A15)^(-'rNPV Model'!B47))/$A15))/(1+$A15)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A15)^(-'rNPV Model'!B57))/$A15))/(1+$A15)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A15)^2.5))+MAX(0,((((('rNPV Model'!B13*B$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A15)^(-'rNPV Model'!B47))/$A15))/(1+$A15)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A15)^(-'rNPV Model'!B57))/$A15))/(1+$A15)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A15)^2.5)))*$D$7+'rNPV Model'!B81+'rNPV Model'!B86)*1000000/'rNPV Model'!B91</f>
         <v>2.2605699938383217</v>
       </c>
       <c r="C15" s="65">
-        <f>(((((('rNPV Model'!B13*C$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A15)^(-'rNPV Model'!B47))/$A15))/(1+$A15)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A15)^(-'rNPV Model'!B57))/$A15))/(1+$A15)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A15)^2.5))+MAX(0,((((('rNPV Model'!B13*C$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A15)^(-'rNPV Model'!B47))/$A15))/(1+$A15)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A15)^(-'rNPV Model'!B57))/$A15))/(1+$A15)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A15)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
+        <f>(((((('rNPV Model'!B13*C$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A15)^(-'rNPV Model'!B47))/$A15))/(1+$A15)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A15)^(-'rNPV Model'!B57))/$A15))/(1+$A15)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A15)^2.5))+MAX(0,((((('rNPV Model'!B13*C$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A15)^(-'rNPV Model'!B47))/$A15))/(1+$A15)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A15)^(-'rNPV Model'!B57))/$A15))/(1+$A15)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A15)^2.5)))*$D$7+'rNPV Model'!B81+'rNPV Model'!B86)*1000000/'rNPV Model'!B91</f>
         <v>2.4312336902103868</v>
       </c>
       <c r="D15" s="65">
-        <f>(((((('rNPV Model'!B13*D$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A15)^(-'rNPV Model'!B47))/$A15))/(1+$A15)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A15)^(-'rNPV Model'!B57))/$A15))/(1+$A15)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A15)^2.5))+MAX(0,((((('rNPV Model'!B13*D$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A15)^(-'rNPV Model'!B47))/$A15))/(1+$A15)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A15)^(-'rNPV Model'!B57))/$A15))/(1+$A15)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A15)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
+        <f>(((((('rNPV Model'!B13*D$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A15)^(-'rNPV Model'!B47))/$A15))/(1+$A15)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A15)^(-'rNPV Model'!B57))/$A15))/(1+$A15)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A15)^2.5))+MAX(0,((((('rNPV Model'!B13*D$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A15)^(-'rNPV Model'!B47))/$A15))/(1+$A15)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A15)^(-'rNPV Model'!B57))/$A15))/(1+$A15)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A15)^2.5)))*$D$7+'rNPV Model'!B81+'rNPV Model'!B86)*1000000/'rNPV Model'!B91</f>
         <v>2.6018973865824502</v>
       </c>
       <c r="E15" s="65">
-        <f>(((((('rNPV Model'!B13*E$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A15)^(-'rNPV Model'!B47))/$A15))/(1+$A15)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A15)^(-'rNPV Model'!B57))/$A15))/(1+$A15)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A15)^2.5))+MAX(0,((((('rNPV Model'!B13*E$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A15)^(-'rNPV Model'!B47))/$A15))/(1+$A15)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A15)^(-'rNPV Model'!B57))/$A15))/(1+$A15)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A15)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
+        <f>(((((('rNPV Model'!B13*E$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A15)^(-'rNPV Model'!B47))/$A15))/(1+$A15)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A15)^(-'rNPV Model'!B57))/$A15))/(1+$A15)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A15)^2.5))+MAX(0,((((('rNPV Model'!B13*E$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A15)^(-'rNPV Model'!B47))/$A15))/(1+$A15)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A15)^(-'rNPV Model'!B57))/$A15))/(1+$A15)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A15)^2.5)))*$D$7+'rNPV Model'!B81+'rNPV Model'!B86)*1000000/'rNPV Model'!B91</f>
         <v>2.7725610829545144</v>
       </c>
       <c r="F15" s="64">
-        <f>(((((('rNPV Model'!B13*F$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A15)^(-'rNPV Model'!B47))/$A15))/(1+$A15)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A15)^(-'rNPV Model'!B57))/$A15))/(1+$A15)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A15)^2.5))+MAX(0,((((('rNPV Model'!B13*F$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A15)^(-'rNPV Model'!B47))/$A15))/(1+$A15)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A15)^(-'rNPV Model'!B57))/$A15))/(1+$A15)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A15)^2.5)))*$D$7+'rNPV Model'!B80+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
+        <f>(((((('rNPV Model'!B13*F$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A15)^(-'rNPV Model'!B47))/$A15))/(1+$A15)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A15)^(-'rNPV Model'!B57))/$A15))/(1+$A15)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A15)^2.5))+MAX(0,((((('rNPV Model'!B13*F$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A15)^(-'rNPV Model'!B47))/$A15))/(1+$A15)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A15)^(-'rNPV Model'!B57))/$A15))/(1+$A15)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A15)^2.5)))*$D$7+'rNPV Model'!B81+'rNPV Model'!B86)*1000000/'rNPV Model'!B91</f>
         <v>2.9432247793265782</v>
       </c>
       <c r="G15" s="53"/>
@@ -2938,8 +2943,8 @@
       <c r="J17" s="53"/>
     </row>
     <row r="18" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="92" t="s">
-        <v>153</v>
+      <c r="A18" s="91" t="s">
+        <v>152</v>
       </c>
       <c r="B18" s="69"/>
       <c r="C18" s="70"/>
@@ -2954,28 +2959,28 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" s="72" t="s">
+        <v>153</v>
+      </c>
+      <c r="B19" s="72" t="s">
         <v>154</v>
       </c>
-      <c r="B19" s="72" t="s">
+      <c r="C19" s="72" t="s">
+        <v>145</v>
+      </c>
+      <c r="D19" s="88" t="s">
+        <v>146</v>
+      </c>
+      <c r="E19" s="88" t="s">
+        <v>171</v>
+      </c>
+      <c r="F19" s="72" t="s">
+        <v>143</v>
+      </c>
+      <c r="G19" s="72" t="s">
         <v>155</v>
       </c>
-      <c r="C19" s="72" t="s">
-        <v>146</v>
-      </c>
-      <c r="D19" s="89" t="s">
-        <v>147</v>
-      </c>
-      <c r="E19" s="89" t="s">
-        <v>173</v>
-      </c>
-      <c r="F19" s="72" t="s">
-        <v>144</v>
-      </c>
-      <c r="G19" s="72" t="s">
+      <c r="H19" s="72" t="s">
         <v>156</v>
-      </c>
-      <c r="H19" s="72" t="s">
-        <v>157</v>
       </c>
       <c r="I19" s="53"/>
       <c r="J19" s="53"/>
@@ -2983,7 +2988,7 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" s="56" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B20" s="76">
         <v>0.02</v>
@@ -2994,18 +2999,18 @@
       <c r="D20" s="77">
         <v>0</v>
       </c>
-      <c r="E20" s="90">
+      <c r="E20" s="89">
         <v>20</v>
       </c>
       <c r="F20" s="76">
         <v>0.14000000000000001</v>
       </c>
       <c r="G20" s="73">
-        <f>((('rNPV Model'!B13*B20*'rNPV Model'!B16*'rNPV Model'!B18*((1-(1+F20)^(-'rNPV Model'!B47))/F20)/(1+F20)^('rNPV Model'!B8-'rNPV Model'!B10)*C20)+('rNPV Model'!B60*((1-(1+F20)^(-'rNPV Model'!B57))/F20)/(1+F20)^('rNPV Model'!B9-'rNPV Model'!B10)*D20)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+F20)^2.5))+MAX(0,(('rNPV Model'!B13*B20*'rNPV Model'!B16*'rNPV Model'!B18*((1-(1+F20)^(-'rNPV Model'!B47))/F20)/(1+F20)^('rNPV Model'!B8-'rNPV Model'!B10)*C20)+('rNPV Model'!B60*((1-(1+F20)^(-'rNPV Model'!B57))/F20)/(1+F20)^('rNPV Model'!B9-'rNPV Model'!B10)*D20)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+F20)^2.5)))*$D$7+E20+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
+        <f>((('rNPV Model'!B13*B20*'rNPV Model'!B16*'rNPV Model'!B18*((1-(1+F20)^(-'rNPV Model'!B47))/F20)/(1+F20)^('rNPV Model'!B8-'rNPV Model'!B10)*C20)+('rNPV Model'!B60*((1-(1+F20)^(-'rNPV Model'!B57))/F20)/(1+F20)^('rNPV Model'!B9-'rNPV Model'!B10)*D20)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+F20)^2.5))+MAX(0,(('rNPV Model'!B13*B20*'rNPV Model'!B16*'rNPV Model'!B18*((1-(1+F20)^(-'rNPV Model'!B47))/F20)/(1+F20)^('rNPV Model'!B8-'rNPV Model'!B10)*C20)+('rNPV Model'!B60*((1-(1+F20)^(-'rNPV Model'!B57))/F20)/(1+F20)^('rNPV Model'!B9-'rNPV Model'!B10)*D20)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+F20)^2.5)))*$D$7+E20+'rNPV Model'!B86)*1000000/'rNPV Model'!B91</f>
         <v>0.65615450400947595</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="I20" s="53"/>
       <c r="J20" s="53"/>
@@ -3013,7 +3018,7 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21" s="56" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B21" s="76">
         <f>'rNPV Model'!B14</f>
@@ -3027,7 +3032,7 @@
         <f>'rNPV Model'!B43</f>
         <v>0.17680000000000004</v>
       </c>
-      <c r="E21" s="90">
+      <c r="E21" s="89">
         <v>50</v>
       </c>
       <c r="F21" s="76">
@@ -3035,7 +3040,7 @@
         <v>0.13</v>
       </c>
       <c r="G21" s="74">
-        <f>((('rNPV Model'!B13*B21*'rNPV Model'!B16*'rNPV Model'!B18*((1-(1+F21)^(-'rNPV Model'!B47))/F21)/(1+F21)^('rNPV Model'!B8-'rNPV Model'!B10)*C21)+('rNPV Model'!B60*((1-(1+F21)^(-'rNPV Model'!B57))/F21)/(1+F21)^('rNPV Model'!B9-'rNPV Model'!B10)*D21)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+F21)^2.5))+MAX(0,(('rNPV Model'!B13*B21*'rNPV Model'!B16*'rNPV Model'!B18*((1-(1+F21)^(-'rNPV Model'!B47))/F21)/(1+F21)^('rNPV Model'!B8-'rNPV Model'!B10)*C21)+('rNPV Model'!B60*((1-(1+F21)^(-'rNPV Model'!B57))/F21)/(1+F21)^('rNPV Model'!B9-'rNPV Model'!B10)*D21)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+F21)^2.5)))*$D$7+E21+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
+        <f>((('rNPV Model'!B13*B21*'rNPV Model'!B16*'rNPV Model'!B18*((1-(1+F21)^(-'rNPV Model'!B47))/F21)/(1+F21)^('rNPV Model'!B8-'rNPV Model'!B10)*C21)+('rNPV Model'!B60*((1-(1+F21)^(-'rNPV Model'!B57))/F21)/(1+F21)^('rNPV Model'!B9-'rNPV Model'!B10)*D21)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+F21)^2.5))+MAX(0,(('rNPV Model'!B13*B21*'rNPV Model'!B16*'rNPV Model'!B18*((1-(1+F21)^(-'rNPV Model'!B47))/F21)/(1+F21)^('rNPV Model'!B8-'rNPV Model'!B10)*C21)+('rNPV Model'!B60*((1-(1+F21)^(-'rNPV Model'!B57))/F21)/(1+F21)^('rNPV Model'!B9-'rNPV Model'!B10)*D21)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+F21)^2.5)))*$D$7+E21+'rNPV Model'!B86)*1000000/'rNPV Model'!B91</f>
         <v>2.7747660602999815</v>
       </c>
       <c r="H21" s="1"/>
@@ -3045,7 +3050,7 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22" s="56" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B22" s="76">
         <v>0.06</v>
@@ -3056,18 +3061,18 @@
       <c r="D22" s="77">
         <v>0.221</v>
       </c>
-      <c r="E22" s="90">
+      <c r="E22" s="89">
         <v>75</v>
       </c>
       <c r="F22" s="76">
         <v>0.13</v>
       </c>
       <c r="G22" s="73">
-        <f>((('rNPV Model'!B13*B22*'rNPV Model'!B16*'rNPV Model'!B18*((1-(1+F22)^(-'rNPV Model'!B47))/F22)/(1+F22)^('rNPV Model'!B8-'rNPV Model'!B10)*C22)+('rNPV Model'!B60*((1-(1+F22)^(-'rNPV Model'!B57))/F22)/(1+F22)^('rNPV Model'!B9-'rNPV Model'!B10)*D22)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+F22)^2.5))+MAX(0,(('rNPV Model'!B13*B22*'rNPV Model'!B16*'rNPV Model'!B18*((1-(1+F22)^(-'rNPV Model'!B47))/F22)/(1+F22)^('rNPV Model'!B8-'rNPV Model'!B10)*C22)+('rNPV Model'!B60*((1-(1+F22)^(-'rNPV Model'!B57))/F22)/(1+F22)^('rNPV Model'!B9-'rNPV Model'!B10)*D22)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+F22)^2.5)))*$D$7+E22+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
+        <f>((('rNPV Model'!B13*B22*'rNPV Model'!B16*'rNPV Model'!B18*((1-(1+F22)^(-'rNPV Model'!B47))/F22)/(1+F22)^('rNPV Model'!B8-'rNPV Model'!B10)*C22)+('rNPV Model'!B60*((1-(1+F22)^(-'rNPV Model'!B57))/F22)/(1+F22)^('rNPV Model'!B9-'rNPV Model'!B10)*D22)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+F22)^2.5))+MAX(0,(('rNPV Model'!B13*B22*'rNPV Model'!B16*'rNPV Model'!B18*((1-(1+F22)^(-'rNPV Model'!B47))/F22)/(1+F22)^('rNPV Model'!B8-'rNPV Model'!B10)*C22)+('rNPV Model'!B60*((1-(1+F22)^(-'rNPV Model'!B57))/F22)/(1+F22)^('rNPV Model'!B9-'rNPV Model'!B10)*D22)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+F22)^2.5)))*$D$7+E22+'rNPV Model'!B86)*1000000/'rNPV Model'!B91</f>
         <v>3.3550775886694248</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="I22" s="53"/>
       <c r="J22" s="53"/>
@@ -3075,7 +3080,7 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23" s="56" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B23" s="76">
         <v>7.0000000000000007E-2</v>
@@ -3086,18 +3091,18 @@
       <c r="D23" s="77">
         <v>0.3</v>
       </c>
-      <c r="E23" s="90">
+      <c r="E23" s="89">
         <v>150</v>
       </c>
       <c r="F23" s="76">
         <v>0.12</v>
       </c>
       <c r="G23" s="73">
-        <f>((('rNPV Model'!B13*B23*'rNPV Model'!B16*'rNPV Model'!B18*((1-(1+F23)^(-'rNPV Model'!B47))/F23)/(1+F23)^('rNPV Model'!B8-'rNPV Model'!B10)*C23)+('rNPV Model'!B60*((1-(1+F23)^(-'rNPV Model'!B57))/F23)/(1+F23)^('rNPV Model'!B9-'rNPV Model'!B10)*D23)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+F23)^2.5))+MAX(0,(('rNPV Model'!B13*B23*'rNPV Model'!B16*'rNPV Model'!B18*((1-(1+F23)^(-'rNPV Model'!B47))/F23)/(1+F23)^('rNPV Model'!B8-'rNPV Model'!B10)*C23)+('rNPV Model'!B60*((1-(1+F23)^(-'rNPV Model'!B57))/F23)/(1+F23)^('rNPV Model'!B9-'rNPV Model'!B10)*D23)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+F23)^2.5)))*$D$7+E23+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
+        <f>((('rNPV Model'!B13*B23*'rNPV Model'!B16*'rNPV Model'!B18*((1-(1+F23)^(-'rNPV Model'!B47))/F23)/(1+F23)^('rNPV Model'!B8-'rNPV Model'!B10)*C23)+('rNPV Model'!B60*((1-(1+F23)^(-'rNPV Model'!B57))/F23)/(1+F23)^('rNPV Model'!B9-'rNPV Model'!B10)*D23)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+F23)^2.5))+MAX(0,(('rNPV Model'!B13*B23*'rNPV Model'!B16*'rNPV Model'!B18*((1-(1+F23)^(-'rNPV Model'!B47))/F23)/(1+F23)^('rNPV Model'!B8-'rNPV Model'!B10)*C23)+('rNPV Model'!B60*((1-(1+F23)^(-'rNPV Model'!B57))/F23)/(1+F23)^('rNPV Model'!B9-'rNPV Model'!B10)*D23)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+F23)^2.5)))*$D$7+E23+'rNPV Model'!B86)*1000000/'rNPV Model'!B91</f>
         <v>4.9618429636502954</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="I23" s="53"/>
       <c r="J23" s="53"/>
@@ -3105,7 +3110,7 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24" s="56" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B24" s="76">
         <v>0.1</v>
@@ -3116,18 +3121,18 @@
       <c r="D24" s="77">
         <v>0.3</v>
       </c>
-      <c r="E24" s="90">
+      <c r="E24" s="89">
         <v>250</v>
       </c>
       <c r="F24" s="76">
         <v>0.1</v>
       </c>
       <c r="G24" s="73">
-        <f>((('rNPV Model'!B13*B24*'rNPV Model'!B16*'rNPV Model'!B18*((1-(1+F24)^(-'rNPV Model'!B47))/F24)/(1+F24)^('rNPV Model'!B8-'rNPV Model'!B10)*C24)+('rNPV Model'!B60*((1-(1+F24)^(-'rNPV Model'!B57))/F24)/(1+F24)^('rNPV Model'!B9-'rNPV Model'!B10)*D24)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+F24)^2.5))+MAX(0,(('rNPV Model'!B13*B24*'rNPV Model'!B16*'rNPV Model'!B18*((1-(1+F24)^(-'rNPV Model'!B47))/F24)/(1+F24)^('rNPV Model'!B8-'rNPV Model'!B10)*C24)+('rNPV Model'!B60*((1-(1+F24)^(-'rNPV Model'!B57))/F24)/(1+F24)^('rNPV Model'!B9-'rNPV Model'!B10)*D24)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+F24)^2.5)))*$D$7+E24+'rNPV Model'!B85)*1000000/'rNPV Model'!B90</f>
+        <f>((('rNPV Model'!B13*B24*'rNPV Model'!B16*'rNPV Model'!B18*((1-(1+F24)^(-'rNPV Model'!B47))/F24)/(1+F24)^('rNPV Model'!B8-'rNPV Model'!B10)*C24)+('rNPV Model'!B60*((1-(1+F24)^(-'rNPV Model'!B57))/F24)/(1+F24)^('rNPV Model'!B9-'rNPV Model'!B10)*D24)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+F24)^2.5))+MAX(0,(('rNPV Model'!B13*B24*'rNPV Model'!B16*'rNPV Model'!B18*((1-(1+F24)^(-'rNPV Model'!B47))/F24)/(1+F24)^('rNPV Model'!B8-'rNPV Model'!B10)*C24)+('rNPV Model'!B60*((1-(1+F24)^(-'rNPV Model'!B57))/F24)/(1+F24)^('rNPV Model'!B9-'rNPV Model'!B10)*D24)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+F24)^2.5)))*$D$7+E24+'rNPV Model'!B86)*1000000/'rNPV Model'!B91</f>
         <v>6.6386016975041242</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I24" s="53"/>
       <c r="J24" s="53"/>
@@ -3147,7 +3152,7 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26" s="75" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B26" s="53"/>
       <c r="C26" s="53"/>
@@ -3161,7 +3166,7 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B27" s="53"/>
       <c r="C27" s="53"/>
@@ -3174,8 +3179,8 @@
       <c r="J27" s="53"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A28" s="87" t="s">
-        <v>172</v>
+      <c r="A28" s="86" t="s">
+        <v>170</v>
       </c>
       <c r="B28" s="53"/>
       <c r="C28" s="53"/>
@@ -3189,7 +3194,7 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B29" s="53"/>
       <c r="C29" s="53"/>
@@ -3203,7 +3208,7 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B30" s="53"/>
       <c r="C30" s="53"/>
@@ -3217,7 +3222,7 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B31" s="53"/>
       <c r="C31" s="53"/>
@@ -3231,7 +3236,7 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B32" s="53"/>
       <c r="C32" s="53"/>
@@ -3256,7 +3261,7 @@
       <c r="J33" s="53"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A34" s="88"/>
+      <c r="A34" s="87"/>
       <c r="B34" s="53"/>
       <c r="C34" s="53"/>
       <c r="D34" s="53"/>

</xml_diff>

<commit_message>
Updated FSCD cPoS projections (bullish)
</commit_message>
<xml_diff>
--- a/PALI_rNPV_Model.xlsx
+++ b/PALI_rNPV_Model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dan\OneDrive\Documents\Equity Research\PALI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AE4AD2D-5C16-4351-93A3-E60FED631349}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD4B844F-2832-40DC-AAF5-5E5270440546}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -578,9 +578,6 @@
     <t>Legacy / Other Warrants</t>
   </si>
   <si>
-    <t>Oct 2025 Pre-Funded Warrants (fully exercised)</t>
-  </si>
-  <si>
     <t>Oct 2025 offering placement agent</t>
   </si>
   <si>
@@ -605,9 +602,6 @@
     <t>FSCD $3B peak: 320K US patients, $40K/yr orphan-adjacent pricing, 16% penetration, 0.5x ROW.</t>
   </si>
   <si>
-    <t xml:space="preserve">Competitor: Cardiac toxicity risks and REMS monitoring severly restricts Agomab adoption; PALI-2108 captures FSCD first-line oral and becomes SoC </t>
-  </si>
-  <si>
     <t>Zero fibrosis signals, FSCD discontinued, and UC becomes a commercial flop. Immediate cash floor is $0.89 ($0.62 w/o Phase 3 raise projection)</t>
   </si>
   <si>
@@ -618,6 +612,12 @@
   </si>
   <si>
     <t>oral dual-mechanism, IP to 2041, validated PDE4B target</t>
+  </si>
+  <si>
+    <t>Competitor: ALK5 class history likely necessitates FDA-mandated cardiac monitoring (REMS) for Agomab despite clean Ph2. PALI-2108 (gut-restricted prodrug) offers unmonitored safety profile, capturing First-Line volume</t>
+  </si>
+  <si>
+    <t>Oct 2025 Pre-Funded Warrants</t>
   </si>
 </sst>
 </file>
@@ -1357,7 +1357,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
@@ -1421,7 +1421,7 @@
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
-        <v>183</v>
+        <v>196</v>
       </c>
       <c r="B8" s="9">
         <v>57270786</v>
@@ -1430,7 +1430,7 @@
         <v>1E-4</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -1458,7 +1458,7 @@
         <v>1.155</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -1566,7 +1566,7 @@
         <v>6</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -1607,7 +1607,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C103"/>
   <sheetViews>
-    <sheetView topLeftCell="A71" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A68" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A104" sqref="A104"/>
     </sheetView>
   </sheetViews>
@@ -1858,7 +1858,7 @@
         <v>320000</v>
       </c>
       <c r="C28" s="21" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -1880,7 +1880,7 @@
         <v>0.16</v>
       </c>
       <c r="C30" s="21" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -1964,7 +1964,7 @@
         <v>52</v>
       </c>
       <c r="B39" s="20">
-        <v>0.8</v>
+        <v>0.85</v>
       </c>
       <c r="C39" s="21" t="s">
         <v>78</v>
@@ -1975,7 +1975,7 @@
         <v>54</v>
       </c>
       <c r="B40" s="20">
-        <v>0.4</v>
+        <v>0.35</v>
       </c>
       <c r="C40" s="21" t="s">
         <v>79</v>
@@ -1986,7 +1986,7 @@
         <v>56</v>
       </c>
       <c r="B41" s="20">
-        <v>0.65</v>
+        <v>0.7</v>
       </c>
       <c r="C41" s="21" t="s">
         <v>80</v>
@@ -1997,7 +1997,7 @@
         <v>58</v>
       </c>
       <c r="B42" s="20">
-        <v>0.85</v>
+        <v>0.9</v>
       </c>
       <c r="C42" s="21" t="s">
         <v>81</v>
@@ -2009,7 +2009,7 @@
       </c>
       <c r="B43" s="25">
         <f>B39*B40*B41*B42</f>
-        <v>0.17680000000000004</v>
+        <v>0.18742500000000001</v>
       </c>
       <c r="C43" s="21" t="s">
         <v>61</v>
@@ -2154,7 +2154,7 @@
         <v>3072</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -2211,7 +2211,7 @@
       </c>
       <c r="B63" s="32">
         <f>B43</f>
-        <v>0.17680000000000004</v>
+        <v>0.18742500000000001</v>
       </c>
       <c r="C63" s="30"/>
     </row>
@@ -2221,7 +2221,7 @@
       </c>
       <c r="B64" s="34">
         <f>B62*B63</f>
-        <v>304.55916569798177</v>
+        <v>322.86200017502387</v>
       </c>
       <c r="C64" s="30"/>
     </row>
@@ -2277,7 +2277,7 @@
       </c>
       <c r="B70" s="36">
         <f>-40*B39*B40</f>
-        <v>-12.8</v>
+        <v>-11.899999999999999</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>179</v>
@@ -2300,7 +2300,7 @@
       </c>
       <c r="B72" s="36">
         <f>(B67+B68+B69+B70+B71)/(1+B5)^2.5</f>
-        <v>-85.86499898982558</v>
+        <v>-85.201948804575963</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>112</v>
@@ -2317,7 +2317,7 @@
       </c>
       <c r="B74" s="37">
         <f>B54+B64</f>
-        <v>409.76278175038232</v>
+        <v>428.06561622742441</v>
       </c>
       <c r="C74" s="30"/>
     </row>
@@ -2327,7 +2327,7 @@
       </c>
       <c r="B75" s="37">
         <f>B72</f>
-        <v>-85.86499898982558</v>
+        <v>-85.201948804575963</v>
       </c>
       <c r="C75" s="30"/>
     </row>
@@ -2337,7 +2337,7 @@
       </c>
       <c r="B76" s="37">
         <f>B74+B75</f>
-        <v>323.89778276055677</v>
+        <v>342.86366742284844</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>116</v>
@@ -2357,7 +2357,7 @@
     </row>
     <row r="79" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A79" s="5" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B79" s="20">
         <v>0.25</v>
@@ -2366,14 +2366,14 @@
     </row>
     <row r="80" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A80" s="5" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B80" s="36">
         <f>MAX(0,B76)*B79</f>
-        <v>80.974445690139191</v>
+        <v>85.715916855712109</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -2407,7 +2407,7 @@
         <v>205.7</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -2442,7 +2442,7 @@
       </c>
       <c r="B88" s="41">
         <f>B76+B80+B81+B86</f>
-        <v>655.572228450696</v>
+        <v>679.27958427856061</v>
       </c>
       <c r="C88" s="42" t="s">
         <v>125</v>
@@ -2476,7 +2476,7 @@
       </c>
       <c r="B92" s="46">
         <f>B88*1000000/B91</f>
-        <v>2.7747660602999815</v>
+        <v>2.8751094907806718</v>
       </c>
       <c r="C92" s="30"/>
     </row>
@@ -2500,7 +2500,7 @@
       </c>
       <c r="B95" s="25">
         <f>(B92-B94)/B94</f>
-        <v>0.59469313810343771</v>
+        <v>0.65236177631073089</v>
       </c>
       <c r="C95" s="30"/>
     </row>
@@ -2550,7 +2550,7 @@
       </c>
       <c r="B101" s="49">
         <f>B76*1000000/B91</f>
-        <v>1.3709253314991536</v>
+        <v>1.451200075883706</v>
       </c>
       <c r="C101" s="1" t="s">
         <v>137</v>
@@ -2561,8 +2561,8 @@
         <v>138</v>
       </c>
       <c r="B102" s="49">
-        <f>(B80+B81)*1000000/B91</f>
-        <v>0.55436064997212375</v>
+        <f>(B79+B81)*1000000/B91</f>
+        <v>0.21268746368282196</v>
       </c>
       <c r="C102" s="1" t="s">
         <v>139</v>
@@ -2574,7 +2574,7 @@
       </c>
       <c r="B103" s="51">
         <f>B92</f>
-        <v>2.7747660602999815</v>
+        <v>2.8751094907806718</v>
       </c>
       <c r="C103" s="1"/>
     </row>
@@ -2677,7 +2677,7 @@
       </c>
       <c r="D5" s="77">
         <f>'rNPV Model'!B43</f>
-        <v>0.17680000000000004</v>
+        <v>0.18742500000000001</v>
       </c>
       <c r="E5" s="60"/>
       <c r="F5" s="60"/>
@@ -2736,7 +2736,7 @@
       </c>
       <c r="B8" s="61">
         <f>'rNPV Model'!B92</f>
-        <v>2.7747660602999815</v>
+        <v>2.8751094907806718</v>
       </c>
       <c r="C8" s="59" t="s">
         <v>149</v>
@@ -2808,23 +2808,23 @@
       </c>
       <c r="B12" s="64">
         <f>(((((('rNPV Model'!B13*B$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A12)^(-'rNPV Model'!B47))/$A12))/(1+$A12)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A12)^(-'rNPV Model'!B57))/$A12))/(1+$A12)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A12)^2.5))+MAX(0,((((('rNPV Model'!B13*B$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A12)^(-'rNPV Model'!B47))/$A12))/(1+$A12)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A12)^(-'rNPV Model'!B57))/$A12))/(1+$A12)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A12)^2.5)))*$D$7+'rNPV Model'!B81+'rNPV Model'!B86)*1000000/'rNPV Model'!B91</f>
-        <v>2.7415196266485968</v>
+        <v>2.861489965815577</v>
       </c>
       <c r="C12" s="64">
         <f>(((((('rNPV Model'!B13*C$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A12)^(-'rNPV Model'!B47))/$A12))/(1+$A12)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A12)^(-'rNPV Model'!B57))/$A12))/(1+$A12)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A12)^2.5))+MAX(0,((((('rNPV Model'!B13*C$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A12)^(-'rNPV Model'!B47))/$A12))/(1+$A12)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A12)^(-'rNPV Model'!B57))/$A12))/(1+$A12)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A12)^2.5)))*$D$7+'rNPV Model'!B81+'rNPV Model'!B86)*1000000/'rNPV Model'!B91</f>
-        <v>2.9616915635072525</v>
+        <v>3.0816619026742336</v>
       </c>
       <c r="D12" s="64">
         <f>(((((('rNPV Model'!B13*D$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A12)^(-'rNPV Model'!B47))/$A12))/(1+$A12)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A12)^(-'rNPV Model'!B57))/$A12))/(1+$A12)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A12)^2.5))+MAX(0,((((('rNPV Model'!B13*D$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A12)^(-'rNPV Model'!B47))/$A12))/(1+$A12)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A12)^(-'rNPV Model'!B57))/$A12))/(1+$A12)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A12)^2.5)))*$D$7+'rNPV Model'!B81+'rNPV Model'!B86)*1000000/'rNPV Model'!B91</f>
-        <v>3.181863500365909</v>
+        <v>3.3018338395328892</v>
       </c>
       <c r="E12" s="64">
         <f>(((((('rNPV Model'!B13*E$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A12)^(-'rNPV Model'!B47))/$A12))/(1+$A12)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A12)^(-'rNPV Model'!B57))/$A12))/(1+$A12)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A12)^2.5))+MAX(0,((((('rNPV Model'!B13*E$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A12)^(-'rNPV Model'!B47))/$A12))/(1+$A12)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A12)^(-'rNPV Model'!B57))/$A12))/(1+$A12)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A12)^2.5)))*$D$7+'rNPV Model'!B81+'rNPV Model'!B86)*1000000/'rNPV Model'!B91</f>
-        <v>3.4020354372245647</v>
+        <v>3.5220057763915449</v>
       </c>
       <c r="F12" s="64">
         <f>(((((('rNPV Model'!B13*F$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A12)^(-'rNPV Model'!B47))/$A12))/(1+$A12)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A12)^(-'rNPV Model'!B57))/$A12))/(1+$A12)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A12)^2.5))+MAX(0,((((('rNPV Model'!B13*F$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A12)^(-'rNPV Model'!B47))/$A12))/(1+$A12)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A12)^(-'rNPV Model'!B57))/$A12))/(1+$A12)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A12)^2.5)))*$D$7+'rNPV Model'!B81+'rNPV Model'!B86)*1000000/'rNPV Model'!B91</f>
-        <v>3.6222073740832208</v>
+        <v>3.7421777132502019</v>
       </c>
       <c r="G12" s="53"/>
       <c r="H12" s="53"/>
@@ -2837,23 +2837,23 @@
       </c>
       <c r="B13" s="65">
         <f>(((((('rNPV Model'!B13*B$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A13)^(-'rNPV Model'!B47))/$A13))/(1+$A13)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A13)^(-'rNPV Model'!B57))/$A13))/(1+$A13)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A13)^2.5))+MAX(0,((((('rNPV Model'!B13*B$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A13)^(-'rNPV Model'!B47))/$A13))/(1+$A13)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A13)^(-'rNPV Model'!B57))/$A13))/(1+$A13)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A13)^2.5)))*$D$7+'rNPV Model'!B81+'rNPV Model'!B86)*1000000/'rNPV Model'!B91</f>
-        <v>2.5633108693686455</v>
+        <v>2.6729509331043224</v>
       </c>
       <c r="C13" s="65">
         <f>(((((('rNPV Model'!B13*C$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A13)^(-'rNPV Model'!B47))/$A13))/(1+$A13)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A13)^(-'rNPV Model'!B57))/$A13))/(1+$A13)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A13)^2.5))+MAX(0,((((('rNPV Model'!B13*C$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A13)^(-'rNPV Model'!B47))/$A13))/(1+$A13)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A13)^(-'rNPV Model'!B57))/$A13))/(1+$A13)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A13)^2.5)))*$D$7+'rNPV Model'!B81+'rNPV Model'!B86)*1000000/'rNPV Model'!B91</f>
-        <v>2.7652840340069265</v>
+        <v>2.8749240977426038</v>
       </c>
       <c r="D13" s="65">
         <f>(((((('rNPV Model'!B13*D$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A13)^(-'rNPV Model'!B47))/$A13))/(1+$A13)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A13)^(-'rNPV Model'!B57))/$A13))/(1+$A13)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A13)^2.5))+MAX(0,((((('rNPV Model'!B13*D$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A13)^(-'rNPV Model'!B47))/$A13))/(1+$A13)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A13)^(-'rNPV Model'!B57))/$A13))/(1+$A13)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A13)^2.5)))*$D$7+'rNPV Model'!B81+'rNPV Model'!B86)*1000000/'rNPV Model'!B91</f>
-        <v>2.9672571986452083</v>
+        <v>3.0768972623808852</v>
       </c>
       <c r="E13" s="65">
         <f>(((((('rNPV Model'!B13*E$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A13)^(-'rNPV Model'!B47))/$A13))/(1+$A13)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A13)^(-'rNPV Model'!B57))/$A13))/(1+$A13)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A13)^2.5))+MAX(0,((((('rNPV Model'!B13*E$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A13)^(-'rNPV Model'!B47))/$A13))/(1+$A13)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A13)^(-'rNPV Model'!B57))/$A13))/(1+$A13)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A13)^2.5)))*$D$7+'rNPV Model'!B81+'rNPV Model'!B86)*1000000/'rNPV Model'!B91</f>
-        <v>3.1692303632834893</v>
+        <v>3.2788704270191666</v>
       </c>
       <c r="F13" s="64">
         <f>(((((('rNPV Model'!B13*F$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A13)^(-'rNPV Model'!B47))/$A13))/(1+$A13)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A13)^(-'rNPV Model'!B57))/$A13))/(1+$A13)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A13)^2.5))+MAX(0,((((('rNPV Model'!B13*F$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A13)^(-'rNPV Model'!B47))/$A13))/(1+$A13)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A13)^(-'rNPV Model'!B57))/$A13))/(1+$A13)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A13)^2.5)))*$D$7+'rNPV Model'!B81+'rNPV Model'!B86)*1000000/'rNPV Model'!B91</f>
-        <v>3.3712035279217707</v>
+        <v>3.4808435916574476</v>
       </c>
       <c r="G13" s="53"/>
       <c r="H13" s="53"/>
@@ -2866,23 +2866,23 @@
       </c>
       <c r="B14" s="65">
         <f>(((((('rNPV Model'!B13*B$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A14)^(-'rNPV Model'!B47))/$A14))/(1+$A14)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A14)^(-'rNPV Model'!B57))/$A14))/(1+$A14)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A14)^2.5))+MAX(0,((((('rNPV Model'!B13*B$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A14)^(-'rNPV Model'!B47))/$A14))/(1+$A14)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A14)^(-'rNPV Model'!B57))/$A14))/(1+$A14)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A14)^2.5)))*$D$7+'rNPV Model'!B81+'rNPV Model'!B86)*1000000/'rNPV Model'!B91</f>
-        <v>2.403696569944318</v>
+        <v>2.5040400004250092</v>
       </c>
       <c r="C14" s="82">
         <f>(((((('rNPV Model'!B13*C$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A14)^(-'rNPV Model'!B47))/$A14))/(1+$A14)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A14)^(-'rNPV Model'!B57))/$A14))/(1+$A14)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A14)^2.5))+MAX(0,((((('rNPV Model'!B13*C$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A14)^(-'rNPV Model'!B47))/$A14))/(1+$A14)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A14)^(-'rNPV Model'!B57))/$A14))/(1+$A14)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A14)^2.5)))*$D$7+'rNPV Model'!B81+'rNPV Model'!B86)*1000000/'rNPV Model'!B91</f>
-        <v>2.5892313151221491</v>
+        <v>2.6895747456028398</v>
       </c>
       <c r="D14" s="81">
         <f>(((((('rNPV Model'!B13*D$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A14)^(-'rNPV Model'!B47))/$A14))/(1+$A14)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A14)^(-'rNPV Model'!B57))/$A14))/(1+$A14)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A14)^2.5))+MAX(0,((((('rNPV Model'!B13*D$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A14)^(-'rNPV Model'!B47))/$A14))/(1+$A14)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A14)^(-'rNPV Model'!B57))/$A14))/(1+$A14)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A14)^2.5)))*$D$7+'rNPV Model'!B81+'rNPV Model'!B86)*1000000/'rNPV Model'!B91</f>
-        <v>2.7747660602999815</v>
+        <v>2.8751094907806718</v>
       </c>
       <c r="E14" s="65">
         <f>(((((('rNPV Model'!B13*E$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A14)^(-'rNPV Model'!B47))/$A14))/(1+$A14)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A14)^(-'rNPV Model'!B57))/$A14))/(1+$A14)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A14)^2.5))+MAX(0,((((('rNPV Model'!B13*E$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A14)^(-'rNPV Model'!B47))/$A14))/(1+$A14)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A14)^(-'rNPV Model'!B57))/$A14))/(1+$A14)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A14)^2.5)))*$D$7+'rNPV Model'!B81+'rNPV Model'!B86)*1000000/'rNPV Model'!B91</f>
-        <v>2.960300805477813</v>
+        <v>3.0606442359585033</v>
       </c>
       <c r="F14" s="66">
         <f>(((((('rNPV Model'!B13*F$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A14)^(-'rNPV Model'!B47))/$A14))/(1+$A14)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A14)^(-'rNPV Model'!B57))/$A14))/(1+$A14)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A14)^2.5))+MAX(0,((((('rNPV Model'!B13*F$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A14)^(-'rNPV Model'!B47))/$A14))/(1+$A14)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A14)^(-'rNPV Model'!B57))/$A14))/(1+$A14)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A14)^2.5)))*$D$7+'rNPV Model'!B81+'rNPV Model'!B86)*1000000/'rNPV Model'!B91</f>
-        <v>3.1458355506556446</v>
+        <v>3.2461789811363349</v>
       </c>
       <c r="G14" s="53"/>
       <c r="H14" s="53"/>
@@ -2895,23 +2895,23 @@
       </c>
       <c r="B15" s="65">
         <f>(((((('rNPV Model'!B13*B$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A15)^(-'rNPV Model'!B47))/$A15))/(1+$A15)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A15)^(-'rNPV Model'!B57))/$A15))/(1+$A15)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A15)^2.5))+MAX(0,((((('rNPV Model'!B13*B$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A15)^(-'rNPV Model'!B47))/$A15))/(1+$A15)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A15)^(-'rNPV Model'!B57))/$A15))/(1+$A15)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A15)^2.5)))*$D$7+'rNPV Model'!B81+'rNPV Model'!B86)*1000000/'rNPV Model'!B91</f>
-        <v>2.2605699938383217</v>
+        <v>2.3525345622744225</v>
       </c>
       <c r="C15" s="65">
         <f>(((((('rNPV Model'!B13*C$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A15)^(-'rNPV Model'!B47))/$A15))/(1+$A15)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A15)^(-'rNPV Model'!B57))/$A15))/(1+$A15)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A15)^2.5))+MAX(0,((((('rNPV Model'!B13*C$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A15)^(-'rNPV Model'!B47))/$A15))/(1+$A15)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A15)^(-'rNPV Model'!B57))/$A15))/(1+$A15)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A15)^2.5)))*$D$7+'rNPV Model'!B81+'rNPV Model'!B86)*1000000/'rNPV Model'!B91</f>
-        <v>2.4312336902103868</v>
+        <v>2.5231982586464867</v>
       </c>
       <c r="D15" s="65">
         <f>(((((('rNPV Model'!B13*D$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A15)^(-'rNPV Model'!B47))/$A15))/(1+$A15)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A15)^(-'rNPV Model'!B57))/$A15))/(1+$A15)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A15)^2.5))+MAX(0,((((('rNPV Model'!B13*D$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A15)^(-'rNPV Model'!B47))/$A15))/(1+$A15)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A15)^(-'rNPV Model'!B57))/$A15))/(1+$A15)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A15)^2.5)))*$D$7+'rNPV Model'!B81+'rNPV Model'!B86)*1000000/'rNPV Model'!B91</f>
-        <v>2.6018973865824502</v>
+        <v>2.693861955018551</v>
       </c>
       <c r="E15" s="65">
         <f>(((((('rNPV Model'!B13*E$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A15)^(-'rNPV Model'!B47))/$A15))/(1+$A15)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A15)^(-'rNPV Model'!B57))/$A15))/(1+$A15)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A15)^2.5))+MAX(0,((((('rNPV Model'!B13*E$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A15)^(-'rNPV Model'!B47))/$A15))/(1+$A15)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A15)^(-'rNPV Model'!B57))/$A15))/(1+$A15)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A15)^2.5)))*$D$7+'rNPV Model'!B81+'rNPV Model'!B86)*1000000/'rNPV Model'!B91</f>
-        <v>2.7725610829545144</v>
+        <v>2.8645256513906148</v>
       </c>
       <c r="F15" s="64">
         <f>(((((('rNPV Model'!B13*F$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A15)^(-'rNPV Model'!B47))/$A15))/(1+$A15)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A15)^(-'rNPV Model'!B57))/$A15))/(1+$A15)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A15)^2.5))+MAX(0,((((('rNPV Model'!B13*F$11*'rNPV Model'!B16*'rNPV Model'!B18)*((1-(1+$A15)^(-'rNPV Model'!B47))/$A15))/(1+$A15)^('rNPV Model'!B8-'rNPV Model'!B10))*'rNPV Model'!B25)+((('rNPV Model'!B60*((1-(1+$A15)^(-'rNPV Model'!B57))/$A15))/(1+$A15)^('rNPV Model'!B9-'rNPV Model'!B10))*'rNPV Model'!B43)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+$A15)^2.5)))*$D$7+'rNPV Model'!B81+'rNPV Model'!B86)*1000000/'rNPV Model'!B91</f>
-        <v>2.9432247793265782</v>
+        <v>3.0351893477626799</v>
       </c>
       <c r="G15" s="53"/>
       <c r="H15" s="53"/>
@@ -3007,10 +3007,10 @@
       </c>
       <c r="G20" s="73">
         <f>((('rNPV Model'!B13*B20*'rNPV Model'!B16*'rNPV Model'!B18*((1-(1+F20)^(-'rNPV Model'!B47))/F20)/(1+F20)^('rNPV Model'!B8-'rNPV Model'!B10)*C20)+('rNPV Model'!B60*((1-(1+F20)^(-'rNPV Model'!B57))/F20)/(1+F20)^('rNPV Model'!B9-'rNPV Model'!B10)*D20)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+F20)^2.5))+MAX(0,(('rNPV Model'!B13*B20*'rNPV Model'!B16*'rNPV Model'!B18*((1-(1+F20)^(-'rNPV Model'!B47))/F20)/(1+F20)^('rNPV Model'!B8-'rNPV Model'!B10)*C20)+('rNPV Model'!B60*((1-(1+F20)^(-'rNPV Model'!B57))/F20)/(1+F20)^('rNPV Model'!B9-'rNPV Model'!B10)*D20)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+F20)^2.5)))*$D$7+E20+'rNPV Model'!B86)*1000000/'rNPV Model'!B91</f>
-        <v>0.65615450400947595</v>
+        <v>0.65889978123534976</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="I20" s="53"/>
       <c r="J20" s="53"/>
@@ -3030,7 +3030,7 @@
       </c>
       <c r="D21" s="77">
         <f>'rNPV Model'!B43</f>
-        <v>0.17680000000000004</v>
+        <v>0.18742500000000001</v>
       </c>
       <c r="E21" s="89">
         <v>50</v>
@@ -3041,7 +3041,7 @@
       </c>
       <c r="G21" s="74">
         <f>((('rNPV Model'!B13*B21*'rNPV Model'!B16*'rNPV Model'!B18*((1-(1+F21)^(-'rNPV Model'!B47))/F21)/(1+F21)^('rNPV Model'!B8-'rNPV Model'!B10)*C21)+('rNPV Model'!B60*((1-(1+F21)^(-'rNPV Model'!B57))/F21)/(1+F21)^('rNPV Model'!B9-'rNPV Model'!B10)*D21)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+F21)^2.5))+MAX(0,(('rNPV Model'!B13*B21*'rNPV Model'!B16*'rNPV Model'!B18*((1-(1+F21)^(-'rNPV Model'!B47))/F21)/(1+F21)^('rNPV Model'!B8-'rNPV Model'!B10)*C21)+('rNPV Model'!B60*((1-(1+F21)^(-'rNPV Model'!B57))/F21)/(1+F21)^('rNPV Model'!B9-'rNPV Model'!B10)*D21)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+F21)^2.5)))*$D$7+E21+'rNPV Model'!B86)*1000000/'rNPV Model'!B91</f>
-        <v>2.7747660602999815</v>
+        <v>2.8751094907806718</v>
       </c>
       <c r="H21" s="1"/>
       <c r="I21" s="53"/>
@@ -3069,7 +3069,7 @@
       </c>
       <c r="G22" s="73">
         <f>((('rNPV Model'!B13*B22*'rNPV Model'!B16*'rNPV Model'!B18*((1-(1+F22)^(-'rNPV Model'!B47))/F22)/(1+F22)^('rNPV Model'!B8-'rNPV Model'!B10)*C22)+('rNPV Model'!B60*((1-(1+F22)^(-'rNPV Model'!B57))/F22)/(1+F22)^('rNPV Model'!B9-'rNPV Model'!B10)*D22)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+F22)^2.5))+MAX(0,(('rNPV Model'!B13*B22*'rNPV Model'!B16*'rNPV Model'!B18*((1-(1+F22)^(-'rNPV Model'!B47))/F22)/(1+F22)^('rNPV Model'!B8-'rNPV Model'!B10)*C22)+('rNPV Model'!B60*((1-(1+F22)^(-'rNPV Model'!B57))/F22)/(1+F22)^('rNPV Model'!B9-'rNPV Model'!B10)*D22)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+F22)^2.5)))*$D$7+E22+'rNPV Model'!B86)*1000000/'rNPV Model'!B91</f>
-        <v>3.3550775886694248</v>
+        <v>3.3585856101170659</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>176</v>
@@ -3089,7 +3089,7 @@
         <v>0.38</v>
       </c>
       <c r="D23" s="77">
-        <v>0.3</v>
+        <v>0.315</v>
       </c>
       <c r="E23" s="89">
         <v>150</v>
@@ -3099,7 +3099,7 @@
       </c>
       <c r="G23" s="73">
         <f>((('rNPV Model'!B13*B23*'rNPV Model'!B16*'rNPV Model'!B18*((1-(1+F23)^(-'rNPV Model'!B47))/F23)/(1+F23)^('rNPV Model'!B8-'rNPV Model'!B10)*C23)+('rNPV Model'!B60*((1-(1+F23)^(-'rNPV Model'!B57))/F23)/(1+F23)^('rNPV Model'!B9-'rNPV Model'!B10)*D23)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+F23)^2.5))+MAX(0,(('rNPV Model'!B13*B23*'rNPV Model'!B16*'rNPV Model'!B18*((1-(1+F23)^(-'rNPV Model'!B47))/F23)/(1+F23)^('rNPV Model'!B8-'rNPV Model'!B10)*C23)+('rNPV Model'!B60*((1-(1+F23)^(-'rNPV Model'!B57))/F23)/(1+F23)^('rNPV Model'!B9-'rNPV Model'!B10)*D23)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+F23)^2.5)))*$D$7+E23+'rNPV Model'!B86)*1000000/'rNPV Model'!B91</f>
-        <v>4.9618429636502954</v>
+        <v>5.1151519974863682</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>177</v>
@@ -3119,7 +3119,7 @@
         <v>0.38</v>
       </c>
       <c r="D24" s="77">
-        <v>0.3</v>
+        <v>0.315</v>
       </c>
       <c r="E24" s="89">
         <v>250</v>
@@ -3129,7 +3129,7 @@
       </c>
       <c r="G24" s="73">
         <f>((('rNPV Model'!B13*B24*'rNPV Model'!B16*'rNPV Model'!B18*((1-(1+F24)^(-'rNPV Model'!B47))/F24)/(1+F24)^('rNPV Model'!B8-'rNPV Model'!B10)*C24)+('rNPV Model'!B60*((1-(1+F24)^(-'rNPV Model'!B57))/F24)/(1+F24)^('rNPV Model'!B9-'rNPV Model'!B10)*D24)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+F24)^2.5))+MAX(0,(('rNPV Model'!B13*B24*'rNPV Model'!B16*'rNPV Model'!B18*((1-(1+F24)^(-'rNPV Model'!B47))/F24)/(1+F24)^('rNPV Model'!B8-'rNPV Model'!B10)*C24)+('rNPV Model'!B60*((1-(1+F24)^(-'rNPV Model'!B57))/F24)/(1+F24)^('rNPV Model'!B9-'rNPV Model'!B10)*D24)+(('rNPV Model'!B67+'rNPV Model'!B68+'rNPV Model'!B69+'rNPV Model'!B70+'rNPV Model'!B71)/(1+F24)^2.5)))*$D$7+E24+'rNPV Model'!B86)*1000000/'rNPV Model'!B91</f>
-        <v>6.6386016975041242</v>
+        <v>6.8226566180598205</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>162</v>
@@ -3208,7 +3208,7 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B30" s="53"/>
       <c r="C30" s="53"/>
@@ -3236,7 +3236,7 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="B32" s="53"/>
       <c r="C32" s="53"/>

</xml_diff>